<commit_message>
change in paropakar and dhan bahadur
</commit_message>
<xml_diff>
--- a/ofc/estimates/परोपकार भवन मर्मत/परोपकार भवन मर्मत.xlsx
+++ b/ofc/estimates/परोपकार भवन मर्मत/परोपकार भवन मर्मत.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="WCR" sheetId="6" r:id="rId1"/>
     <sheet name="Sheet4 (2)" sheetId="17" r:id="rId2"/>
     <sheet name="rate analysis" sheetId="18" r:id="rId3"/>
-    <sheet name="upvc" sheetId="19" r:id="rId4"/>
+    <sheet name="upvc" sheetId="20" r:id="rId4"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId5"/>
@@ -91,7 +91,7 @@
     <definedName name="plywood4">'[1]update Rate'!$N$69</definedName>
     <definedName name="plywood6">'[1]update Rate'!$N$71</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Sheet4 (2)'!$A$1:$K$114</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">upvc!$A$1:$K$114</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">upvc!$A$1:$K$127</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Sheet4 (2)'!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">upvc!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">WCR!$1:$12</definedName>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="150">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -258,9 +258,6 @@
   </si>
   <si>
     <t>sqm</t>
-  </si>
-  <si>
-    <t>Date:2081/09/11</t>
   </si>
   <si>
     <t>Project:- परोपकार भवन मर्मत</t>
@@ -660,6 +657,51 @@
   <si>
     <t>Date:2081/09/29</t>
   </si>
+  <si>
+    <t>sfk]{6 b'jf]</t>
+  </si>
+  <si>
+    <t>-for open spaces</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <r>
+      <t>Area (m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>;km]{;nfO{ 8«]l;Ë ug]{ sfo{ vfN6f] k'g]{, p7]sf] df6f] sf6\g], ;tx ldnfpg]</t>
+  </si>
+  <si>
+    <t>cflb sfo{ ;d]t -;le{;/f]8 cflb_</t>
+  </si>
+  <si>
+    <t>;km]{;nfO{ 8«]l;Ë ug]{ sfo{ vfN6f] k'g]{, p7]sf] df6f] sf6\g], ;tx ldnfpg] cflb sfo{ ;d]t -;le{;/f]8 cflb_</t>
+  </si>
+  <si>
+    <t>-as of item no. 15</t>
+  </si>
 </sst>
 </file>
 
@@ -670,7 +712,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="37">
+  <fonts count="39">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -881,6 +923,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Preeti"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -986,7 +1039,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1317,6 +1370,24 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1341,55 +1412,49 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1411,18 +1476,27 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1854,8 +1928,8 @@
       <sheetName val="PPMO_BOQ"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1">
         <row r="16">
           <cell r="B16" t="str">
             <v>Clearing and Grubbing Road Land ., Clearing and grubbing road land including uprooting rank vegetation, grass, bushes, shrubs, saplings and trees girth up to 300 mm, removal of stumps of trees cut earlier and disposal of unserviceable materials and stacking of serviceable Material to be used or auctioned, up to a lead of 30 meters including removal and disposal of top organic soil not exceeding 150 mm in thickness., By Mechanical Means, In area of light jungle (less than 15 number per 100 sqm )</v>
@@ -1897,25 +1971,25 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1948,33 +2022,33 @@
       <sheetName val="PPMO_BOQ"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1">
         <row r="33">
           <cell r="B33" t="str">
             <v>Earthwork Excavation in Cutting., Roadway Excavation in all types of Soil by Manual Means ., Roadway Excavation in all types of soil as per drawing and technical specification, including removal of stumps and other deleterious matter, with all lifts and lead as per Drawing and instruction of the Engineer.</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2436,90 +2510,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="142"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="G1" s="142"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="142"/>
-      <c r="J1" s="142"/>
-      <c r="K1" s="142"/>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="134"/>
+      <c r="I1" s="134"/>
+      <c r="J1" s="134"/>
+      <c r="K1" s="134"/>
     </row>
     <row r="2" spans="1:11" ht="24.6">
-      <c r="A2" s="143" t="s">
+      <c r="A2" s="135" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="143"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
-      <c r="F2" s="143"/>
-      <c r="G2" s="143"/>
-      <c r="H2" s="143"/>
-      <c r="I2" s="143"/>
-      <c r="J2" s="143"/>
-      <c r="K2" s="143"/>
+      <c r="B2" s="135"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="135"/>
+      <c r="K2" s="135"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1">
-      <c r="A3" s="144" t="s">
+      <c r="A3" s="136" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="144"/>
-      <c r="C3" s="144"/>
-      <c r="D3" s="144"/>
-      <c r="E3" s="144"/>
-      <c r="F3" s="144"/>
-      <c r="G3" s="144"/>
-      <c r="H3" s="144"/>
-      <c r="I3" s="144"/>
-      <c r="J3" s="144"/>
-      <c r="K3" s="144"/>
+      <c r="B3" s="136"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="136"/>
+      <c r="E3" s="136"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="136"/>
+      <c r="H3" s="136"/>
+      <c r="I3" s="136"/>
+      <c r="J3" s="136"/>
+      <c r="K3" s="136"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1">
-      <c r="A4" s="144" t="s">
+      <c r="A4" s="136" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="144"/>
-      <c r="C4" s="144"/>
-      <c r="D4" s="144"/>
-      <c r="E4" s="144"/>
-      <c r="F4" s="144"/>
-      <c r="G4" s="144"/>
-      <c r="H4" s="144"/>
-      <c r="I4" s="144"/>
-      <c r="J4" s="144"/>
-      <c r="K4" s="144"/>
+      <c r="B4" s="136"/>
+      <c r="C4" s="136"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
+      <c r="H4" s="136"/>
+      <c r="I4" s="136"/>
+      <c r="J4" s="136"/>
+      <c r="K4" s="136"/>
     </row>
     <row r="5" spans="1:11" ht="18">
-      <c r="A5" s="145" t="s">
+      <c r="A5" s="137" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="145"/>
-      <c r="C5" s="145"/>
-      <c r="D5" s="145"/>
-      <c r="E5" s="145"/>
-      <c r="F5" s="145"/>
-      <c r="G5" s="145"/>
-      <c r="H5" s="145"/>
-      <c r="I5" s="145"/>
-      <c r="J5" s="145"/>
-      <c r="K5" s="145"/>
+      <c r="B5" s="137"/>
+      <c r="C5" s="137"/>
+      <c r="D5" s="137"/>
+      <c r="E5" s="137"/>
+      <c r="F5" s="137"/>
+      <c r="G5" s="137"/>
+      <c r="H5" s="137"/>
+      <c r="I5" s="137"/>
+      <c r="J5" s="137"/>
+      <c r="K5" s="137"/>
     </row>
     <row r="6" spans="1:11" ht="18">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="140" t="e">
+      <c r="C6" s="132" t="e">
         <f>F18</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="141"/>
+      <c r="D6" s="133"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -2527,11 +2601,11 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="140" t="e">
+      <c r="J6" s="132" t="e">
         <f>I18</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="141"/>
+      <c r="K6" s="133"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="25" t="s">
@@ -2540,77 +2614,77 @@
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="135"/>
-      <c r="G7" s="135"/>
-      <c r="I7" s="136" t="s">
+      <c r="F7" s="141"/>
+      <c r="G7" s="141"/>
+      <c r="I7" s="142" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="136"/>
-      <c r="K7" s="136"/>
+      <c r="J7" s="142"/>
+      <c r="K7" s="142"/>
     </row>
     <row r="8" spans="1:11" ht="15.6">
-      <c r="A8" s="134" t="e">
+      <c r="A8" s="140" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="134"/>
-      <c r="C8" s="134"/>
-      <c r="D8" s="134"/>
-      <c r="E8" s="134"/>
-      <c r="F8" s="134"/>
-      <c r="I8" s="137" t="s">
+      <c r="B8" s="140"/>
+      <c r="C8" s="140"/>
+      <c r="D8" s="140"/>
+      <c r="E8" s="140"/>
+      <c r="F8" s="140"/>
+      <c r="I8" s="143" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="137"/>
-      <c r="K8" s="137"/>
+      <c r="J8" s="143"/>
+      <c r="K8" s="143"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="138" t="e">
+      <c r="A9" s="144" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="138"/>
-      <c r="C9" s="138"/>
-      <c r="D9" s="138"/>
-      <c r="E9" s="138"/>
-      <c r="F9" s="138"/>
-      <c r="I9" s="137" t="s">
+      <c r="B9" s="144"/>
+      <c r="C9" s="144"/>
+      <c r="D9" s="144"/>
+      <c r="E9" s="144"/>
+      <c r="F9" s="144"/>
+      <c r="I9" s="143" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="137"/>
-      <c r="K9" s="137"/>
+      <c r="J9" s="143"/>
+      <c r="K9" s="143"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="132" t="s">
+      <c r="A11" s="138" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="132" t="s">
+      <c r="B11" s="138" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="132" t="s">
+      <c r="C11" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="139" t="s">
+      <c r="D11" s="145" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="139"/>
-      <c r="F11" s="139"/>
-      <c r="G11" s="139" t="s">
+      <c r="E11" s="145"/>
+      <c r="F11" s="145"/>
+      <c r="G11" s="145" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="139"/>
-      <c r="I11" s="139"/>
-      <c r="J11" s="132" t="s">
+      <c r="H11" s="145"/>
+      <c r="I11" s="145"/>
+      <c r="J11" s="138" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="133" t="s">
+      <c r="K11" s="139" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="132"/>
-      <c r="B12" s="132"/>
-      <c r="C12" s="132"/>
+      <c r="A12" s="138"/>
+      <c r="B12" s="138"/>
+      <c r="C12" s="138"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -2629,8 +2703,8 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="132"/>
-      <c r="K12" s="133"/>
+      <c r="J12" s="138"/>
+      <c r="K12" s="139"/>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="15.6">
       <c r="A13" s="26" t="e">
@@ -2792,13 +2866,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -2812,6 +2879,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2829,7 +2903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -2848,113 +2922,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
-      <c r="A1" s="152" t="s">
+      <c r="A1" s="147" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="152"/>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
-      <c r="H1" s="152"/>
-      <c r="I1" s="152"/>
-      <c r="J1" s="152"/>
-      <c r="K1" s="152"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147"/>
+      <c r="G1" s="147"/>
+      <c r="H1" s="147"/>
+      <c r="I1" s="147"/>
+      <c r="J1" s="147"/>
+      <c r="K1" s="147"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="22.8">
-      <c r="A2" s="153" t="s">
+      <c r="A2" s="148" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="153"/>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
-      <c r="G2" s="153"/>
-      <c r="H2" s="153"/>
-      <c r="I2" s="153"/>
-      <c r="J2" s="153"/>
-      <c r="K2" s="153"/>
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="148"/>
+      <c r="K2" s="148"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1">
-      <c r="A3" s="144" t="s">
+      <c r="A3" s="136" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="144"/>
-      <c r="C3" s="144"/>
-      <c r="D3" s="144"/>
-      <c r="E3" s="144"/>
-      <c r="F3" s="144"/>
-      <c r="G3" s="144"/>
-      <c r="H3" s="144"/>
-      <c r="I3" s="144"/>
-      <c r="J3" s="144"/>
-      <c r="K3" s="144"/>
+      <c r="B3" s="136"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="136"/>
+      <c r="E3" s="136"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="136"/>
+      <c r="H3" s="136"/>
+      <c r="I3" s="136"/>
+      <c r="J3" s="136"/>
+      <c r="K3" s="136"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1">
-      <c r="A4" s="144" t="s">
+      <c r="A4" s="136" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="144"/>
-      <c r="C4" s="144"/>
-      <c r="D4" s="144"/>
-      <c r="E4" s="144"/>
-      <c r="F4" s="144"/>
-      <c r="G4" s="144"/>
-      <c r="H4" s="144"/>
-      <c r="I4" s="144"/>
-      <c r="J4" s="144"/>
-      <c r="K4" s="144"/>
+      <c r="B4" s="136"/>
+      <c r="C4" s="136"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
+      <c r="H4" s="136"/>
+      <c r="I4" s="136"/>
+      <c r="J4" s="136"/>
+      <c r="K4" s="136"/>
     </row>
     <row r="5" spans="1:14" ht="17.399999999999999">
-      <c r="A5" s="154" t="s">
+      <c r="A5" s="149" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="154"/>
-      <c r="C5" s="154"/>
-      <c r="D5" s="154"/>
-      <c r="E5" s="154"/>
-      <c r="F5" s="154"/>
-      <c r="G5" s="154"/>
-      <c r="H5" s="154"/>
-      <c r="I5" s="154"/>
-      <c r="J5" s="154"/>
-      <c r="K5" s="154"/>
+      <c r="B5" s="149"/>
+      <c r="C5" s="149"/>
+      <c r="D5" s="149"/>
+      <c r="E5" s="149"/>
+      <c r="F5" s="149"/>
+      <c r="G5" s="149"/>
+      <c r="H5" s="149"/>
+      <c r="I5" s="149"/>
+      <c r="J5" s="149"/>
+      <c r="K5" s="149"/>
     </row>
     <row r="6" spans="1:14" ht="15.6">
-      <c r="A6" s="134" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="134"/>
-      <c r="C6" s="134"/>
-      <c r="D6" s="134"/>
-      <c r="E6" s="134"/>
-      <c r="F6" s="134"/>
+      <c r="A6" s="140" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="140"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="140"/>
+      <c r="F6" s="140"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="151" t="s">
+      <c r="H6" s="146" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="151"/>
-      <c r="J6" s="151"/>
-      <c r="K6" s="151"/>
+      <c r="I6" s="146"/>
+      <c r="J6" s="146"/>
+      <c r="K6" s="146"/>
     </row>
     <row r="7" spans="1:14" ht="15.6">
-      <c r="A7" s="148" t="s">
+      <c r="A7" s="150" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="148"/>
-      <c r="C7" s="148"/>
-      <c r="D7" s="148"/>
-      <c r="E7" s="148"/>
-      <c r="F7" s="148"/>
+      <c r="B7" s="150"/>
+      <c r="C7" s="150"/>
+      <c r="D7" s="150"/>
+      <c r="E7" s="150"/>
+      <c r="F7" s="150"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="149" t="s">
-        <v>142</v>
-      </c>
-      <c r="I7" s="149"/>
-      <c r="J7" s="149"/>
-      <c r="K7" s="149"/>
+      <c r="H7" s="151" t="s">
+        <v>141</v>
+      </c>
+      <c r="I7" s="151"/>
+      <c r="J7" s="151"/>
+      <c r="K7" s="151"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1">
       <c r="A8" s="4" t="s">
@@ -2996,7 +3070,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="60"/>
       <c r="D9" s="38"/>
@@ -3011,7 +3085,7 @@
     <row r="10" spans="1:14" ht="15" customHeight="1">
       <c r="A10" s="18"/>
       <c r="B10" s="36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="35">
         <v>1</v>
@@ -3151,7 +3225,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="35"/>
       <c r="D16" s="37"/>
@@ -3166,7 +3240,7 @@
     <row r="17" spans="1:19" ht="15" customHeight="1">
       <c r="A17" s="18"/>
       <c r="B17" s="36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="35">
         <v>2</v>
@@ -3254,7 +3328,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" s="35"/>
       <c r="D21" s="37"/>
@@ -3269,7 +3343,7 @@
     <row r="22" spans="1:19" ht="15" customHeight="1">
       <c r="A22" s="18"/>
       <c r="B22" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C22" s="35">
         <v>2</v>
@@ -3311,7 +3385,7 @@
         <v>1.7555623285583659</v>
       </c>
       <c r="H23" s="39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I23" s="39">
         <v>1950.4</v>
@@ -3358,7 +3432,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="87" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C26" s="19"/>
       <c r="D26" s="20"/>
@@ -3380,7 +3454,7 @@
     <row r="27" spans="1:19" ht="15" customHeight="1">
       <c r="A27" s="18"/>
       <c r="B27" s="36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C27" s="19">
         <v>1</v>
@@ -3418,7 +3492,7 @@
         <v>0.48765620237732393</v>
       </c>
       <c r="H28" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I28" s="23">
         <v>663.31</v>
@@ -3447,7 +3521,7 @@
         <v>5</v>
       </c>
       <c r="B30" s="89" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C30" s="19"/>
       <c r="D30" s="20"/>
@@ -3548,7 +3622,7 @@
         <v>6</v>
       </c>
       <c r="B35" s="89" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C35" s="19"/>
       <c r="D35" s="20"/>
@@ -3604,7 +3678,7 @@
         <v>0.68271868332825347</v>
       </c>
       <c r="H37" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I37" s="23">
         <v>1014.97</v>
@@ -3651,7 +3725,7 @@
         <v>7</v>
       </c>
       <c r="B40" s="60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C40" s="35"/>
       <c r="D40" s="37"/>
@@ -3663,7 +3737,7 @@
       <c r="J40" s="41"/>
       <c r="K40" s="21"/>
       <c r="N40" s="66" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O40" s="66"/>
       <c r="P40" s="66"/>
@@ -3675,7 +3749,7 @@
     <row r="41" spans="1:20" ht="15" customHeight="1">
       <c r="A41" s="18"/>
       <c r="B41" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C41" s="35">
         <v>2</v>
@@ -3698,15 +3772,15 @@
       <c r="I41" s="39"/>
       <c r="J41" s="39"/>
       <c r="K41" s="61"/>
-      <c r="N41" s="146" t="s">
-        <v>88</v>
-      </c>
-      <c r="O41" s="146"/>
-      <c r="P41" s="146"/>
-      <c r="Q41" s="146"/>
-      <c r="R41" s="146"/>
-      <c r="S41" s="146"/>
-      <c r="T41" s="146"/>
+      <c r="N41" s="154" t="s">
+        <v>87</v>
+      </c>
+      <c r="O41" s="154"/>
+      <c r="P41" s="154"/>
+      <c r="Q41" s="154"/>
+      <c r="R41" s="154"/>
+      <c r="S41" s="154"/>
+      <c r="T41" s="154"/>
     </row>
     <row r="42" spans="1:20" ht="15" customHeight="1">
       <c r="A42" s="18"/>
@@ -3722,7 +3796,7 @@
         <v>1.7555623285583659</v>
       </c>
       <c r="H42" s="39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I42" s="39">
         <v>8569.2999999999993</v>
@@ -3773,22 +3847,22 @@
         <v>8</v>
       </c>
       <c r="B45" s="89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C45" s="19" t="s">
         <v>7</v>
       </c>
       <c r="D45" s="90" t="s">
+        <v>94</v>
+      </c>
+      <c r="E45" s="91" t="s">
         <v>95</v>
       </c>
-      <c r="E45" s="91" t="s">
+      <c r="F45" s="91" t="s">
         <v>96</v>
       </c>
-      <c r="F45" s="91" t="s">
+      <c r="G45" s="91" t="s">
         <v>97</v>
-      </c>
-      <c r="G45" s="91" t="s">
-        <v>98</v>
       </c>
       <c r="H45" s="22"/>
       <c r="I45" s="23"/>
@@ -3798,7 +3872,7 @@
     <row r="46" spans="1:20" ht="15" customHeight="1">
       <c r="A46" s="18"/>
       <c r="B46" s="36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C46" s="19">
         <f>TRUNC((D47-0.1)/0.15,0)+1</f>
@@ -3920,7 +3994,7 @@
         <v>2.3221315392401441E-2</v>
       </c>
       <c r="H50" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I50" s="23">
         <v>131940</v>
@@ -3967,7 +4041,7 @@
         <v>9</v>
       </c>
       <c r="B53" s="89" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C53" s="19"/>
       <c r="D53" s="20"/>
@@ -3982,7 +4056,7 @@
     <row r="54" spans="1:20" ht="15" customHeight="1">
       <c r="A54" s="18"/>
       <c r="B54" s="36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C54" s="35">
         <f>2*13</f>
@@ -4003,15 +4077,15 @@
       <c r="I54" s="39"/>
       <c r="J54" s="39"/>
       <c r="K54" s="61"/>
-      <c r="N54" s="146" t="s">
-        <v>88</v>
-      </c>
-      <c r="O54" s="146"/>
-      <c r="P54" s="146"/>
-      <c r="Q54" s="146"/>
-      <c r="R54" s="146"/>
-      <c r="S54" s="146"/>
-      <c r="T54" s="146"/>
+      <c r="N54" s="154" t="s">
+        <v>87</v>
+      </c>
+      <c r="O54" s="154"/>
+      <c r="P54" s="154"/>
+      <c r="Q54" s="154"/>
+      <c r="R54" s="154"/>
+      <c r="S54" s="154"/>
+      <c r="T54" s="154"/>
     </row>
     <row r="55" spans="1:20" ht="15" customHeight="1">
       <c r="A55" s="18"/>
@@ -4164,7 +4238,7 @@
         <v>10</v>
       </c>
       <c r="B61" s="89" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C61" s="35"/>
       <c r="D61" s="37"/>
@@ -4183,7 +4257,7 @@
     <row r="62" spans="1:20" ht="15" customHeight="1">
       <c r="A62" s="18"/>
       <c r="B62" s="36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C62" s="35">
         <v>1</v>
@@ -4207,15 +4281,15 @@
       <c r="I62" s="39"/>
       <c r="J62" s="39"/>
       <c r="K62" s="61"/>
-      <c r="N62" s="146" t="s">
-        <v>88</v>
-      </c>
-      <c r="O62" s="146"/>
-      <c r="P62" s="146"/>
-      <c r="Q62" s="146"/>
-      <c r="R62" s="146"/>
-      <c r="S62" s="146"/>
-      <c r="T62" s="146"/>
+      <c r="N62" s="154" t="s">
+        <v>87</v>
+      </c>
+      <c r="O62" s="154"/>
+      <c r="P62" s="154"/>
+      <c r="Q62" s="154"/>
+      <c r="R62" s="154"/>
+      <c r="S62" s="154"/>
+      <c r="T62" s="154"/>
     </row>
     <row r="63" spans="1:20" ht="15" customHeight="1">
       <c r="A63" s="18"/>
@@ -4263,7 +4337,7 @@
         <v>0.75815300213349579</v>
       </c>
       <c r="H64" s="39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I64" s="23">
         <f>81404.27/100</f>
@@ -4311,22 +4385,22 @@
         <v>11</v>
       </c>
       <c r="B67" s="121" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C67" s="19" t="s">
         <v>7</v>
       </c>
       <c r="D67" s="90" t="s">
+        <v>94</v>
+      </c>
+      <c r="E67" s="91" t="s">
         <v>95</v>
       </c>
-      <c r="E67" s="91" t="s">
+      <c r="F67" s="91" t="s">
         <v>96</v>
       </c>
-      <c r="F67" s="91" t="s">
-        <v>97</v>
-      </c>
       <c r="G67" s="91" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H67" s="22"/>
       <c r="I67" s="23"/>
@@ -4336,7 +4410,7 @@
     <row r="68" spans="1:13">
       <c r="A68" s="122"/>
       <c r="B68" s="126" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C68" s="124">
         <v>6</v>
@@ -4390,7 +4464,7 @@
     <row r="70" spans="1:13">
       <c r="A70" s="122"/>
       <c r="B70" s="126" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C70" s="124">
         <f>TRUNC(D75/0.1,0)</f>
@@ -4419,7 +4493,7 @@
     <row r="71" spans="1:13" s="1" customFormat="1" ht="27.6">
       <c r="A71" s="122"/>
       <c r="B71" s="127" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C71" s="124">
         <v>4</v>
@@ -4448,7 +4522,7 @@
     <row r="72" spans="1:13" s="1" customFormat="1" ht="41.4">
       <c r="A72" s="122"/>
       <c r="B72" s="127" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C72" s="124">
         <v>1</v>
@@ -4504,7 +4578,7 @@
     <row r="74" spans="1:13" s="1" customFormat="1" ht="27.6">
       <c r="A74" s="122"/>
       <c r="B74" s="127" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C74" s="124">
         <v>1</v>
@@ -4533,7 +4607,7 @@
     <row r="75" spans="1:13" s="1" customFormat="1">
       <c r="A75" s="122"/>
       <c r="B75" s="127" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C75" s="124">
         <v>2</v>
@@ -4562,7 +4636,7 @@
     <row r="76" spans="1:13" s="1" customFormat="1">
       <c r="A76" s="122"/>
       <c r="B76" s="127" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C76" s="124">
         <f>C70</f>
@@ -4603,7 +4677,7 @@
         <v>734.74624078024999</v>
       </c>
       <c r="H77" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I77" s="23">
         <v>181.17</v>
@@ -4650,7 +4724,7 @@
         <v>12</v>
       </c>
       <c r="B80" s="130" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C80" s="19"/>
       <c r="D80" s="20"/>
@@ -4665,7 +4739,7 @@
     <row r="81" spans="1:11" s="1" customFormat="1">
       <c r="A81" s="18"/>
       <c r="B81" s="127" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C81" s="19">
         <v>2</v>
@@ -4877,7 +4951,7 @@
     <row r="90" spans="1:11" s="1" customFormat="1">
       <c r="A90" s="18"/>
       <c r="B90" s="127" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C90" s="19"/>
       <c r="D90" s="20"/>
@@ -4902,7 +4976,7 @@
     <row r="91" spans="1:11" s="1" customFormat="1">
       <c r="A91" s="18"/>
       <c r="B91" s="127" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C91" s="19"/>
       <c r="D91" s="20"/>
@@ -4935,7 +5009,7 @@
         <v>13</v>
       </c>
       <c r="B93" s="121" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C93" s="19"/>
       <c r="D93" s="20"/>
@@ -4950,7 +5024,7 @@
     <row r="94" spans="1:11" ht="15" customHeight="1">
       <c r="A94" s="18"/>
       <c r="B94" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C94" s="19">
         <v>1</v>
@@ -5028,7 +5102,7 @@
         <v>14</v>
       </c>
       <c r="B98" s="121" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C98" s="19"/>
       <c r="D98" s="20"/>
@@ -5043,7 +5117,7 @@
     <row r="99" spans="1:11" ht="15" customHeight="1">
       <c r="A99" s="18"/>
       <c r="B99" s="36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C99" s="19">
         <v>1</v>
@@ -5127,7 +5201,7 @@
         <v>15</v>
       </c>
       <c r="B103" s="36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C103" s="19">
         <v>1</v>
@@ -5140,7 +5214,7 @@
         <v>1</v>
       </c>
       <c r="H103" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I103" s="23">
         <v>3000</v>
@@ -5242,11 +5316,11 @@
       <c r="B109" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C109" s="147">
+      <c r="C109" s="152">
         <f>J107</f>
         <v>336917.6969730733</v>
       </c>
-      <c r="D109" s="147"/>
+      <c r="D109" s="152"/>
       <c r="E109" s="38">
         <v>100</v>
       </c>
@@ -5262,10 +5336,10 @@
       <c r="B110" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C110" s="150">
+      <c r="C110" s="153">
         <v>300000</v>
       </c>
-      <c r="D110" s="150"/>
+      <c r="D110" s="153"/>
       <c r="E110" s="38"/>
       <c r="F110" s="45"/>
       <c r="G110" s="44"/>
@@ -5279,11 +5353,11 @@
       <c r="B111" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C111" s="150">
+      <c r="C111" s="153">
         <f>C110-C113-C114</f>
         <v>285000</v>
       </c>
-      <c r="D111" s="150"/>
+      <c r="D111" s="153"/>
       <c r="E111" s="38">
         <f>C111/C109*100</f>
         <v>84.590391825804687</v>
@@ -5300,11 +5374,11 @@
       <c r="B112" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C112" s="147">
+      <c r="C112" s="152">
         <f>C109-C111</f>
         <v>51917.696973073296</v>
       </c>
-      <c r="D112" s="147"/>
+      <c r="D112" s="152"/>
       <c r="E112" s="38">
         <f>100-E111</f>
         <v>15.409608174195313</v>
@@ -5321,11 +5395,11 @@
       <c r="B113" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C113" s="147">
+      <c r="C113" s="152">
         <f>C110*0.03</f>
         <v>9000</v>
       </c>
-      <c r="D113" s="147"/>
+      <c r="D113" s="152"/>
       <c r="E113" s="38">
         <v>3</v>
       </c>
@@ -5341,11 +5415,11 @@
       <c r="B114" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C114" s="147">
+      <c r="C114" s="152">
         <f>C110*0.02</f>
         <v>6000</v>
       </c>
-      <c r="D114" s="147"/>
+      <c r="D114" s="152"/>
       <c r="E114" s="38">
         <v>2</v>
       </c>
@@ -5427,6 +5501,17 @@
     <row r="171" s="34" customFormat="1"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="N41:T41"/>
+    <mergeCell ref="N54:T54"/>
+    <mergeCell ref="N62:T62"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C111:D111"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
@@ -5434,17 +5519,6 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="N41:T41"/>
-    <mergeCell ref="N54:T54"/>
-    <mergeCell ref="N62:T62"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="C112:D112"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B80" r:id="rId1"/>
@@ -5496,7 +5570,7 @@
     <row r="2" spans="1:10" ht="20.25" customHeight="1">
       <c r="A2" s="65"/>
       <c r="B2" s="66" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="66"/>
       <c r="D2" s="66"/>
@@ -5507,67 +5581,67 @@
     </row>
     <row r="3" spans="1:10" ht="17.399999999999999">
       <c r="A3" s="67" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="155" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="164" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="164"/>
-      <c r="D3" s="164"/>
-      <c r="E3" s="164"/>
-      <c r="F3" s="164"/>
-      <c r="G3" s="164"/>
-      <c r="H3" s="164"/>
+      <c r="C3" s="155"/>
+      <c r="D3" s="155"/>
+      <c r="E3" s="155"/>
+      <c r="F3" s="155"/>
+      <c r="G3" s="155"/>
+      <c r="H3" s="155"/>
     </row>
     <row r="4" spans="1:10" ht="15">
       <c r="A4" s="68"/>
-      <c r="B4" s="165" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="165"/>
-      <c r="D4" s="165"/>
-      <c r="E4" s="165"/>
-      <c r="F4" s="165"/>
-      <c r="G4" s="165"/>
-      <c r="H4" s="165"/>
+      <c r="B4" s="156" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="156"/>
+      <c r="D4" s="156"/>
+      <c r="E4" s="156"/>
+      <c r="F4" s="156"/>
+      <c r="G4" s="156"/>
+      <c r="H4" s="156"/>
     </row>
     <row r="5" spans="1:10" ht="32.4">
       <c r="A5" s="68"/>
       <c r="B5" s="69" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="69" t="s">
+      <c r="D5" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="E5" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="69" t="s">
+      <c r="F5" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="69" t="s">
+      <c r="G5" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="G5" s="69" t="s">
+      <c r="H5" s="69" t="s">
         <v>58</v>
-      </c>
-      <c r="H5" s="69" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="18">
       <c r="A6" s="68"/>
-      <c r="B6" s="166" t="s">
+      <c r="B6" s="157" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="69" t="s">
         <v>60</v>
-      </c>
-      <c r="C6" s="69" t="s">
-        <v>61</v>
       </c>
       <c r="D6" s="70">
         <v>1</v>
       </c>
       <c r="E6" s="71" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F6" s="72">
         <v>1225</v>
@@ -5580,15 +5654,15 @@
     </row>
     <row r="7" spans="1:10" ht="18">
       <c r="A7" s="68"/>
-      <c r="B7" s="167"/>
+      <c r="B7" s="158"/>
       <c r="C7" s="71" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="70">
         <v>2</v>
       </c>
       <c r="E7" s="71" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F7" s="73">
         <v>920</v>
@@ -5604,17 +5678,17 @@
     </row>
     <row r="8" spans="1:10" ht="43.8">
       <c r="A8" s="68"/>
-      <c r="B8" s="166" t="s">
+      <c r="B8" s="157" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="75" t="s">
         <v>64</v>
-      </c>
-      <c r="C8" s="75" t="s">
-        <v>65</v>
       </c>
       <c r="D8" s="70">
         <v>0</v>
       </c>
       <c r="E8" s="71" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F8" s="73">
         <v>58</v>
@@ -5627,15 +5701,15 @@
     </row>
     <row r="9" spans="1:10" ht="18">
       <c r="A9" s="68"/>
-      <c r="B9" s="166"/>
+      <c r="B9" s="157"/>
       <c r="C9" s="71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" s="76">
         <v>0.1028</v>
       </c>
       <c r="E9" s="71" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F9" s="73">
         <v>12131</v>
@@ -5648,15 +5722,15 @@
     </row>
     <row r="10" spans="1:10" ht="18">
       <c r="A10" s="68"/>
-      <c r="B10" s="166"/>
+      <c r="B10" s="157"/>
       <c r="C10" s="71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="76">
         <v>0.17150000000000001</v>
       </c>
       <c r="E10" s="71" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F10" s="73">
         <v>3177</v>
@@ -5673,15 +5747,15 @@
     </row>
     <row r="11" spans="1:10" ht="18">
       <c r="A11" s="68"/>
-      <c r="B11" s="166"/>
+      <c r="B11" s="157"/>
       <c r="C11" s="71" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11" s="76">
         <v>0.15160000000000001</v>
       </c>
       <c r="E11" s="71" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F11" s="73">
         <f>35*35.28</f>
@@ -5695,15 +5769,15 @@
     </row>
     <row r="12" spans="1:10" ht="18">
       <c r="A12" s="68"/>
-      <c r="B12" s="166"/>
+      <c r="B12" s="157"/>
       <c r="C12" s="71" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D12" s="76">
         <v>35</v>
       </c>
       <c r="E12" s="71" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F12" s="79">
         <f>100</f>
@@ -5721,15 +5795,15 @@
     </row>
     <row r="13" spans="1:10" ht="18">
       <c r="A13" s="68"/>
-      <c r="B13" s="166"/>
+      <c r="B13" s="157"/>
       <c r="C13" s="71" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" s="70">
         <v>90</v>
       </c>
       <c r="E13" s="71" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F13" s="73">
         <f>'[1]Update Descrip'!F665</f>
@@ -5751,7 +5825,7 @@
       <c r="D14" s="68"/>
       <c r="E14" s="68"/>
       <c r="F14" s="80" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G14" s="81"/>
       <c r="H14" s="82">
@@ -5761,11 +5835,11 @@
     </row>
     <row r="15" spans="1:10" ht="18">
       <c r="B15" s="83" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E15" s="68"/>
       <c r="F15" s="80" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G15" s="81"/>
       <c r="H15" s="73">
@@ -5775,19 +5849,19 @@
     </row>
     <row r="16" spans="1:10" ht="18">
       <c r="A16" s="84" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B16" s="73">
         <f>+H16</f>
         <v>9854.6899999999987</v>
       </c>
       <c r="C16" s="68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D16" s="68"/>
       <c r="E16" s="68"/>
       <c r="F16" s="80" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G16" s="81"/>
       <c r="H16" s="73">
@@ -5802,7 +5876,7 @@
       <c r="D17" s="68"/>
       <c r="E17" s="68"/>
       <c r="F17" s="80" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G17" s="81"/>
       <c r="H17" s="73">
@@ -5817,7 +5891,7 @@
       <c r="D18" s="68"/>
       <c r="E18" s="68"/>
       <c r="F18" s="80" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G18" s="81"/>
       <c r="H18" s="73">
@@ -5828,7 +5902,7 @@
     <row r="19" spans="1:8" ht="18">
       <c r="A19" s="84"/>
       <c r="B19" s="86" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C19" s="86"/>
       <c r="D19" s="86"/>
@@ -5842,74 +5916,74 @@
         <f>+A9+1</f>
         <v>1</v>
       </c>
-      <c r="B22" s="156"/>
-      <c r="C22" s="156"/>
-      <c r="D22" s="156"/>
-      <c r="E22" s="156"/>
-      <c r="F22" s="156"/>
-      <c r="G22" s="156"/>
-      <c r="H22" s="156"/>
+      <c r="B22" s="159"/>
+      <c r="C22" s="159"/>
+      <c r="D22" s="159"/>
+      <c r="E22" s="159"/>
+      <c r="F22" s="159"/>
+      <c r="G22" s="159"/>
+      <c r="H22" s="159"/>
     </row>
     <row r="23" spans="1:8" s="94" customFormat="1" ht="19.8">
       <c r="A23" s="95" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" s="159" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" s="159"/>
+      <c r="D23" s="159"/>
+      <c r="E23" s="159"/>
+      <c r="F23" s="159"/>
+      <c r="G23" s="159"/>
+      <c r="H23" s="159"/>
+    </row>
+    <row r="24" spans="1:8" s="94" customFormat="1" ht="15">
+      <c r="B24" s="161" t="s">
         <v>103</v>
       </c>
-      <c r="B23" s="156" t="s">
-        <v>117</v>
-      </c>
-      <c r="C23" s="156"/>
-      <c r="D23" s="156"/>
-      <c r="E23" s="156"/>
-      <c r="F23" s="156"/>
-      <c r="G23" s="156"/>
-      <c r="H23" s="156"/>
-    </row>
-    <row r="24" spans="1:8" s="94" customFormat="1" ht="15">
-      <c r="B24" s="157" t="s">
-        <v>104</v>
-      </c>
-      <c r="C24" s="157"/>
-      <c r="D24" s="157"/>
-      <c r="E24" s="157"/>
-      <c r="F24" s="157"/>
-      <c r="G24" s="157"/>
-      <c r="H24" s="157"/>
+      <c r="C24" s="161"/>
+      <c r="D24" s="161"/>
+      <c r="E24" s="161"/>
+      <c r="F24" s="161"/>
+      <c r="G24" s="161"/>
+      <c r="H24" s="161"/>
     </row>
     <row r="25" spans="1:8" s="94" customFormat="1" ht="30" customHeight="1">
       <c r="B25" s="96" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="96" t="s">
+      <c r="D25" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="96" t="s">
+      <c r="E25" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="E25" s="96" t="s">
+      <c r="F25" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="96" t="s">
+      <c r="G25" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="G25" s="96" t="s">
+      <c r="H25" s="96" t="s">
         <v>58</v>
       </c>
-      <c r="H25" s="96" t="s">
+    </row>
+    <row r="26" spans="1:8" s="94" customFormat="1" ht="24.75" customHeight="1">
+      <c r="B26" s="162" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" s="94" customFormat="1" ht="24.75" customHeight="1">
-      <c r="B26" s="158" t="s">
+      <c r="C26" s="97" t="s">
         <v>60</v>
-      </c>
-      <c r="C26" s="97" t="s">
-        <v>61</v>
       </c>
       <c r="D26" s="98">
         <v>17.2</v>
       </c>
       <c r="E26" s="99" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F26" s="100">
         <v>1225</v>
@@ -5921,15 +5995,15 @@
       <c r="H26" s="102"/>
     </row>
     <row r="27" spans="1:8" s="94" customFormat="1" ht="18">
-      <c r="B27" s="159"/>
+      <c r="B27" s="163"/>
       <c r="C27" s="103" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D27" s="104">
         <v>25.7</v>
       </c>
       <c r="E27" s="105" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F27" s="106">
         <v>920</v>
@@ -5944,17 +6018,17 @@
       </c>
     </row>
     <row r="28" spans="1:8" s="94" customFormat="1" ht="18">
-      <c r="B28" s="160" t="s">
-        <v>64</v>
+      <c r="B28" s="164" t="s">
+        <v>63</v>
       </c>
       <c r="C28" s="99" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D28" s="108">
         <v>16.5</v>
       </c>
       <c r="E28" s="99" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F28" s="101">
         <v>1215.8800000000001</v>
@@ -5966,15 +6040,15 @@
       <c r="H28" s="102"/>
     </row>
     <row r="29" spans="1:8" s="94" customFormat="1" ht="18">
-      <c r="B29" s="161"/>
+      <c r="B29" s="165"/>
       <c r="C29" s="103" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D29" s="109">
         <v>0.23200000000000001</v>
       </c>
       <c r="E29" s="103" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F29" s="106">
         <f>Jwood</f>
@@ -5987,15 +6061,15 @@
       <c r="H29" s="107"/>
     </row>
     <row r="30" spans="1:8" s="94" customFormat="1" ht="27.6">
-      <c r="B30" s="161"/>
+      <c r="B30" s="165"/>
       <c r="C30" s="110" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D30" s="109">
         <v>0</v>
       </c>
       <c r="E30" s="103" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F30" s="106">
         <f>'[7]update Rate'!$N$215</f>
@@ -6008,15 +6082,15 @@
       <c r="H30" s="107"/>
     </row>
     <row r="31" spans="1:8" s="94" customFormat="1" ht="18">
-      <c r="B31" s="162"/>
+      <c r="B31" s="166"/>
       <c r="C31" s="105" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D31" s="111">
         <v>25</v>
       </c>
       <c r="E31" s="105" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F31" s="112">
         <f>'[7]update Rate'!$N$59</f>
@@ -6033,7 +6107,7 @@
     </row>
     <row r="32" spans="1:8" s="94" customFormat="1" ht="18">
       <c r="F32" s="114" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G32" s="114"/>
       <c r="H32" s="112">
@@ -6043,10 +6117,10 @@
     </row>
     <row r="33" spans="1:8" s="94" customFormat="1" ht="18">
       <c r="B33" s="94" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F33" s="114" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G33" s="114"/>
       <c r="H33" s="115">
@@ -6061,17 +6135,17 @@
         <v>93614.91</v>
       </c>
       <c r="C34" s="116" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D34" s="115">
         <f>INT(B34/B35*100)/100</f>
         <v>936.14</v>
       </c>
       <c r="E34" s="94" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" s="114" t="s">
         <v>80</v>
-      </c>
-      <c r="F34" s="114" t="s">
-        <v>81</v>
       </c>
       <c r="G34" s="114"/>
       <c r="H34" s="115">
@@ -6085,54 +6159,54 @@
       </c>
     </row>
     <row r="36" spans="1:8" s="94" customFormat="1" ht="12" customHeight="1">
-      <c r="A36" s="163" t="s">
-        <v>119</v>
-      </c>
-      <c r="B36" s="163"/>
-      <c r="C36" s="163"/>
-      <c r="D36" s="163"/>
-      <c r="E36" s="163"/>
-      <c r="F36" s="163"/>
-      <c r="G36" s="163"/>
-      <c r="H36" s="163"/>
+      <c r="A36" s="167" t="s">
+        <v>118</v>
+      </c>
+      <c r="B36" s="167"/>
+      <c r="C36" s="167"/>
+      <c r="D36" s="167"/>
+      <c r="E36" s="167"/>
+      <c r="F36" s="167"/>
+      <c r="G36" s="167"/>
+      <c r="H36" s="167"/>
     </row>
     <row r="37" spans="1:8" s="94" customFormat="1" ht="12" customHeight="1">
       <c r="B37" s="119" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="94" customFormat="1" ht="12" customHeight="1">
+      <c r="A38" s="160" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" s="94" customFormat="1" ht="12" customHeight="1">
-      <c r="A38" s="155" t="s">
-        <v>113</v>
-      </c>
-      <c r="B38" s="155"/>
-      <c r="C38" s="155"/>
-      <c r="D38" s="155"/>
-      <c r="E38" s="155"/>
-      <c r="F38" s="155"/>
-      <c r="G38" s="155"/>
-      <c r="H38" s="155"/>
+      <c r="B38" s="160"/>
+      <c r="C38" s="160"/>
+      <c r="D38" s="160"/>
+      <c r="E38" s="160"/>
+      <c r="F38" s="160"/>
+      <c r="G38" s="160"/>
+      <c r="H38" s="160"/>
     </row>
     <row r="39" spans="1:8" s="94" customFormat="1" ht="12" customHeight="1">
       <c r="B39" s="119" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="94" customFormat="1" ht="12" customHeight="1">
+      <c r="A40" s="160" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" s="94" customFormat="1" ht="12" customHeight="1">
-      <c r="A40" s="155" t="s">
-        <v>115</v>
-      </c>
-      <c r="B40" s="155"/>
-      <c r="C40" s="155"/>
-      <c r="D40" s="155"/>
-      <c r="E40" s="155"/>
-      <c r="F40" s="155"/>
-      <c r="G40" s="155"/>
-      <c r="H40" s="155"/>
+      <c r="B40" s="160"/>
+      <c r="C40" s="160"/>
+      <c r="D40" s="160"/>
+      <c r="E40" s="160"/>
+      <c r="F40" s="160"/>
+      <c r="G40" s="160"/>
+      <c r="H40" s="160"/>
     </row>
     <row r="41" spans="1:8" s="94" customFormat="1" ht="12" customHeight="1">
       <c r="B41" s="119" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="94" customFormat="1" ht="12" customHeight="1">
@@ -6140,11 +6214,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="B22:H22"/>
     <mergeCell ref="A38:H38"/>
     <mergeCell ref="A40:H40"/>
     <mergeCell ref="B23:H23"/>
@@ -6152,6 +6221,11 @@
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="A36:H36"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="B22:H22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6160,10 +6234,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T171"/>
+  <dimension ref="A1:T184"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I104" sqref="I104"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G112" sqref="G112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6173,121 +6247,121 @@
     <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5546875" customWidth="1"/>
     <col min="5" max="5" width="8.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.44140625" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.88671875" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
-      <c r="A1" s="152" t="s">
+      <c r="A1" s="147" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="152"/>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
-      <c r="H1" s="152"/>
-      <c r="I1" s="152"/>
-      <c r="J1" s="152"/>
-      <c r="K1" s="152"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147"/>
+      <c r="G1" s="147"/>
+      <c r="H1" s="147"/>
+      <c r="I1" s="147"/>
+      <c r="J1" s="147"/>
+      <c r="K1" s="147"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="22.8">
-      <c r="A2" s="153" t="s">
+      <c r="A2" s="148" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="153"/>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
-      <c r="G2" s="153"/>
-      <c r="H2" s="153"/>
-      <c r="I2" s="153"/>
-      <c r="J2" s="153"/>
-      <c r="K2" s="153"/>
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="148"/>
+      <c r="K2" s="148"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1">
-      <c r="A3" s="144" t="s">
+      <c r="A3" s="136" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="144"/>
-      <c r="C3" s="144"/>
-      <c r="D3" s="144"/>
-      <c r="E3" s="144"/>
-      <c r="F3" s="144"/>
-      <c r="G3" s="144"/>
-      <c r="H3" s="144"/>
-      <c r="I3" s="144"/>
-      <c r="J3" s="144"/>
-      <c r="K3" s="144"/>
+      <c r="B3" s="136"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="136"/>
+      <c r="E3" s="136"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="136"/>
+      <c r="H3" s="136"/>
+      <c r="I3" s="136"/>
+      <c r="J3" s="136"/>
+      <c r="K3" s="136"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1">
-      <c r="A4" s="144" t="s">
+      <c r="A4" s="136" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="144"/>
-      <c r="C4" s="144"/>
-      <c r="D4" s="144"/>
-      <c r="E4" s="144"/>
-      <c r="F4" s="144"/>
-      <c r="G4" s="144"/>
-      <c r="H4" s="144"/>
-      <c r="I4" s="144"/>
-      <c r="J4" s="144"/>
-      <c r="K4" s="144"/>
+      <c r="B4" s="136"/>
+      <c r="C4" s="136"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
+      <c r="H4" s="136"/>
+      <c r="I4" s="136"/>
+      <c r="J4" s="136"/>
+      <c r="K4" s="136"/>
     </row>
     <row r="5" spans="1:14" ht="17.399999999999999">
-      <c r="A5" s="154" t="s">
+      <c r="A5" s="149" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="154"/>
-      <c r="C5" s="154"/>
-      <c r="D5" s="154"/>
-      <c r="E5" s="154"/>
-      <c r="F5" s="154"/>
-      <c r="G5" s="154"/>
-      <c r="H5" s="154"/>
-      <c r="I5" s="154"/>
-      <c r="J5" s="154"/>
-      <c r="K5" s="154"/>
+      <c r="B5" s="149"/>
+      <c r="C5" s="149"/>
+      <c r="D5" s="149"/>
+      <c r="E5" s="149"/>
+      <c r="F5" s="149"/>
+      <c r="G5" s="149"/>
+      <c r="H5" s="149"/>
+      <c r="I5" s="149"/>
+      <c r="J5" s="149"/>
+      <c r="K5" s="149"/>
     </row>
     <row r="6" spans="1:14" ht="15.6">
-      <c r="A6" s="134" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="134"/>
-      <c r="C6" s="134"/>
-      <c r="D6" s="134"/>
-      <c r="E6" s="134"/>
-      <c r="F6" s="134"/>
+      <c r="A6" s="140" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="140"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="140"/>
+      <c r="F6" s="140"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="151" t="s">
+      <c r="H6" s="146" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="151"/>
-      <c r="J6" s="151"/>
-      <c r="K6" s="151"/>
+      <c r="I6" s="146"/>
+      <c r="J6" s="146"/>
+      <c r="K6" s="146"/>
     </row>
     <row r="7" spans="1:14" ht="15.6">
-      <c r="A7" s="148" t="s">
+      <c r="A7" s="150" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="148"/>
-      <c r="C7" s="148"/>
-      <c r="D7" s="148"/>
-      <c r="E7" s="148"/>
-      <c r="F7" s="148"/>
+      <c r="B7" s="150"/>
+      <c r="C7" s="150"/>
+      <c r="D7" s="150"/>
+      <c r="E7" s="150"/>
+      <c r="F7" s="150"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="149" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="149"/>
-      <c r="J7" s="149"/>
-      <c r="K7" s="149"/>
+      <c r="H7" s="151" t="s">
+        <v>141</v>
+      </c>
+      <c r="I7" s="151"/>
+      <c r="J7" s="151"/>
+      <c r="K7" s="151"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1">
       <c r="A8" s="4" t="s">
@@ -6329,7 +6403,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="60"/>
       <c r="D9" s="38"/>
@@ -6344,7 +6418,7 @@
     <row r="10" spans="1:14" ht="15" customHeight="1">
       <c r="A10" s="18"/>
       <c r="B10" s="36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="35">
         <v>1</v>
@@ -6484,7 +6558,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="35"/>
       <c r="D16" s="37"/>
@@ -6499,7 +6573,7 @@
     <row r="17" spans="1:19" ht="15" customHeight="1">
       <c r="A17" s="18"/>
       <c r="B17" s="36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="35">
         <v>2</v>
@@ -6587,7 +6661,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" s="35"/>
       <c r="D21" s="37"/>
@@ -6602,7 +6676,7 @@
     <row r="22" spans="1:19" ht="15" customHeight="1">
       <c r="A22" s="18"/>
       <c r="B22" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C22" s="35">
         <v>2</v>
@@ -6644,7 +6718,7 @@
         <v>1.7555623285583659</v>
       </c>
       <c r="H23" s="39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I23" s="39">
         <v>1950.4</v>
@@ -6691,7 +6765,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="87" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C26" s="19"/>
       <c r="D26" s="20"/>
@@ -6713,7 +6787,7 @@
     <row r="27" spans="1:19" ht="15" customHeight="1">
       <c r="A27" s="18"/>
       <c r="B27" s="36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C27" s="19">
         <v>1</v>
@@ -6751,7 +6825,7 @@
         <v>0.48765620237732393</v>
       </c>
       <c r="H28" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I28" s="23">
         <v>663.31</v>
@@ -6780,7 +6854,7 @@
         <v>5</v>
       </c>
       <c r="B30" s="89" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C30" s="19"/>
       <c r="D30" s="20"/>
@@ -6881,7 +6955,7 @@
         <v>6</v>
       </c>
       <c r="B35" s="89" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C35" s="19"/>
       <c r="D35" s="20"/>
@@ -6937,7 +7011,7 @@
         <v>0.68271868332825347</v>
       </c>
       <c r="H37" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I37" s="23">
         <v>1014.97</v>
@@ -6984,7 +7058,7 @@
         <v>7</v>
       </c>
       <c r="B40" s="60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C40" s="35"/>
       <c r="D40" s="37"/>
@@ -6996,7 +7070,7 @@
       <c r="J40" s="41"/>
       <c r="K40" s="21"/>
       <c r="N40" s="66" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O40" s="66"/>
       <c r="P40" s="66"/>
@@ -7008,7 +7082,7 @@
     <row r="41" spans="1:20" ht="15" customHeight="1">
       <c r="A41" s="18"/>
       <c r="B41" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C41" s="35">
         <v>2</v>
@@ -7031,15 +7105,15 @@
       <c r="I41" s="39"/>
       <c r="J41" s="39"/>
       <c r="K41" s="61"/>
-      <c r="N41" s="146" t="s">
-        <v>88</v>
-      </c>
-      <c r="O41" s="146"/>
-      <c r="P41" s="146"/>
-      <c r="Q41" s="146"/>
-      <c r="R41" s="146"/>
-      <c r="S41" s="146"/>
-      <c r="T41" s="146"/>
+      <c r="N41" s="154" t="s">
+        <v>87</v>
+      </c>
+      <c r="O41" s="154"/>
+      <c r="P41" s="154"/>
+      <c r="Q41" s="154"/>
+      <c r="R41" s="154"/>
+      <c r="S41" s="154"/>
+      <c r="T41" s="154"/>
     </row>
     <row r="42" spans="1:20" ht="15" customHeight="1">
       <c r="A42" s="18"/>
@@ -7055,7 +7129,7 @@
         <v>1.7555623285583659</v>
       </c>
       <c r="H42" s="39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I42" s="39">
         <v>8569.2999999999993</v>
@@ -7106,22 +7180,22 @@
         <v>8</v>
       </c>
       <c r="B45" s="89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C45" s="19" t="s">
         <v>7</v>
       </c>
       <c r="D45" s="90" t="s">
+        <v>94</v>
+      </c>
+      <c r="E45" s="91" t="s">
         <v>95</v>
       </c>
-      <c r="E45" s="91" t="s">
+      <c r="F45" s="91" t="s">
         <v>96</v>
       </c>
-      <c r="F45" s="91" t="s">
+      <c r="G45" s="91" t="s">
         <v>97</v>
-      </c>
-      <c r="G45" s="91" t="s">
-        <v>98</v>
       </c>
       <c r="H45" s="22"/>
       <c r="I45" s="23"/>
@@ -7131,7 +7205,7 @@
     <row r="46" spans="1:20" ht="15" customHeight="1">
       <c r="A46" s="18"/>
       <c r="B46" s="36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C46" s="19">
         <f>TRUNC((D47-0.1)/0.15,0)+1</f>
@@ -7253,7 +7327,7 @@
         <v>2.3221315392401441E-2</v>
       </c>
       <c r="H50" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I50" s="23">
         <v>131940</v>
@@ -7300,7 +7374,7 @@
         <v>9</v>
       </c>
       <c r="B53" s="89" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C53" s="19"/>
       <c r="D53" s="20"/>
@@ -7315,7 +7389,7 @@
     <row r="54" spans="1:20" ht="15" customHeight="1">
       <c r="A54" s="18"/>
       <c r="B54" s="36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C54" s="35">
         <f>2*13</f>
@@ -7336,15 +7410,15 @@
       <c r="I54" s="39"/>
       <c r="J54" s="39"/>
       <c r="K54" s="61"/>
-      <c r="N54" s="146" t="s">
-        <v>88</v>
-      </c>
-      <c r="O54" s="146"/>
-      <c r="P54" s="146"/>
-      <c r="Q54" s="146"/>
-      <c r="R54" s="146"/>
-      <c r="S54" s="146"/>
-      <c r="T54" s="146"/>
+      <c r="N54" s="154" t="s">
+        <v>87</v>
+      </c>
+      <c r="O54" s="154"/>
+      <c r="P54" s="154"/>
+      <c r="Q54" s="154"/>
+      <c r="R54" s="154"/>
+      <c r="S54" s="154"/>
+      <c r="T54" s="154"/>
     </row>
     <row r="55" spans="1:20" ht="15" customHeight="1">
       <c r="A55" s="18"/>
@@ -7497,7 +7571,7 @@
         <v>10</v>
       </c>
       <c r="B61" s="89" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C61" s="35"/>
       <c r="D61" s="37"/>
@@ -7516,7 +7590,7 @@
     <row r="62" spans="1:20" ht="15" customHeight="1">
       <c r="A62" s="18"/>
       <c r="B62" s="36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C62" s="35">
         <v>1</v>
@@ -7540,15 +7614,15 @@
       <c r="I62" s="39"/>
       <c r="J62" s="39"/>
       <c r="K62" s="61"/>
-      <c r="N62" s="146" t="s">
-        <v>88</v>
-      </c>
-      <c r="O62" s="146"/>
-      <c r="P62" s="146"/>
-      <c r="Q62" s="146"/>
-      <c r="R62" s="146"/>
-      <c r="S62" s="146"/>
-      <c r="T62" s="146"/>
+      <c r="N62" s="154" t="s">
+        <v>87</v>
+      </c>
+      <c r="O62" s="154"/>
+      <c r="P62" s="154"/>
+      <c r="Q62" s="154"/>
+      <c r="R62" s="154"/>
+      <c r="S62" s="154"/>
+      <c r="T62" s="154"/>
     </row>
     <row r="63" spans="1:20" ht="15" customHeight="1">
       <c r="A63" s="18"/>
@@ -7596,7 +7670,7 @@
         <v>0.75815300213349579</v>
       </c>
       <c r="H64" s="39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I64" s="23">
         <f>81404.27/100</f>
@@ -7644,22 +7718,22 @@
         <v>11</v>
       </c>
       <c r="B67" s="121" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C67" s="19" t="s">
         <v>7</v>
       </c>
       <c r="D67" s="90" t="s">
+        <v>94</v>
+      </c>
+      <c r="E67" s="91" t="s">
         <v>95</v>
       </c>
-      <c r="E67" s="91" t="s">
+      <c r="F67" s="91" t="s">
         <v>96</v>
       </c>
-      <c r="F67" s="91" t="s">
-        <v>97</v>
-      </c>
       <c r="G67" s="91" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H67" s="22"/>
       <c r="I67" s="23"/>
@@ -7669,7 +7743,7 @@
     <row r="68" spans="1:13">
       <c r="A68" s="122"/>
       <c r="B68" s="126" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C68" s="124">
         <v>6</v>
@@ -7723,7 +7797,7 @@
     <row r="70" spans="1:13">
       <c r="A70" s="122"/>
       <c r="B70" s="126" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C70" s="124">
         <f>TRUNC(D75/0.1,0)</f>
@@ -7752,7 +7826,7 @@
     <row r="71" spans="1:13" s="1" customFormat="1" ht="27.6">
       <c r="A71" s="122"/>
       <c r="B71" s="127" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C71" s="124">
         <v>4</v>
@@ -7781,7 +7855,7 @@
     <row r="72" spans="1:13" s="1" customFormat="1" ht="41.4">
       <c r="A72" s="122"/>
       <c r="B72" s="127" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C72" s="124">
         <v>1</v>
@@ -7837,7 +7911,7 @@
     <row r="74" spans="1:13" s="1" customFormat="1" ht="27.6">
       <c r="A74" s="122"/>
       <c r="B74" s="127" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C74" s="124">
         <v>1</v>
@@ -7866,7 +7940,7 @@
     <row r="75" spans="1:13" s="1" customFormat="1">
       <c r="A75" s="122"/>
       <c r="B75" s="127" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C75" s="124">
         <v>2</v>
@@ -7895,7 +7969,7 @@
     <row r="76" spans="1:13" s="1" customFormat="1">
       <c r="A76" s="122"/>
       <c r="B76" s="127" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C76" s="124">
         <f>C70</f>
@@ -7936,7 +8010,7 @@
         <v>734.74624078024999</v>
       </c>
       <c r="H77" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I77" s="23">
         <v>181.17</v>
@@ -7983,7 +8057,7 @@
         <v>12</v>
       </c>
       <c r="B80" s="130" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C80" s="19"/>
       <c r="D80" s="20"/>
@@ -7998,7 +8072,7 @@
     <row r="81" spans="1:11" s="1" customFormat="1">
       <c r="A81" s="18"/>
       <c r="B81" s="127" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C81" s="19">
         <v>2</v>
@@ -8210,7 +8284,7 @@
     <row r="90" spans="1:11" s="1" customFormat="1">
       <c r="A90" s="18"/>
       <c r="B90" s="127" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C90" s="19"/>
       <c r="D90" s="20"/>
@@ -8235,7 +8309,7 @@
     <row r="91" spans="1:11" s="1" customFormat="1">
       <c r="A91" s="18"/>
       <c r="B91" s="127" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C91" s="19"/>
       <c r="D91" s="20"/>
@@ -8268,7 +8342,7 @@
         <v>13</v>
       </c>
       <c r="B93" s="121" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C93" s="19"/>
       <c r="D93" s="20"/>
@@ -8283,7 +8357,7 @@
     <row r="94" spans="1:11" ht="15" customHeight="1">
       <c r="A94" s="18"/>
       <c r="B94" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C94" s="19">
         <v>1</v>
@@ -8343,7 +8417,7 @@
       </c>
       <c r="K96" s="21"/>
     </row>
-    <row r="97" spans="1:11" ht="15" customHeight="1">
+    <row r="97" spans="1:20" ht="15" customHeight="1">
       <c r="A97" s="18"/>
       <c r="B97" s="36"/>
       <c r="C97" s="19"/>
@@ -8356,12 +8430,12 @@
       <c r="J97" s="40"/>
       <c r="K97" s="21"/>
     </row>
-    <row r="98" spans="1:11" s="1" customFormat="1" ht="30">
+    <row r="98" spans="1:20" s="1" customFormat="1" ht="30">
       <c r="A98" s="18">
         <v>14</v>
       </c>
       <c r="B98" s="121" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C98" s="19"/>
       <c r="D98" s="20"/>
@@ -8373,10 +8447,10 @@
       <c r="J98" s="125"/>
       <c r="K98" s="21"/>
     </row>
-    <row r="99" spans="1:11" ht="15" customHeight="1">
+    <row r="99" spans="1:20" ht="15" customHeight="1">
       <c r="A99" s="18"/>
       <c r="B99" s="36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C99" s="19">
         <v>1</v>
@@ -8399,7 +8473,7 @@
       <c r="J99" s="40"/>
       <c r="K99" s="21"/>
     </row>
-    <row r="100" spans="1:11" ht="15" customHeight="1">
+    <row r="100" spans="1:20" ht="15" customHeight="1">
       <c r="A100" s="18"/>
       <c r="B100" s="36" t="s">
         <v>41</v>
@@ -8424,7 +8498,7 @@
       </c>
       <c r="K100" s="21"/>
     </row>
-    <row r="101" spans="1:11" ht="15" customHeight="1">
+    <row r="101" spans="1:20" ht="15" customHeight="1">
       <c r="A101" s="18"/>
       <c r="B101" s="36" t="s">
         <v>40</v>
@@ -8442,7 +8516,7 @@
       </c>
       <c r="K101" s="21"/>
     </row>
-    <row r="102" spans="1:11" ht="15" customHeight="1">
+    <row r="102" spans="1:20" ht="15" customHeight="1">
       <c r="A102" s="18"/>
       <c r="B102" s="36"/>
       <c r="C102" s="19"/>
@@ -8455,266 +8529,540 @@
       <c r="J102" s="40"/>
       <c r="K102" s="21"/>
     </row>
-    <row r="103" spans="1:11" ht="15" customHeight="1">
-      <c r="A103" s="18">
+    <row r="103" spans="1:20" s="180" customFormat="1" ht="17.399999999999999">
+      <c r="A103" s="177">
         <v>15</v>
       </c>
-      <c r="B103" s="36" t="s">
+      <c r="B103" s="168" t="s">
+        <v>142</v>
+      </c>
+      <c r="C103" s="169"/>
+      <c r="D103" s="170"/>
+      <c r="E103" s="178"/>
+      <c r="F103" s="170" t="s">
+        <v>145</v>
+      </c>
+      <c r="G103" s="170"/>
+      <c r="H103" s="170"/>
+      <c r="I103" s="170"/>
+      <c r="J103" s="172"/>
+      <c r="K103" s="179"/>
+    </row>
+    <row r="104" spans="1:20" ht="15" customHeight="1">
+      <c r="A104" s="18"/>
+      <c r="B104" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="C104" s="35">
+        <v>1</v>
+      </c>
+      <c r="D104" s="37"/>
+      <c r="E104" s="5"/>
+      <c r="F104" s="173">
+        <f>CONVERT(48.3735,"ft2","m2")</f>
+        <v>4.49404520544</v>
+      </c>
+      <c r="G104" s="128">
+        <f>PRODUCT(C104:F104)</f>
+        <v>4.49404520544</v>
+      </c>
+      <c r="H104" s="39"/>
+      <c r="I104" s="39"/>
+      <c r="J104" s="39"/>
+      <c r="K104" s="21"/>
+      <c r="M104" s="1"/>
+      <c r="N104" s="1"/>
+      <c r="O104" s="1"/>
+      <c r="P104" s="88"/>
+      <c r="Q104" s="88"/>
+    </row>
+    <row r="105" spans="1:20" ht="15" customHeight="1">
+      <c r="A105" s="18"/>
+      <c r="B105" s="36"/>
+      <c r="C105" s="35">
+        <v>1</v>
+      </c>
+      <c r="D105" s="37"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="173">
+        <f>CONVERT(224.2762,"ft2","m2")</f>
+        <v>20.835940779647999</v>
+      </c>
+      <c r="G105" s="128">
+        <f>PRODUCT(C105:F105)</f>
+        <v>20.835940779647999</v>
+      </c>
+      <c r="H105" s="39"/>
+      <c r="I105" s="39"/>
+      <c r="J105" s="39"/>
+      <c r="K105" s="21"/>
+      <c r="M105" s="1"/>
+      <c r="N105" s="1"/>
+      <c r="O105" s="1"/>
+      <c r="P105" s="88"/>
+      <c r="Q105" s="88"/>
+    </row>
+    <row r="106" spans="1:20" ht="15" customHeight="1">
+      <c r="A106" s="18"/>
+      <c r="B106" s="36"/>
+      <c r="C106" s="35">
+        <v>1</v>
+      </c>
+      <c r="D106" s="37">
+        <v>4.25</v>
+      </c>
+      <c r="E106" s="37">
+        <f>2.6</f>
+        <v>2.6</v>
+      </c>
+      <c r="F106" s="37"/>
+      <c r="G106" s="128">
+        <f t="shared" ref="G106:G107" si="7">PRODUCT(C106:F106)</f>
+        <v>11.05</v>
+      </c>
+      <c r="H106" s="39"/>
+      <c r="I106" s="39"/>
+      <c r="J106" s="39"/>
+      <c r="K106" s="21"/>
+      <c r="M106" s="1"/>
+      <c r="N106" s="1"/>
+      <c r="O106" s="1"/>
+      <c r="P106" s="88"/>
+      <c r="Q106" s="88"/>
+    </row>
+    <row r="107" spans="1:20" ht="15" customHeight="1">
+      <c r="A107" s="18"/>
+      <c r="B107" s="36"/>
+      <c r="C107" s="35">
+        <v>1</v>
+      </c>
+      <c r="D107" s="37">
+        <v>7</v>
+      </c>
+      <c r="E107" s="37">
+        <f>((2.5+4.75)/2)/3.281</f>
+        <v>1.1048460835111247</v>
+      </c>
+      <c r="F107" s="37"/>
+      <c r="G107" s="128">
+        <f t="shared" si="7"/>
+        <v>7.733922584577873</v>
+      </c>
+      <c r="H107" s="39"/>
+      <c r="I107" s="39"/>
+      <c r="J107" s="39"/>
+      <c r="K107" s="21"/>
+      <c r="M107" s="1"/>
+      <c r="N107" s="174" t="s">
+        <v>146</v>
+      </c>
+      <c r="O107" s="174"/>
+      <c r="P107" s="174"/>
+      <c r="Q107" s="174"/>
+      <c r="R107" s="174"/>
+      <c r="S107" s="174"/>
+      <c r="T107" s="174"/>
+    </row>
+    <row r="108" spans="1:20" ht="15" customHeight="1">
+      <c r="A108" s="18"/>
+      <c r="B108" s="36"/>
+      <c r="C108" s="35"/>
+      <c r="D108" s="37"/>
+      <c r="E108" s="37"/>
+      <c r="F108" s="37"/>
+      <c r="G108" s="128"/>
+      <c r="H108" s="39"/>
+      <c r="I108" s="39"/>
+      <c r="J108" s="39"/>
+      <c r="K108" s="21"/>
+      <c r="M108" s="1"/>
+      <c r="N108" s="174" t="s">
+        <v>147</v>
+      </c>
+      <c r="O108" s="174"/>
+      <c r="P108" s="174"/>
+      <c r="Q108" s="174"/>
+      <c r="R108" s="174"/>
+      <c r="S108" s="174"/>
+      <c r="T108" s="174"/>
+    </row>
+    <row r="109" spans="1:20" ht="15" customHeight="1">
+      <c r="A109" s="39"/>
+      <c r="B109" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C109" s="169"/>
+      <c r="D109" s="170"/>
+      <c r="E109" s="170"/>
+      <c r="F109" s="170"/>
+      <c r="G109" s="171">
+        <f>SUM(G104:G108)</f>
+        <v>44.113908569665874</v>
+      </c>
+      <c r="H109" s="171" t="s">
+        <v>144</v>
+      </c>
+      <c r="I109" s="171">
+        <f>35*10.7639</f>
+        <v>376.73649999999998</v>
+      </c>
+      <c r="J109" s="172">
+        <f>G109*I109</f>
+        <v>16619.319515855928</v>
+      </c>
+      <c r="K109" s="35"/>
+    </row>
+    <row r="110" spans="1:20" ht="15" customHeight="1">
+      <c r="A110" s="39"/>
+      <c r="B110" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C110" s="169"/>
+      <c r="D110" s="170"/>
+      <c r="E110" s="170"/>
+      <c r="F110" s="170"/>
+      <c r="G110" s="170"/>
+      <c r="H110" s="170"/>
+      <c r="I110" s="170"/>
+      <c r="J110" s="41">
+        <f>0.13*J109</f>
+        <v>2160.5115370612707</v>
+      </c>
+      <c r="K110" s="35"/>
+    </row>
+    <row r="111" spans="1:20" ht="15" customHeight="1">
+      <c r="A111" s="39"/>
+      <c r="B111" s="36"/>
+      <c r="C111" s="169"/>
+      <c r="D111" s="170"/>
+      <c r="E111" s="170"/>
+      <c r="F111" s="170"/>
+      <c r="G111" s="170"/>
+      <c r="H111" s="170"/>
+      <c r="I111" s="170"/>
+      <c r="J111" s="41"/>
+      <c r="K111" s="35"/>
+    </row>
+    <row r="112" spans="1:20" s="1" customFormat="1" ht="45">
+      <c r="A112" s="59">
+        <v>16</v>
+      </c>
+      <c r="B112" s="175" t="s">
+        <v>148</v>
+      </c>
+      <c r="C112" s="176"/>
+      <c r="D112" s="38"/>
+      <c r="E112" s="38"/>
+      <c r="F112" s="38"/>
+      <c r="G112" s="38"/>
+      <c r="H112" s="38"/>
+      <c r="I112" s="38"/>
+      <c r="J112" s="41"/>
+      <c r="K112" s="28"/>
+    </row>
+    <row r="113" spans="1:11" ht="15" customHeight="1">
+      <c r="A113" s="39"/>
+      <c r="B113" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="C113" s="169"/>
+      <c r="D113" s="170"/>
+      <c r="E113" s="170"/>
+      <c r="F113" s="170"/>
+      <c r="G113" s="170">
+        <f>G109</f>
+        <v>44.113908569665874</v>
+      </c>
+      <c r="H113" s="170"/>
+      <c r="I113" s="170"/>
+      <c r="J113" s="41"/>
+      <c r="K113" s="35"/>
+    </row>
+    <row r="114" spans="1:11" ht="15" customHeight="1">
+      <c r="A114" s="39"/>
+      <c r="B114" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C114" s="169"/>
+      <c r="D114" s="170"/>
+      <c r="E114" s="170"/>
+      <c r="F114" s="170"/>
+      <c r="G114" s="171">
+        <f>SUM(G113)</f>
+        <v>44.113908569665874</v>
+      </c>
+      <c r="H114" s="171" t="s">
+        <v>144</v>
+      </c>
+      <c r="I114" s="171">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="J114" s="172">
+        <f>G114*I114</f>
+        <v>405.84795884092603</v>
+      </c>
+      <c r="K114" s="35"/>
+    </row>
+    <row r="115" spans="1:11" ht="15" customHeight="1">
+      <c r="A115" s="18"/>
+      <c r="B115" s="36"/>
+      <c r="C115" s="19"/>
+      <c r="D115" s="20"/>
+      <c r="E115" s="21"/>
+      <c r="F115" s="21"/>
+      <c r="G115" s="23"/>
+      <c r="H115" s="22"/>
+      <c r="I115" s="23"/>
+      <c r="J115" s="40"/>
+      <c r="K115" s="21"/>
+    </row>
+    <row r="116" spans="1:11" ht="15" customHeight="1">
+      <c r="A116" s="18">
+        <v>17</v>
+      </c>
+      <c r="B116" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="C116" s="19">
+        <v>1</v>
+      </c>
+      <c r="D116" s="20"/>
+      <c r="E116" s="21"/>
+      <c r="F116" s="21"/>
+      <c r="G116" s="128">
+        <f t="shared" ref="G116" si="8">PRODUCT(C116:F116)</f>
+        <v>1</v>
+      </c>
+      <c r="H116" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="C103" s="19">
+      <c r="I116" s="23">
+        <v>3000</v>
+      </c>
+      <c r="J116" s="33">
+        <f>G116*I116</f>
+        <v>3000</v>
+      </c>
+      <c r="K116" s="21"/>
+    </row>
+    <row r="117" spans="1:11" ht="15" customHeight="1">
+      <c r="A117" s="18"/>
+      <c r="B117" s="36"/>
+      <c r="C117" s="19"/>
+      <c r="D117" s="20"/>
+      <c r="E117" s="21"/>
+      <c r="F117" s="21"/>
+      <c r="G117" s="23"/>
+      <c r="H117" s="22"/>
+      <c r="I117" s="23"/>
+      <c r="J117" s="40"/>
+      <c r="K117" s="21"/>
+    </row>
+    <row r="118" spans="1:11" ht="15" customHeight="1">
+      <c r="A118" s="18">
+        <v>18</v>
+      </c>
+      <c r="B118" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C118" s="19">
         <v>1</v>
       </c>
-      <c r="D103" s="20"/>
-      <c r="E103" s="21"/>
-      <c r="F103" s="21"/>
-      <c r="G103" s="128">
-        <f t="shared" ref="G103" si="7">PRODUCT(C103:F103)</f>
+      <c r="D118" s="20"/>
+      <c r="E118" s="21"/>
+      <c r="F118" s="21"/>
+      <c r="G118" s="33">
+        <f t="shared" ref="G118" si="9">PRODUCT(C118:F118)</f>
         <v>1</v>
       </c>
-      <c r="H103" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="I103" s="23">
-        <v>3000</v>
-      </c>
-      <c r="J103" s="33">
-        <f>G103*I103</f>
-        <v>3000</v>
-      </c>
-      <c r="K103" s="21"/>
-    </row>
-    <row r="104" spans="1:11" ht="15" customHeight="1">
-      <c r="A104" s="18"/>
-      <c r="B104" s="36"/>
-      <c r="C104" s="19"/>
-      <c r="D104" s="20"/>
-      <c r="E104" s="21"/>
-      <c r="F104" s="21"/>
-      <c r="G104" s="23"/>
-      <c r="H104" s="22"/>
-      <c r="I104" s="23"/>
-      <c r="J104" s="40"/>
-      <c r="K104" s="21"/>
-    </row>
-    <row r="105" spans="1:11" ht="15" customHeight="1">
-      <c r="A105" s="18">
-        <v>15</v>
-      </c>
-      <c r="B105" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C105" s="19">
-        <v>1</v>
-      </c>
-      <c r="D105" s="20"/>
-      <c r="E105" s="21"/>
-      <c r="F105" s="21"/>
-      <c r="G105" s="33">
-        <f t="shared" ref="G105" si="8">PRODUCT(C105:F105)</f>
-        <v>1</v>
-      </c>
-      <c r="H105" s="22" t="s">
+      <c r="H118" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="I105" s="23">
+      <c r="I118" s="23">
         <v>500</v>
       </c>
-      <c r="J105" s="33">
-        <f>G105*I105</f>
+      <c r="J118" s="33">
+        <f>G118*I118</f>
         <v>500</v>
       </c>
-      <c r="K105" s="21"/>
-    </row>
-    <row r="106" spans="1:11" ht="15" customHeight="1">
-      <c r="A106" s="18"/>
-      <c r="B106" s="24"/>
-      <c r="C106" s="19"/>
-      <c r="D106" s="20"/>
-      <c r="E106" s="21"/>
-      <c r="F106" s="21"/>
-      <c r="G106" s="23"/>
-      <c r="H106" s="22"/>
-      <c r="I106" s="23"/>
-      <c r="J106" s="40"/>
-      <c r="K106" s="21"/>
-    </row>
-    <row r="107" spans="1:11">
-      <c r="A107" s="39"/>
-      <c r="B107" s="42" t="s">
+      <c r="K118" s="21"/>
+    </row>
+    <row r="119" spans="1:11" ht="15" customHeight="1">
+      <c r="A119" s="18"/>
+      <c r="B119" s="24"/>
+      <c r="C119" s="19"/>
+      <c r="D119" s="20"/>
+      <c r="E119" s="21"/>
+      <c r="F119" s="21"/>
+      <c r="G119" s="23"/>
+      <c r="H119" s="22"/>
+      <c r="I119" s="23"/>
+      <c r="J119" s="40"/>
+      <c r="K119" s="21"/>
+    </row>
+    <row r="120" spans="1:11">
+      <c r="A120" s="39"/>
+      <c r="B120" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C107" s="43"/>
-      <c r="D107" s="37"/>
-      <c r="E107" s="37"/>
-      <c r="F107" s="37"/>
-      <c r="G107" s="40"/>
-      <c r="H107" s="40"/>
-      <c r="I107" s="40"/>
-      <c r="J107" s="40">
-        <f>SUM(J9:J105)</f>
-        <v>336917.6969730733</v>
-      </c>
-      <c r="K107" s="35"/>
-    </row>
-    <row r="108" spans="1:11">
-      <c r="A108" s="54"/>
-      <c r="B108" s="57"/>
-      <c r="C108" s="58"/>
-      <c r="D108" s="55"/>
-      <c r="E108" s="55"/>
-      <c r="F108" s="55"/>
-      <c r="G108" s="56"/>
-      <c r="H108" s="56"/>
-      <c r="I108" s="56"/>
-      <c r="J108" s="56"/>
-      <c r="K108" s="53"/>
-    </row>
-    <row r="109" spans="1:11" s="1" customFormat="1">
-      <c r="A109" s="46"/>
-      <c r="B109" s="28" t="s">
+      <c r="C120" s="43"/>
+      <c r="D120" s="37"/>
+      <c r="E120" s="37"/>
+      <c r="F120" s="37"/>
+      <c r="G120" s="40"/>
+      <c r="H120" s="40"/>
+      <c r="I120" s="40"/>
+      <c r="J120" s="40">
+        <f>SUM(J9:J118)</f>
+        <v>356103.37598483142</v>
+      </c>
+      <c r="K120" s="35"/>
+    </row>
+    <row r="121" spans="1:11">
+      <c r="A121" s="54"/>
+      <c r="B121" s="57"/>
+      <c r="C121" s="58"/>
+      <c r="D121" s="55"/>
+      <c r="E121" s="55"/>
+      <c r="F121" s="55"/>
+      <c r="G121" s="56"/>
+      <c r="H121" s="56"/>
+      <c r="I121" s="56"/>
+      <c r="J121" s="56"/>
+      <c r="K121" s="53"/>
+    </row>
+    <row r="122" spans="1:11" s="1" customFormat="1">
+      <c r="A122" s="46"/>
+      <c r="B122" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C109" s="147">
-        <f>J107</f>
-        <v>336917.6969730733</v>
-      </c>
-      <c r="D109" s="147"/>
-      <c r="E109" s="38">
+      <c r="C122" s="152">
+        <f>J120</f>
+        <v>356103.37598483142</v>
+      </c>
+      <c r="D122" s="152"/>
+      <c r="E122" s="38">
         <v>100</v>
       </c>
-      <c r="F109" s="47"/>
-      <c r="G109" s="48"/>
-      <c r="H109" s="47"/>
-      <c r="I109" s="49"/>
-      <c r="J109" s="50"/>
-      <c r="K109" s="51"/>
-    </row>
-    <row r="110" spans="1:11">
-      <c r="A110" s="52"/>
-      <c r="B110" s="28" t="s">
+      <c r="F122" s="47"/>
+      <c r="G122" s="48"/>
+      <c r="H122" s="47"/>
+      <c r="I122" s="49"/>
+      <c r="J122" s="50"/>
+      <c r="K122" s="51"/>
+    </row>
+    <row r="123" spans="1:11">
+      <c r="A123" s="52"/>
+      <c r="B123" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C110" s="150">
-        <v>300000</v>
-      </c>
-      <c r="D110" s="150"/>
-      <c r="E110" s="38"/>
-      <c r="F110" s="45"/>
-      <c r="G110" s="44"/>
-      <c r="H110" s="44"/>
-      <c r="I110" s="44"/>
-      <c r="J110" s="44"/>
-      <c r="K110" s="45"/>
-    </row>
-    <row r="111" spans="1:11">
-      <c r="A111" s="52"/>
-      <c r="B111" s="28" t="s">
+      <c r="C123" s="153">
+        <v>500000</v>
+      </c>
+      <c r="D123" s="153"/>
+      <c r="E123" s="38"/>
+      <c r="F123" s="45"/>
+      <c r="G123" s="44"/>
+      <c r="H123" s="44"/>
+      <c r="I123" s="44"/>
+      <c r="J123" s="44"/>
+      <c r="K123" s="45"/>
+    </row>
+    <row r="124" spans="1:11">
+      <c r="A124" s="52"/>
+      <c r="B124" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C111" s="150">
-        <f>C110-C113-C114</f>
-        <v>285000</v>
-      </c>
-      <c r="D111" s="150"/>
-      <c r="E111" s="38">
-        <f>C111/C109*100</f>
-        <v>84.590391825804687</v>
-      </c>
-      <c r="F111" s="45"/>
-      <c r="G111" s="44"/>
-      <c r="H111" s="44"/>
-      <c r="I111" s="44"/>
-      <c r="J111" s="44"/>
-      <c r="K111" s="45"/>
-    </row>
-    <row r="112" spans="1:11">
-      <c r="A112" s="52"/>
-      <c r="B112" s="28" t="s">
+      <c r="C124" s="153">
+        <f>C123-C126-C127</f>
+        <v>475000</v>
+      </c>
+      <c r="D124" s="153"/>
+      <c r="E124" s="38">
+        <f>C124/C122*100</f>
+        <v>133.38823275301752</v>
+      </c>
+      <c r="F124" s="45"/>
+      <c r="G124" s="44"/>
+      <c r="H124" s="44"/>
+      <c r="I124" s="44"/>
+      <c r="J124" s="44"/>
+      <c r="K124" s="45"/>
+    </row>
+    <row r="125" spans="1:11">
+      <c r="A125" s="52"/>
+      <c r="B125" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C112" s="147">
-        <f>C109-C111</f>
-        <v>51917.696973073296</v>
-      </c>
-      <c r="D112" s="147"/>
-      <c r="E112" s="38">
-        <f>100-E111</f>
-        <v>15.409608174195313</v>
-      </c>
-      <c r="F112" s="45"/>
-      <c r="G112" s="44"/>
-      <c r="H112" s="44"/>
-      <c r="I112" s="44"/>
-      <c r="J112" s="44"/>
-      <c r="K112" s="45"/>
-    </row>
-    <row r="113" spans="1:11">
-      <c r="A113" s="52"/>
-      <c r="B113" s="28" t="s">
+      <c r="C125" s="152">
+        <f>C122-C124</f>
+        <v>-118896.62401516858</v>
+      </c>
+      <c r="D125" s="152"/>
+      <c r="E125" s="38">
+        <f>100-E124</f>
+        <v>-33.388232753017519</v>
+      </c>
+      <c r="F125" s="45"/>
+      <c r="G125" s="44"/>
+      <c r="H125" s="44"/>
+      <c r="I125" s="44"/>
+      <c r="J125" s="44"/>
+      <c r="K125" s="45"/>
+    </row>
+    <row r="126" spans="1:11">
+      <c r="A126" s="52"/>
+      <c r="B126" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C113" s="147">
-        <f>C110*0.03</f>
-        <v>9000</v>
-      </c>
-      <c r="D113" s="147"/>
-      <c r="E113" s="38">
+      <c r="C126" s="152">
+        <f>C123*0.03</f>
+        <v>15000</v>
+      </c>
+      <c r="D126" s="152"/>
+      <c r="E126" s="38">
         <v>3</v>
       </c>
-      <c r="F113" s="45"/>
-      <c r="G113" s="44"/>
-      <c r="H113" s="44"/>
-      <c r="I113" s="44"/>
-      <c r="J113" s="44"/>
-      <c r="K113" s="45"/>
-    </row>
-    <row r="114" spans="1:11">
-      <c r="A114" s="52"/>
-      <c r="B114" s="28" t="s">
+      <c r="F126" s="45"/>
+      <c r="G126" s="44"/>
+      <c r="H126" s="44"/>
+      <c r="I126" s="44"/>
+      <c r="J126" s="44"/>
+      <c r="K126" s="45"/>
+    </row>
+    <row r="127" spans="1:11">
+      <c r="A127" s="52"/>
+      <c r="B127" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C114" s="147">
-        <f>C110*0.02</f>
-        <v>6000</v>
-      </c>
-      <c r="D114" s="147"/>
-      <c r="E114" s="38">
+      <c r="C127" s="152">
+        <f>C123*0.02</f>
+        <v>10000</v>
+      </c>
+      <c r="D127" s="152"/>
+      <c r="E127" s="38">
         <v>2</v>
       </c>
-      <c r="F114" s="45"/>
-      <c r="G114" s="44"/>
-      <c r="H114" s="44"/>
-      <c r="I114" s="44"/>
-      <c r="J114" s="44"/>
-      <c r="K114" s="45"/>
-    </row>
-    <row r="115" spans="1:11" s="34" customFormat="1">
-      <c r="A115" s="53"/>
-      <c r="B115" s="53"/>
-      <c r="C115" s="53"/>
-      <c r="D115" s="53"/>
-      <c r="E115" s="53"/>
-      <c r="F115" s="53"/>
-      <c r="G115" s="53"/>
-      <c r="H115" s="53"/>
-      <c r="I115" s="53"/>
-      <c r="J115" s="53"/>
-      <c r="K115" s="53"/>
-    </row>
-    <row r="116" spans="1:11" s="34" customFormat="1"/>
-    <row r="117" spans="1:11" s="34" customFormat="1"/>
-    <row r="118" spans="1:11" s="34" customFormat="1"/>
-    <row r="119" spans="1:11" s="34" customFormat="1"/>
-    <row r="120" spans="1:11" s="34" customFormat="1"/>
-    <row r="121" spans="1:11" s="34" customFormat="1"/>
-    <row r="122" spans="1:11" s="34" customFormat="1"/>
-    <row r="123" spans="1:11" s="34" customFormat="1"/>
-    <row r="124" spans="1:11" s="34" customFormat="1"/>
-    <row r="125" spans="1:11" s="34" customFormat="1"/>
-    <row r="126" spans="1:11" s="34" customFormat="1"/>
-    <row r="127" spans="1:11" s="34" customFormat="1"/>
-    <row r="128" spans="1:11" s="34" customFormat="1"/>
+      <c r="F127" s="45"/>
+      <c r="G127" s="44"/>
+      <c r="H127" s="44"/>
+      <c r="I127" s="44"/>
+      <c r="J127" s="44"/>
+      <c r="K127" s="45"/>
+    </row>
+    <row r="128" spans="1:11" s="34" customFormat="1">
+      <c r="A128" s="53"/>
+      <c r="B128" s="53"/>
+      <c r="C128" s="53"/>
+      <c r="D128" s="53"/>
+      <c r="E128" s="53"/>
+      <c r="F128" s="53"/>
+      <c r="G128" s="53"/>
+      <c r="H128" s="53"/>
+      <c r="I128" s="53"/>
+      <c r="J128" s="53"/>
+      <c r="K128" s="53"/>
+    </row>
     <row r="129" s="34" customFormat="1"/>
     <row r="130" s="34" customFormat="1"/>
     <row r="131" s="34" customFormat="1"/>
@@ -8758,19 +9106,34 @@
     <row r="169" s="34" customFormat="1"/>
     <row r="170" s="34" customFormat="1"/>
     <row r="171" s="34" customFormat="1"/>
+    <row r="172" s="34" customFormat="1"/>
+    <row r="173" s="34" customFormat="1"/>
+    <row r="174" s="34" customFormat="1"/>
+    <row r="175" s="34" customFormat="1"/>
+    <row r="176" s="34" customFormat="1"/>
+    <row r="177" s="34" customFormat="1"/>
+    <row r="178" s="34" customFormat="1"/>
+    <row r="179" s="34" customFormat="1"/>
+    <row r="180" s="34" customFormat="1"/>
+    <row r="181" s="34" customFormat="1"/>
+    <row r="182" s="34" customFormat="1"/>
+    <row r="183" s="34" customFormat="1"/>
+    <row r="184" s="34" customFormat="1"/>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C114:D114"/>
+  <mergeCells count="20">
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="N107:T107"/>
+    <mergeCell ref="N108:T108"/>
     <mergeCell ref="A7:F7"/>
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="N41:T41"/>
     <mergeCell ref="N54:T54"/>
     <mergeCell ref="N62:T62"/>
-    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C122:D122"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>

</xml_diff>

<commit_message>
some traces added for new tahara and paropakar estimate given
</commit_message>
<xml_diff>
--- a/ofc/estimates/परोपकार भवन मर्मत/परोपकार भवन मर्मत.xlsx
+++ b/ofc/estimates/परोपकार भवन मर्मत/परोपकार भवन मर्मत.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\परोपकार भवन मर्मत\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\081-082\ofc\estimates\परोपकार भवन मर्मत\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="WCR" sheetId="6" r:id="rId1"/>
@@ -132,7 +132,7 @@
     <definedName name="Ttile">'[1]update Rate'!$N$43</definedName>
     <definedName name="unskilled">'[2]Material rate'!$D$154</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="163">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -794,15 +794,18 @@
   <si>
     <t>-at compound</t>
   </si>
+  <si>
+    <t>Date:2081/10/13</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1132,10 +1135,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="185">
+  <cellXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1143,7 +1146,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1163,14 +1166,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1179,7 +1182,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1203,7 +1206,7 @@
     <xf numFmtId="1" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1241,7 +1244,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1256,7 +1259,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1272,7 +1275,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1314,7 +1317,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="24" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
@@ -1352,7 +1355,7 @@
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1442,7 +1445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1472,7 +1475,7 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1480,7 +1483,7 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1495,6 +1498,24 @@
     </xf>
     <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1520,37 +1541,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1563,11 +1553,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1590,20 +1605,11 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2602,106 +2608,106 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="150" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="158"/>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="158"/>
-      <c r="G1" s="158"/>
-      <c r="H1" s="158"/>
-      <c r="I1" s="158"/>
-      <c r="J1" s="158"/>
-      <c r="K1" s="158"/>
-    </row>
-    <row r="2" spans="1:11" ht="24.6">
-      <c r="A2" s="159" t="s">
+      <c r="B1" s="150"/>
+      <c r="C1" s="150"/>
+      <c r="D1" s="150"/>
+      <c r="E1" s="150"/>
+      <c r="F1" s="150"/>
+      <c r="G1" s="150"/>
+      <c r="H1" s="150"/>
+      <c r="I1" s="150"/>
+      <c r="J1" s="150"/>
+      <c r="K1" s="150"/>
+    </row>
+    <row r="2" spans="1:11" ht="25.5">
+      <c r="A2" s="151" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="159"/>
-      <c r="C2" s="159"/>
-      <c r="D2" s="159"/>
-      <c r="E2" s="159"/>
-      <c r="F2" s="159"/>
-      <c r="G2" s="159"/>
-      <c r="H2" s="159"/>
-      <c r="I2" s="159"/>
-      <c r="J2" s="159"/>
-      <c r="K2" s="159"/>
+      <c r="B2" s="151"/>
+      <c r="C2" s="151"/>
+      <c r="D2" s="151"/>
+      <c r="E2" s="151"/>
+      <c r="F2" s="151"/>
+      <c r="G2" s="151"/>
+      <c r="H2" s="151"/>
+      <c r="I2" s="151"/>
+      <c r="J2" s="151"/>
+      <c r="K2" s="151"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="152" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="160"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160"/>
+      <c r="B3" s="152"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="152"/>
+      <c r="G3" s="152"/>
+      <c r="H3" s="152"/>
+      <c r="I3" s="152"/>
+      <c r="J3" s="152"/>
+      <c r="K3" s="152"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1">
-      <c r="A4" s="160" t="s">
+      <c r="A4" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="160"/>
-      <c r="C4" s="160"/>
-      <c r="D4" s="160"/>
-      <c r="E4" s="160"/>
-      <c r="F4" s="160"/>
-      <c r="G4" s="160"/>
-      <c r="H4" s="160"/>
-      <c r="I4" s="160"/>
-      <c r="J4" s="160"/>
-      <c r="K4" s="160"/>
-    </row>
-    <row r="5" spans="1:11" ht="18">
-      <c r="A5" s="161" t="s">
+      <c r="B4" s="152"/>
+      <c r="C4" s="152"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="152"/>
+      <c r="F4" s="152"/>
+      <c r="G4" s="152"/>
+      <c r="H4" s="152"/>
+      <c r="I4" s="152"/>
+      <c r="J4" s="152"/>
+      <c r="K4" s="152"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75">
+      <c r="A5" s="153" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="161"/>
-      <c r="C5" s="161"/>
-      <c r="D5" s="161"/>
-      <c r="E5" s="161"/>
-      <c r="F5" s="161"/>
-      <c r="G5" s="161"/>
-      <c r="H5" s="161"/>
-      <c r="I5" s="161"/>
-      <c r="J5" s="161"/>
-      <c r="K5" s="161"/>
-    </row>
-    <row r="6" spans="1:11" ht="18">
+      <c r="B5" s="153"/>
+      <c r="C5" s="153"/>
+      <c r="D5" s="153"/>
+      <c r="E5" s="153"/>
+      <c r="F5" s="153"/>
+      <c r="G5" s="153"/>
+      <c r="H5" s="153"/>
+      <c r="I5" s="153"/>
+      <c r="J5" s="153"/>
+      <c r="K5" s="153"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="156" t="e">
+      <c r="C6" s="148" t="e">
         <f>F18</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="157"/>
+      <c r="D6" s="149"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -2709,11 +2715,11 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="156" t="e">
+      <c r="J6" s="148" t="e">
         <f>I18</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="157"/>
+      <c r="K6" s="149"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="25" t="s">
@@ -2722,77 +2728,77 @@
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="151"/>
-      <c r="G7" s="151"/>
-      <c r="I7" s="152" t="s">
+      <c r="F7" s="157"/>
+      <c r="G7" s="157"/>
+      <c r="I7" s="158" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="152"/>
-      <c r="K7" s="152"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.6">
-      <c r="A8" s="150" t="e">
+      <c r="J7" s="158"/>
+      <c r="K7" s="158"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75">
+      <c r="A8" s="156" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="150"/>
-      <c r="C8" s="150"/>
-      <c r="D8" s="150"/>
-      <c r="E8" s="150"/>
-      <c r="F8" s="150"/>
-      <c r="I8" s="153" t="s">
+      <c r="B8" s="156"/>
+      <c r="C8" s="156"/>
+      <c r="D8" s="156"/>
+      <c r="E8" s="156"/>
+      <c r="F8" s="156"/>
+      <c r="I8" s="159" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="153"/>
-      <c r="K8" s="153"/>
+      <c r="J8" s="159"/>
+      <c r="K8" s="159"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="154" t="e">
+      <c r="A9" s="160" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="154"/>
-      <c r="C9" s="154"/>
-      <c r="D9" s="154"/>
-      <c r="E9" s="154"/>
-      <c r="F9" s="154"/>
-      <c r="I9" s="153" t="s">
+      <c r="B9" s="160"/>
+      <c r="C9" s="160"/>
+      <c r="D9" s="160"/>
+      <c r="E9" s="160"/>
+      <c r="F9" s="160"/>
+      <c r="I9" s="159" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="153"/>
-      <c r="K9" s="153"/>
+      <c r="J9" s="159"/>
+      <c r="K9" s="159"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="148" t="s">
+      <c r="A11" s="154" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="148" t="s">
+      <c r="B11" s="154" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="148" t="s">
+      <c r="C11" s="154" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="155" t="s">
+      <c r="D11" s="161" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="155"/>
-      <c r="F11" s="155"/>
-      <c r="G11" s="155" t="s">
+      <c r="E11" s="161"/>
+      <c r="F11" s="161"/>
+      <c r="G11" s="161" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="155"/>
-      <c r="I11" s="155"/>
-      <c r="J11" s="148" t="s">
+      <c r="H11" s="161"/>
+      <c r="I11" s="161"/>
+      <c r="J11" s="154" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="149" t="s">
+      <c r="K11" s="155" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="148"/>
-      <c r="B12" s="148"/>
-      <c r="C12" s="148"/>
+      <c r="A12" s="154"/>
+      <c r="B12" s="154"/>
+      <c r="C12" s="154"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -2811,10 +2817,10 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="148"/>
-      <c r="K12" s="149"/>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="15.6">
+      <c r="J12" s="154"/>
+      <c r="K12" s="155"/>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A13" s="26" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -2857,7 +2863,7 @@
       </c>
       <c r="K13" s="14"/>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A14" s="26"/>
       <c r="B14" s="32" t="e">
         <f>#REF!</f>
@@ -2974,13 +2980,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -2994,6 +2993,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3015,128 +3021,128 @@
       <selection activeCell="D17" sqref="D17:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
-      <c r="A1" s="168" t="s">
+      <c r="A1" s="163" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="168"/>
-      <c r="C1" s="168"/>
-      <c r="D1" s="168"/>
-      <c r="E1" s="168"/>
-      <c r="F1" s="168"/>
-      <c r="G1" s="168"/>
-      <c r="H1" s="168"/>
-      <c r="I1" s="168"/>
-      <c r="J1" s="168"/>
-      <c r="K1" s="168"/>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="22.8">
-      <c r="A2" s="169" t="s">
+      <c r="B1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="163"/>
+      <c r="H1" s="163"/>
+      <c r="I1" s="163"/>
+      <c r="J1" s="163"/>
+      <c r="K1" s="163"/>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="22.5">
+      <c r="A2" s="164" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="169"/>
-      <c r="I2" s="169"/>
-      <c r="J2" s="169"/>
-      <c r="K2" s="169"/>
+      <c r="B2" s="164"/>
+      <c r="C2" s="164"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="164"/>
+      <c r="F2" s="164"/>
+      <c r="G2" s="164"/>
+      <c r="H2" s="164"/>
+      <c r="I2" s="164"/>
+      <c r="J2" s="164"/>
+      <c r="K2" s="164"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="152" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="160"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160"/>
+      <c r="B3" s="152"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="152"/>
+      <c r="G3" s="152"/>
+      <c r="H3" s="152"/>
+      <c r="I3" s="152"/>
+      <c r="J3" s="152"/>
+      <c r="K3" s="152"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1">
-      <c r="A4" s="160" t="s">
+      <c r="A4" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="160"/>
-      <c r="C4" s="160"/>
-      <c r="D4" s="160"/>
-      <c r="E4" s="160"/>
-      <c r="F4" s="160"/>
-      <c r="G4" s="160"/>
-      <c r="H4" s="160"/>
-      <c r="I4" s="160"/>
-      <c r="J4" s="160"/>
-      <c r="K4" s="160"/>
-    </row>
-    <row r="5" spans="1:14" ht="17.399999999999999">
-      <c r="A5" s="170" t="s">
+      <c r="B4" s="152"/>
+      <c r="C4" s="152"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="152"/>
+      <c r="F4" s="152"/>
+      <c r="G4" s="152"/>
+      <c r="H4" s="152"/>
+      <c r="I4" s="152"/>
+      <c r="J4" s="152"/>
+      <c r="K4" s="152"/>
+    </row>
+    <row r="5" spans="1:14" ht="18.75">
+      <c r="A5" s="165" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="170"/>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="170"/>
-      <c r="H5" s="170"/>
-      <c r="I5" s="170"/>
-      <c r="J5" s="170"/>
-      <c r="K5" s="170"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.6">
-      <c r="A6" s="150" t="s">
+      <c r="B5" s="165"/>
+      <c r="C5" s="165"/>
+      <c r="D5" s="165"/>
+      <c r="E5" s="165"/>
+      <c r="F5" s="165"/>
+      <c r="G5" s="165"/>
+      <c r="H5" s="165"/>
+      <c r="I5" s="165"/>
+      <c r="J5" s="165"/>
+      <c r="K5" s="165"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.75">
+      <c r="A6" s="156" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="150"/>
-      <c r="C6" s="150"/>
-      <c r="D6" s="150"/>
-      <c r="E6" s="150"/>
-      <c r="F6" s="150"/>
+      <c r="B6" s="156"/>
+      <c r="C6" s="156"/>
+      <c r="D6" s="156"/>
+      <c r="E6" s="156"/>
+      <c r="F6" s="156"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="167" t="s">
+      <c r="H6" s="162" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="167"/>
-      <c r="J6" s="167"/>
-      <c r="K6" s="167"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.6">
-      <c r="A7" s="164" t="s">
+      <c r="I6" s="162"/>
+      <c r="J6" s="162"/>
+      <c r="K6" s="162"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75">
+      <c r="A7" s="166" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="164"/>
-      <c r="C7" s="164"/>
-      <c r="D7" s="164"/>
-      <c r="E7" s="164"/>
-      <c r="F7" s="164"/>
+      <c r="B7" s="166"/>
+      <c r="C7" s="166"/>
+      <c r="D7" s="166"/>
+      <c r="E7" s="166"/>
+      <c r="F7" s="166"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="165" t="s">
+      <c r="H7" s="167" t="s">
         <v>141</v>
       </c>
-      <c r="I7" s="165"/>
-      <c r="J7" s="165"/>
-      <c r="K7" s="165"/>
+      <c r="I7" s="167"/>
+      <c r="J7" s="167"/>
+      <c r="K7" s="167"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1">
       <c r="A8" s="4" t="s">
@@ -3173,7 +3179,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="1" customFormat="1" ht="55.2">
+    <row r="9" spans="1:14" s="1" customFormat="1" ht="57">
       <c r="A9" s="59">
         <v>1</v>
       </c>
@@ -3328,7 +3334,7 @@
       <c r="J15" s="41"/>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="1:14" ht="27.6">
+    <row r="16" spans="1:14" ht="28.5">
       <c r="A16" s="18">
         <v>2</v>
       </c>
@@ -3431,7 +3437,7 @@
       <c r="J20" s="41"/>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="1:19" ht="41.4">
+    <row r="21" spans="1:19" ht="42.75">
       <c r="A21" s="18">
         <v>3</v>
       </c>
@@ -3535,7 +3541,7 @@
       <c r="J25" s="41"/>
       <c r="K25" s="21"/>
     </row>
-    <row r="26" spans="1:19" ht="30.6">
+    <row r="26" spans="1:19" ht="30.75">
       <c r="A26" s="18">
         <v>4</v>
       </c>
@@ -3624,7 +3630,7 @@
       <c r="J29" s="40"/>
       <c r="K29" s="21"/>
     </row>
-    <row r="30" spans="1:19" ht="15">
+    <row r="30" spans="1:19">
       <c r="A30" s="18">
         <v>5</v>
       </c>
@@ -3815,7 +3821,7 @@
       </c>
       <c r="K38" s="21"/>
     </row>
-    <row r="39" spans="1:20" ht="15">
+    <row r="39" spans="1:20">
       <c r="A39" s="18"/>
       <c r="B39" s="89"/>
       <c r="C39" s="19"/>
@@ -3828,7 +3834,7 @@
       <c r="J39" s="40"/>
       <c r="K39" s="21"/>
     </row>
-    <row r="40" spans="1:20" ht="39">
+    <row r="40" spans="1:20" ht="39.75">
       <c r="A40" s="18">
         <v>7</v>
       </c>
@@ -3880,15 +3886,15 @@
       <c r="I41" s="39"/>
       <c r="J41" s="39"/>
       <c r="K41" s="61"/>
-      <c r="N41" s="162" t="s">
+      <c r="N41" s="170" t="s">
         <v>87</v>
       </c>
-      <c r="O41" s="162"/>
-      <c r="P41" s="162"/>
-      <c r="Q41" s="162"/>
-      <c r="R41" s="162"/>
-      <c r="S41" s="162"/>
-      <c r="T41" s="162"/>
+      <c r="O41" s="170"/>
+      <c r="P41" s="170"/>
+      <c r="Q41" s="170"/>
+      <c r="R41" s="170"/>
+      <c r="S41" s="170"/>
+      <c r="T41" s="170"/>
     </row>
     <row r="42" spans="1:20" ht="15" customHeight="1">
       <c r="A42" s="18"/>
@@ -4185,15 +4191,15 @@
       <c r="I54" s="39"/>
       <c r="J54" s="39"/>
       <c r="K54" s="61"/>
-      <c r="N54" s="162" t="s">
+      <c r="N54" s="170" t="s">
         <v>87</v>
       </c>
-      <c r="O54" s="162"/>
-      <c r="P54" s="162"/>
-      <c r="Q54" s="162"/>
-      <c r="R54" s="162"/>
-      <c r="S54" s="162"/>
-      <c r="T54" s="162"/>
+      <c r="O54" s="170"/>
+      <c r="P54" s="170"/>
+      <c r="Q54" s="170"/>
+      <c r="R54" s="170"/>
+      <c r="S54" s="170"/>
+      <c r="T54" s="170"/>
     </row>
     <row r="55" spans="1:20" ht="15" customHeight="1">
       <c r="A55" s="18"/>
@@ -4389,15 +4395,15 @@
       <c r="I62" s="39"/>
       <c r="J62" s="39"/>
       <c r="K62" s="61"/>
-      <c r="N62" s="162" t="s">
+      <c r="N62" s="170" t="s">
         <v>87</v>
       </c>
-      <c r="O62" s="162"/>
-      <c r="P62" s="162"/>
-      <c r="Q62" s="162"/>
-      <c r="R62" s="162"/>
-      <c r="S62" s="162"/>
-      <c r="T62" s="162"/>
+      <c r="O62" s="170"/>
+      <c r="P62" s="170"/>
+      <c r="Q62" s="170"/>
+      <c r="R62" s="170"/>
+      <c r="S62" s="170"/>
+      <c r="T62" s="170"/>
     </row>
     <row r="63" spans="1:20" ht="15" customHeight="1">
       <c r="A63" s="18"/>
@@ -4488,7 +4494,7 @@
       <c r="J66" s="41"/>
       <c r="K66" s="21"/>
     </row>
-    <row r="67" spans="1:13" ht="30.6">
+    <row r="67" spans="1:13" ht="30.75">
       <c r="A67" s="18">
         <v>11</v>
       </c>
@@ -4598,7 +4604,7 @@
       <c r="J70" s="125"/>
       <c r="K70" s="123"/>
     </row>
-    <row r="71" spans="1:13" s="1" customFormat="1" ht="27.6">
+    <row r="71" spans="1:13" s="1" customFormat="1" ht="30">
       <c r="A71" s="122"/>
       <c r="B71" s="127" t="s">
         <v>125</v>
@@ -4627,7 +4633,7 @@
       <c r="K71" s="123"/>
       <c r="M71" s="129"/>
     </row>
-    <row r="72" spans="1:13" s="1" customFormat="1" ht="41.4">
+    <row r="72" spans="1:13" s="1" customFormat="1" ht="45">
       <c r="A72" s="122"/>
       <c r="B72" s="127" t="s">
         <v>126</v>
@@ -4683,7 +4689,7 @@
       <c r="K73" s="123"/>
       <c r="M73" s="129"/>
     </row>
-    <row r="74" spans="1:13" s="1" customFormat="1" ht="27.6">
+    <row r="74" spans="1:13" s="1" customFormat="1" ht="30">
       <c r="A74" s="122"/>
       <c r="B74" s="127" t="s">
         <v>133</v>
@@ -5112,7 +5118,7 @@
       <c r="J92" s="125"/>
       <c r="K92" s="21"/>
     </row>
-    <row r="93" spans="1:11" ht="30.6">
+    <row r="93" spans="1:11" ht="30.75">
       <c r="A93" s="18">
         <v>13</v>
       </c>
@@ -5424,11 +5430,11 @@
       <c r="B109" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C109" s="163">
+      <c r="C109" s="168">
         <f>J107</f>
         <v>336917.6969730733</v>
       </c>
-      <c r="D109" s="163"/>
+      <c r="D109" s="168"/>
       <c r="E109" s="38">
         <v>100</v>
       </c>
@@ -5444,10 +5450,10 @@
       <c r="B110" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C110" s="166">
+      <c r="C110" s="169">
         <v>300000</v>
       </c>
-      <c r="D110" s="166"/>
+      <c r="D110" s="169"/>
       <c r="E110" s="38"/>
       <c r="F110" s="45"/>
       <c r="G110" s="44"/>
@@ -5461,11 +5467,11 @@
       <c r="B111" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C111" s="166">
+      <c r="C111" s="169">
         <f>C110-C113-C114</f>
         <v>285000</v>
       </c>
-      <c r="D111" s="166"/>
+      <c r="D111" s="169"/>
       <c r="E111" s="38">
         <f>C111/C109*100</f>
         <v>84.590391825804687</v>
@@ -5482,11 +5488,11 @@
       <c r="B112" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C112" s="163">
+      <c r="C112" s="168">
         <f>C109-C111</f>
         <v>51917.696973073296</v>
       </c>
-      <c r="D112" s="163"/>
+      <c r="D112" s="168"/>
       <c r="E112" s="38">
         <f>100-E111</f>
         <v>15.409608174195313</v>
@@ -5503,11 +5509,11 @@
       <c r="B113" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C113" s="163">
+      <c r="C113" s="168">
         <f>C110*0.03</f>
         <v>9000</v>
       </c>
-      <c r="D113" s="163"/>
+      <c r="D113" s="168"/>
       <c r="E113" s="38">
         <v>3</v>
       </c>
@@ -5523,11 +5529,11 @@
       <c r="B114" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C114" s="163">
+      <c r="C114" s="168">
         <f>C110*0.02</f>
         <v>6000</v>
       </c>
-      <c r="D114" s="163"/>
+      <c r="D114" s="168"/>
       <c r="E114" s="38">
         <v>2</v>
       </c>
@@ -5609,6 +5615,17 @@
     <row r="171" s="34" customFormat="1"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="N41:T41"/>
+    <mergeCell ref="N54:T54"/>
+    <mergeCell ref="N62:T62"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C111:D111"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
@@ -5616,17 +5633,6 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="N41:T41"/>
-    <mergeCell ref="N54:T54"/>
-    <mergeCell ref="N62:T62"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="C112:D112"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B80" r:id="rId1"/>
@@ -5648,21 +5654,21 @@
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="64"/>
-    <col min="2" max="2" width="11.44140625" style="64" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" style="64" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="64"/>
-    <col min="6" max="6" width="10.44140625" style="64" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" style="64" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" style="64" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="64"/>
+    <col min="1" max="1" width="8.85546875" style="64"/>
+    <col min="2" max="2" width="11.42578125" style="64" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="64" customWidth="1"/>
+    <col min="4" max="5" width="8.85546875" style="64"/>
+    <col min="6" max="6" width="10.42578125" style="64" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="64" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="64" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="64"/>
     <col min="10" max="10" width="12" style="64" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="64"/>
+    <col min="11" max="16384" width="8.85546875" style="64"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21">
+    <row r="1" spans="1:10" ht="20.25">
       <c r="A1" s="62" t="e">
         <f>+#REF!+1</f>
         <v>#REF!</v>
@@ -5687,33 +5693,33 @@
       <c r="G2" s="66"/>
       <c r="H2" s="66"/>
     </row>
-    <row r="3" spans="1:10" ht="17.399999999999999">
+    <row r="3" spans="1:10" ht="18">
       <c r="A3" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="180" t="s">
+      <c r="B3" s="171" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="180"/>
-      <c r="D3" s="180"/>
-      <c r="E3" s="180"/>
-      <c r="F3" s="180"/>
-      <c r="G3" s="180"/>
-      <c r="H3" s="180"/>
-    </row>
-    <row r="4" spans="1:10" ht="15">
+      <c r="C3" s="171"/>
+      <c r="D3" s="171"/>
+      <c r="E3" s="171"/>
+      <c r="F3" s="171"/>
+      <c r="G3" s="171"/>
+      <c r="H3" s="171"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75">
       <c r="A4" s="68"/>
-      <c r="B4" s="181" t="s">
+      <c r="B4" s="172" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="181"/>
-      <c r="D4" s="181"/>
-      <c r="E4" s="181"/>
-      <c r="F4" s="181"/>
-      <c r="G4" s="181"/>
-      <c r="H4" s="181"/>
-    </row>
-    <row r="5" spans="1:10" ht="32.4">
+      <c r="C4" s="172"/>
+      <c r="D4" s="172"/>
+      <c r="E4" s="172"/>
+      <c r="F4" s="172"/>
+      <c r="G4" s="172"/>
+      <c r="H4" s="172"/>
+    </row>
+    <row r="5" spans="1:10" ht="31.5">
       <c r="A5" s="68"/>
       <c r="B5" s="69" t="s">
         <v>52</v>
@@ -5737,9 +5743,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18">
+    <row r="6" spans="1:10" ht="17.25">
       <c r="A6" s="68"/>
-      <c r="B6" s="182" t="s">
+      <c r="B6" s="173" t="s">
         <v>59</v>
       </c>
       <c r="C6" s="69" t="s">
@@ -5760,9 +5766,9 @@
       </c>
       <c r="H6" s="74"/>
     </row>
-    <row r="7" spans="1:10" ht="18">
+    <row r="7" spans="1:10" ht="17.25">
       <c r="A7" s="68"/>
-      <c r="B7" s="183"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="71" t="s">
         <v>62</v>
       </c>
@@ -5784,9 +5790,9 @@
         <v>3065</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="43.8">
+    <row r="8" spans="1:10" ht="45">
       <c r="A8" s="68"/>
-      <c r="B8" s="182" t="s">
+      <c r="B8" s="173" t="s">
         <v>63</v>
       </c>
       <c r="C8" s="75" t="s">
@@ -5807,9 +5813,9 @@
       </c>
       <c r="H8" s="74"/>
     </row>
-    <row r="9" spans="1:10" ht="18">
+    <row r="9" spans="1:10" ht="17.25">
       <c r="A9" s="68"/>
-      <c r="B9" s="182"/>
+      <c r="B9" s="173"/>
       <c r="C9" s="71" t="s">
         <v>66</v>
       </c>
@@ -5828,9 +5834,9 @@
       </c>
       <c r="H9" s="77"/>
     </row>
-    <row r="10" spans="1:10" ht="18">
+    <row r="10" spans="1:10" ht="17.25">
       <c r="A10" s="68"/>
-      <c r="B10" s="182"/>
+      <c r="B10" s="173"/>
       <c r="C10" s="71" t="s">
         <v>68</v>
       </c>
@@ -5853,9 +5859,9 @@
         <v>99000</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="18">
+    <row r="11" spans="1:10" ht="17.25">
       <c r="A11" s="68"/>
-      <c r="B11" s="182"/>
+      <c r="B11" s="173"/>
       <c r="C11" s="71" t="s">
         <v>70</v>
       </c>
@@ -5875,9 +5881,9 @@
       </c>
       <c r="H11" s="77"/>
     </row>
-    <row r="12" spans="1:10" ht="18">
+    <row r="12" spans="1:10" ht="17.25">
       <c r="A12" s="68"/>
-      <c r="B12" s="182"/>
+      <c r="B12" s="173"/>
       <c r="C12" s="71" t="s">
         <v>71</v>
       </c>
@@ -5901,9 +5907,9 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="18">
+    <row r="13" spans="1:10" ht="17.25">
       <c r="A13" s="68"/>
-      <c r="B13" s="182"/>
+      <c r="B13" s="173"/>
       <c r="C13" s="71" t="s">
         <v>73</v>
       </c>
@@ -5926,7 +5932,7 @@
         <v>5504.3</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="18">
+    <row r="14" spans="1:10" ht="17.25">
       <c r="A14" s="68"/>
       <c r="B14" s="68"/>
       <c r="C14" s="68"/>
@@ -5941,7 +5947,7 @@
         <v>8569.2999999999993</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="18">
+    <row r="15" spans="1:10" ht="17.25">
       <c r="B15" s="83" t="s">
         <v>76</v>
       </c>
@@ -5955,7 +5961,7 @@
         <v>1285.3900000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="18">
+    <row r="16" spans="1:10" ht="17.25">
       <c r="A16" s="84" t="s">
         <v>78</v>
       </c>
@@ -5977,7 +5983,7 @@
         <v>9854.6899999999987</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="18">
+    <row r="17" spans="1:8" ht="17.25">
       <c r="A17" s="84"/>
       <c r="B17" s="85"/>
       <c r="C17" s="68"/>
@@ -5992,7 +5998,7 @@
         <v>1094.9655555555555</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18">
+    <row r="18" spans="1:8" ht="17.25">
       <c r="A18" s="84"/>
       <c r="B18" s="85"/>
       <c r="C18" s="68"/>
@@ -6007,7 +6013,7 @@
         <v>952.14396135265702</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="18">
+    <row r="19" spans="1:8" ht="17.25">
       <c r="A19" s="84"/>
       <c r="B19" s="86" t="s">
         <v>83</v>
@@ -6019,43 +6025,43 @@
       <c r="G19" s="81"/>
       <c r="H19" s="85"/>
     </row>
-    <row r="22" spans="1:8" s="94" customFormat="1" ht="21">
+    <row r="22" spans="1:8" s="94" customFormat="1" ht="20.25">
       <c r="A22" s="93">
         <f>+A9+1</f>
         <v>1</v>
       </c>
-      <c r="B22" s="172"/>
-      <c r="C22" s="172"/>
-      <c r="D22" s="172"/>
-      <c r="E22" s="172"/>
-      <c r="F22" s="172"/>
-      <c r="G22" s="172"/>
-      <c r="H22" s="172"/>
-    </row>
-    <row r="23" spans="1:8" s="94" customFormat="1" ht="19.8">
+      <c r="B22" s="175"/>
+      <c r="C22" s="175"/>
+      <c r="D22" s="175"/>
+      <c r="E22" s="175"/>
+      <c r="F22" s="175"/>
+      <c r="G22" s="175"/>
+      <c r="H22" s="175"/>
+    </row>
+    <row r="23" spans="1:8" s="94" customFormat="1" ht="19.5">
       <c r="A23" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="172" t="s">
+      <c r="B23" s="175" t="s">
         <v>116</v>
       </c>
-      <c r="C23" s="172"/>
-      <c r="D23" s="172"/>
-      <c r="E23" s="172"/>
-      <c r="F23" s="172"/>
-      <c r="G23" s="172"/>
-      <c r="H23" s="172"/>
+      <c r="C23" s="175"/>
+      <c r="D23" s="175"/>
+      <c r="E23" s="175"/>
+      <c r="F23" s="175"/>
+      <c r="G23" s="175"/>
+      <c r="H23" s="175"/>
     </row>
     <row r="24" spans="1:8" s="94" customFormat="1" ht="15">
-      <c r="B24" s="173" t="s">
+      <c r="B24" s="177" t="s">
         <v>103</v>
       </c>
-      <c r="C24" s="173"/>
-      <c r="D24" s="173"/>
-      <c r="E24" s="173"/>
-      <c r="F24" s="173"/>
-      <c r="G24" s="173"/>
-      <c r="H24" s="173"/>
+      <c r="C24" s="177"/>
+      <c r="D24" s="177"/>
+      <c r="E24" s="177"/>
+      <c r="F24" s="177"/>
+      <c r="G24" s="177"/>
+      <c r="H24" s="177"/>
     </row>
     <row r="25" spans="1:8" s="94" customFormat="1" ht="30" customHeight="1">
       <c r="B25" s="96" t="s">
@@ -6081,7 +6087,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" s="94" customFormat="1" ht="24.75" customHeight="1">
-      <c r="B26" s="174" t="s">
+      <c r="B26" s="178" t="s">
         <v>59</v>
       </c>
       <c r="C26" s="97" t="s">
@@ -6102,8 +6108,8 @@
       </c>
       <c r="H26" s="102"/>
     </row>
-    <row r="27" spans="1:8" s="94" customFormat="1" ht="18">
-      <c r="B27" s="175"/>
+    <row r="27" spans="1:8" s="94" customFormat="1" ht="17.25">
+      <c r="B27" s="179"/>
       <c r="C27" s="103" t="s">
         <v>62</v>
       </c>
@@ -6125,8 +6131,8 @@
         <v>44714</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="94" customFormat="1" ht="18">
-      <c r="B28" s="176" t="s">
+    <row r="28" spans="1:8" s="94" customFormat="1" ht="17.25">
+      <c r="B28" s="180" t="s">
         <v>63</v>
       </c>
       <c r="C28" s="99" t="s">
@@ -6147,8 +6153,8 @@
       </c>
       <c r="H28" s="102"/>
     </row>
-    <row r="29" spans="1:8" s="94" customFormat="1" ht="18">
-      <c r="B29" s="177"/>
+    <row r="29" spans="1:8" s="94" customFormat="1" ht="17.25">
+      <c r="B29" s="181"/>
       <c r="C29" s="103" t="s">
         <v>106</v>
       </c>
@@ -6168,8 +6174,8 @@
       </c>
       <c r="H29" s="107"/>
     </row>
-    <row r="30" spans="1:8" s="94" customFormat="1" ht="27.6">
-      <c r="B30" s="177"/>
+    <row r="30" spans="1:8" s="94" customFormat="1" ht="27.75">
+      <c r="B30" s="181"/>
       <c r="C30" s="110" t="s">
         <v>117</v>
       </c>
@@ -6189,8 +6195,8 @@
       </c>
       <c r="H30" s="107"/>
     </row>
-    <row r="31" spans="1:8" s="94" customFormat="1" ht="18">
-      <c r="B31" s="178"/>
+    <row r="31" spans="1:8" s="94" customFormat="1" ht="17.25">
+      <c r="B31" s="182"/>
       <c r="C31" s="105" t="s">
         <v>108</v>
       </c>
@@ -6213,7 +6219,7 @@
         <v>36690.270000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="94" customFormat="1" ht="18">
+    <row r="32" spans="1:8" s="94" customFormat="1" ht="17.25">
       <c r="F32" s="114" t="s">
         <v>75</v>
       </c>
@@ -6223,7 +6229,7 @@
         <v>81404.27</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="94" customFormat="1" ht="18">
+    <row r="33" spans="1:8" s="94" customFormat="1" ht="17.25">
       <c r="B33" s="94" t="s">
         <v>110</v>
       </c>
@@ -6267,16 +6273,16 @@
       </c>
     </row>
     <row r="36" spans="1:8" s="94" customFormat="1" ht="12" customHeight="1">
-      <c r="A36" s="179" t="s">
+      <c r="A36" s="183" t="s">
         <v>118</v>
       </c>
-      <c r="B36" s="179"/>
-      <c r="C36" s="179"/>
-      <c r="D36" s="179"/>
-      <c r="E36" s="179"/>
-      <c r="F36" s="179"/>
-      <c r="G36" s="179"/>
-      <c r="H36" s="179"/>
+      <c r="B36" s="183"/>
+      <c r="C36" s="183"/>
+      <c r="D36" s="183"/>
+      <c r="E36" s="183"/>
+      <c r="F36" s="183"/>
+      <c r="G36" s="183"/>
+      <c r="H36" s="183"/>
     </row>
     <row r="37" spans="1:8" s="94" customFormat="1" ht="12" customHeight="1">
       <c r="B37" s="119" t="s">
@@ -6284,16 +6290,16 @@
       </c>
     </row>
     <row r="38" spans="1:8" s="94" customFormat="1" ht="12" customHeight="1">
-      <c r="A38" s="171" t="s">
+      <c r="A38" s="176" t="s">
         <v>112</v>
       </c>
-      <c r="B38" s="171"/>
-      <c r="C38" s="171"/>
-      <c r="D38" s="171"/>
-      <c r="E38" s="171"/>
-      <c r="F38" s="171"/>
-      <c r="G38" s="171"/>
-      <c r="H38" s="171"/>
+      <c r="B38" s="176"/>
+      <c r="C38" s="176"/>
+      <c r="D38" s="176"/>
+      <c r="E38" s="176"/>
+      <c r="F38" s="176"/>
+      <c r="G38" s="176"/>
+      <c r="H38" s="176"/>
     </row>
     <row r="39" spans="1:8" s="94" customFormat="1" ht="12" customHeight="1">
       <c r="B39" s="119" t="s">
@@ -6301,16 +6307,16 @@
       </c>
     </row>
     <row r="40" spans="1:8" s="94" customFormat="1" ht="12" customHeight="1">
-      <c r="A40" s="171" t="s">
+      <c r="A40" s="176" t="s">
         <v>114</v>
       </c>
-      <c r="B40" s="171"/>
-      <c r="C40" s="171"/>
-      <c r="D40" s="171"/>
-      <c r="E40" s="171"/>
-      <c r="F40" s="171"/>
-      <c r="G40" s="171"/>
-      <c r="H40" s="171"/>
+      <c r="B40" s="176"/>
+      <c r="C40" s="176"/>
+      <c r="D40" s="176"/>
+      <c r="E40" s="176"/>
+      <c r="F40" s="176"/>
+      <c r="G40" s="176"/>
+      <c r="H40" s="176"/>
     </row>
     <row r="41" spans="1:8" s="94" customFormat="1" ht="12" customHeight="1">
       <c r="B41" s="119" t="s">
@@ -6322,11 +6328,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="B22:H22"/>
     <mergeCell ref="A38:H38"/>
     <mergeCell ref="A40:H40"/>
     <mergeCell ref="B23:H23"/>
@@ -6334,6 +6335,11 @@
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="A36:H36"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="B22:H22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6348,128 +6354,128 @@
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
-      <c r="A1" s="168" t="s">
+      <c r="A1" s="163" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="168"/>
-      <c r="C1" s="168"/>
-      <c r="D1" s="168"/>
-      <c r="E1" s="168"/>
-      <c r="F1" s="168"/>
-      <c r="G1" s="168"/>
-      <c r="H1" s="168"/>
-      <c r="I1" s="168"/>
-      <c r="J1" s="168"/>
-      <c r="K1" s="168"/>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="22.8">
-      <c r="A2" s="169" t="s">
+      <c r="B1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="163"/>
+      <c r="H1" s="163"/>
+      <c r="I1" s="163"/>
+      <c r="J1" s="163"/>
+      <c r="K1" s="163"/>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="22.5">
+      <c r="A2" s="164" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="169"/>
-      <c r="I2" s="169"/>
-      <c r="J2" s="169"/>
-      <c r="K2" s="169"/>
+      <c r="B2" s="164"/>
+      <c r="C2" s="164"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="164"/>
+      <c r="F2" s="164"/>
+      <c r="G2" s="164"/>
+      <c r="H2" s="164"/>
+      <c r="I2" s="164"/>
+      <c r="J2" s="164"/>
+      <c r="K2" s="164"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="152" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="160"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160"/>
+      <c r="B3" s="152"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="152"/>
+      <c r="G3" s="152"/>
+      <c r="H3" s="152"/>
+      <c r="I3" s="152"/>
+      <c r="J3" s="152"/>
+      <c r="K3" s="152"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1">
-      <c r="A4" s="160" t="s">
+      <c r="A4" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="160"/>
-      <c r="C4" s="160"/>
-      <c r="D4" s="160"/>
-      <c r="E4" s="160"/>
-      <c r="F4" s="160"/>
-      <c r="G4" s="160"/>
-      <c r="H4" s="160"/>
-      <c r="I4" s="160"/>
-      <c r="J4" s="160"/>
-      <c r="K4" s="160"/>
-    </row>
-    <row r="5" spans="1:14" ht="17.399999999999999">
-      <c r="A5" s="170" t="s">
+      <c r="B4" s="152"/>
+      <c r="C4" s="152"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="152"/>
+      <c r="F4" s="152"/>
+      <c r="G4" s="152"/>
+      <c r="H4" s="152"/>
+      <c r="I4" s="152"/>
+      <c r="J4" s="152"/>
+      <c r="K4" s="152"/>
+    </row>
+    <row r="5" spans="1:14" ht="18.75">
+      <c r="A5" s="165" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="170"/>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="170"/>
-      <c r="H5" s="170"/>
-      <c r="I5" s="170"/>
-      <c r="J5" s="170"/>
-      <c r="K5" s="170"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.6">
-      <c r="A6" s="150" t="s">
+      <c r="B5" s="165"/>
+      <c r="C5" s="165"/>
+      <c r="D5" s="165"/>
+      <c r="E5" s="165"/>
+      <c r="F5" s="165"/>
+      <c r="G5" s="165"/>
+      <c r="H5" s="165"/>
+      <c r="I5" s="165"/>
+      <c r="J5" s="165"/>
+      <c r="K5" s="165"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.75">
+      <c r="A6" s="156" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="150"/>
-      <c r="C6" s="150"/>
-      <c r="D6" s="150"/>
-      <c r="E6" s="150"/>
-      <c r="F6" s="150"/>
+      <c r="B6" s="156"/>
+      <c r="C6" s="156"/>
+      <c r="D6" s="156"/>
+      <c r="E6" s="156"/>
+      <c r="F6" s="156"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="167" t="s">
+      <c r="H6" s="162" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="167"/>
-      <c r="J6" s="167"/>
-      <c r="K6" s="167"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.6">
-      <c r="A7" s="164" t="s">
+      <c r="I6" s="162"/>
+      <c r="J6" s="162"/>
+      <c r="K6" s="162"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75">
+      <c r="A7" s="166" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="164"/>
-      <c r="C7" s="164"/>
-      <c r="D7" s="164"/>
-      <c r="E7" s="164"/>
-      <c r="F7" s="164"/>
+      <c r="B7" s="166"/>
+      <c r="C7" s="166"/>
+      <c r="D7" s="166"/>
+      <c r="E7" s="166"/>
+      <c r="F7" s="166"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="165" t="s">
+      <c r="H7" s="167" t="s">
         <v>141</v>
       </c>
-      <c r="I7" s="165"/>
-      <c r="J7" s="165"/>
-      <c r="K7" s="165"/>
+      <c r="I7" s="167"/>
+      <c r="J7" s="167"/>
+      <c r="K7" s="167"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1">
       <c r="A8" s="4" t="s">
@@ -6506,7 +6512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="27.6">
+    <row r="9" spans="1:14" ht="28.5">
       <c r="A9" s="18">
         <v>1</v>
       </c>
@@ -6594,7 +6600,7 @@
       <c r="J12" s="41"/>
       <c r="K12" s="21"/>
     </row>
-    <row r="13" spans="1:14" ht="27.6">
+    <row r="13" spans="1:14" ht="28.5">
       <c r="A13" s="18">
         <v>2</v>
       </c>
@@ -6725,7 +6731,7 @@
       <c r="J18" s="41"/>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="1:14" s="1" customFormat="1" ht="55.2">
+    <row r="19" spans="1:14" s="1" customFormat="1" ht="57">
       <c r="A19" s="59">
         <v>3</v>
       </c>
@@ -6880,7 +6886,7 @@
       <c r="J25" s="41"/>
       <c r="K25" s="21"/>
     </row>
-    <row r="26" spans="1:14" ht="27.6">
+    <row r="26" spans="1:14" ht="28.5">
       <c r="A26" s="18">
         <v>4</v>
       </c>
@@ -6983,7 +6989,7 @@
       <c r="J30" s="41"/>
       <c r="K30" s="21"/>
     </row>
-    <row r="31" spans="1:14" ht="27.6">
+    <row r="31" spans="1:14" ht="28.5">
       <c r="A31" s="18">
         <v>5</v>
       </c>
@@ -7083,7 +7089,7 @@
       <c r="J35" s="41"/>
       <c r="K35" s="21"/>
     </row>
-    <row r="36" spans="1:19" ht="41.4">
+    <row r="36" spans="1:19" ht="42.75">
       <c r="A36" s="18">
         <v>6</v>
       </c>
@@ -7187,7 +7193,7 @@
       <c r="J40" s="41"/>
       <c r="K40" s="21"/>
     </row>
-    <row r="41" spans="1:19" ht="30.6">
+    <row r="41" spans="1:19" ht="30.75">
       <c r="A41" s="18">
         <v>7</v>
       </c>
@@ -7276,7 +7282,7 @@
       <c r="J44" s="40"/>
       <c r="K44" s="21"/>
     </row>
-    <row r="45" spans="1:19" ht="15">
+    <row r="45" spans="1:19">
       <c r="A45" s="18">
         <v>8</v>
       </c>
@@ -7581,7 +7587,7 @@
       </c>
       <c r="K57" s="21"/>
     </row>
-    <row r="58" spans="1:20" ht="15">
+    <row r="58" spans="1:20">
       <c r="A58" s="18"/>
       <c r="B58" s="89"/>
       <c r="C58" s="19"/>
@@ -7594,7 +7600,7 @@
       <c r="J58" s="40"/>
       <c r="K58" s="21"/>
     </row>
-    <row r="59" spans="1:20" ht="39">
+    <row r="59" spans="1:20" ht="39.75">
       <c r="A59" s="18">
         <v>10</v>
       </c>
@@ -7646,15 +7652,15 @@
       <c r="I60" s="39"/>
       <c r="J60" s="39"/>
       <c r="K60" s="61"/>
-      <c r="N60" s="162" t="s">
+      <c r="N60" s="170" t="s">
         <v>87</v>
       </c>
-      <c r="O60" s="162"/>
-      <c r="P60" s="162"/>
-      <c r="Q60" s="162"/>
-      <c r="R60" s="162"/>
-      <c r="S60" s="162"/>
-      <c r="T60" s="162"/>
+      <c r="O60" s="170"/>
+      <c r="P60" s="170"/>
+      <c r="Q60" s="170"/>
+      <c r="R60" s="170"/>
+      <c r="S60" s="170"/>
+      <c r="T60" s="170"/>
     </row>
     <row r="61" spans="1:20" ht="15" customHeight="1">
       <c r="A61" s="18"/>
@@ -7951,15 +7957,15 @@
       <c r="I73" s="39"/>
       <c r="J73" s="39"/>
       <c r="K73" s="61"/>
-      <c r="N73" s="162" t="s">
+      <c r="N73" s="170" t="s">
         <v>87</v>
       </c>
-      <c r="O73" s="162"/>
-      <c r="P73" s="162"/>
-      <c r="Q73" s="162"/>
-      <c r="R73" s="162"/>
-      <c r="S73" s="162"/>
-      <c r="T73" s="162"/>
+      <c r="O73" s="170"/>
+      <c r="P73" s="170"/>
+      <c r="Q73" s="170"/>
+      <c r="R73" s="170"/>
+      <c r="S73" s="170"/>
+      <c r="T73" s="170"/>
     </row>
     <row r="74" spans="1:20" ht="15" customHeight="1">
       <c r="A74" s="18"/>
@@ -8155,15 +8161,15 @@
       <c r="I81" s="39"/>
       <c r="J81" s="39"/>
       <c r="K81" s="61"/>
-      <c r="N81" s="162" t="s">
+      <c r="N81" s="170" t="s">
         <v>87</v>
       </c>
-      <c r="O81" s="162"/>
-      <c r="P81" s="162"/>
-      <c r="Q81" s="162"/>
-      <c r="R81" s="162"/>
-      <c r="S81" s="162"/>
-      <c r="T81" s="162"/>
+      <c r="O81" s="170"/>
+      <c r="P81" s="170"/>
+      <c r="Q81" s="170"/>
+      <c r="R81" s="170"/>
+      <c r="S81" s="170"/>
+      <c r="T81" s="170"/>
     </row>
     <row r="82" spans="1:20" ht="15" customHeight="1">
       <c r="A82" s="18"/>
@@ -8286,7 +8292,7 @@
       <c r="J86" s="41"/>
       <c r="K86" s="21"/>
     </row>
-    <row r="87" spans="1:20" ht="30.6">
+    <row r="87" spans="1:20" ht="30.75">
       <c r="A87" s="18">
         <v>14</v>
       </c>
@@ -8396,7 +8402,7 @@
       <c r="J90" s="125"/>
       <c r="K90" s="123"/>
     </row>
-    <row r="91" spans="1:20" s="1" customFormat="1" ht="27.6">
+    <row r="91" spans="1:20" s="1" customFormat="1" ht="30">
       <c r="A91" s="122"/>
       <c r="B91" s="127" t="s">
         <v>125</v>
@@ -8425,7 +8431,7 @@
       <c r="K91" s="123"/>
       <c r="M91" s="129"/>
     </row>
-    <row r="92" spans="1:20" s="1" customFormat="1" ht="41.4">
+    <row r="92" spans="1:20" s="1" customFormat="1" ht="45">
       <c r="A92" s="122"/>
       <c r="B92" s="127" t="s">
         <v>126</v>
@@ -8481,7 +8487,7 @@
       <c r="K93" s="123"/>
       <c r="M93" s="129"/>
     </row>
-    <row r="94" spans="1:20" s="1" customFormat="1" ht="27.6">
+    <row r="94" spans="1:20" s="1" customFormat="1" ht="30">
       <c r="A94" s="122"/>
       <c r="B94" s="127" t="s">
         <v>133</v>
@@ -8965,7 +8971,7 @@
       <c r="J114" s="125"/>
       <c r="K114" s="21"/>
     </row>
-    <row r="115" spans="1:17" ht="30.6">
+    <row r="115" spans="1:17" ht="30.75">
       <c r="A115" s="18">
         <v>16</v>
       </c>
@@ -9058,7 +9064,7 @@
       <c r="J119" s="40"/>
       <c r="K119" s="21"/>
     </row>
-    <row r="120" spans="1:17" s="1" customFormat="1" ht="46.2">
+    <row r="120" spans="1:17" s="1" customFormat="1" ht="48">
       <c r="A120" s="18">
         <v>17</v>
       </c>
@@ -9155,7 +9161,7 @@
       <c r="J124" s="40"/>
       <c r="K124" s="21"/>
     </row>
-    <row r="125" spans="1:17" s="144" customFormat="1" ht="17.399999999999999">
+    <row r="125" spans="1:17" s="144" customFormat="1" ht="18">
       <c r="A125" s="141">
         <v>18</v>
       </c>
@@ -9380,7 +9386,7 @@
       <c r="J133" s="41"/>
       <c r="K133" s="35"/>
     </row>
-    <row r="134" spans="1:20" s="1" customFormat="1" ht="45">
+    <row r="134" spans="1:20" s="1" customFormat="1" ht="60">
       <c r="A134" s="59">
         <v>19</v>
       </c>
@@ -9600,11 +9606,11 @@
       <c r="B145" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C145" s="163">
+      <c r="C145" s="168">
         <f>J143</f>
         <v>487209.35310074891</v>
       </c>
-      <c r="D145" s="163"/>
+      <c r="D145" s="168"/>
       <c r="E145" s="38">
         <v>100</v>
       </c>
@@ -9620,10 +9626,10 @@
       <c r="B146" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C146" s="166">
+      <c r="C146" s="169">
         <v>500000</v>
       </c>
-      <c r="D146" s="166"/>
+      <c r="D146" s="169"/>
       <c r="E146" s="38"/>
       <c r="F146" s="45"/>
       <c r="G146" s="44"/>
@@ -9637,11 +9643,11 @@
       <c r="B147" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C147" s="166">
+      <c r="C147" s="169">
         <f>C146-C149-C150</f>
         <v>475000</v>
       </c>
-      <c r="D147" s="166"/>
+      <c r="D147" s="169"/>
       <c r="E147" s="38">
         <f>C147/C145*100</f>
         <v>97.494023252418117</v>
@@ -9658,11 +9664,11 @@
       <c r="B148" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C148" s="163">
+      <c r="C148" s="168">
         <f>C145-C147</f>
         <v>12209.353100748907</v>
       </c>
-      <c r="D148" s="163"/>
+      <c r="D148" s="168"/>
       <c r="E148" s="38">
         <f>100-E147</f>
         <v>2.505976747581883</v>
@@ -9679,11 +9685,11 @@
       <c r="B149" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C149" s="163">
+      <c r="C149" s="168">
         <f>C146*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D149" s="163"/>
+      <c r="D149" s="168"/>
       <c r="E149" s="38">
         <v>3</v>
       </c>
@@ -9699,11 +9705,11 @@
       <c r="B150" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C150" s="163">
+      <c r="C150" s="168">
         <f>C146*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D150" s="163"/>
+      <c r="D150" s="168"/>
       <c r="E150" s="38">
         <v>2</v>
       </c>
@@ -9785,6 +9791,18 @@
     <row r="207" s="34" customFormat="1"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C146:D146"/>
+    <mergeCell ref="C147:D147"/>
+    <mergeCell ref="C148:D148"/>
+    <mergeCell ref="C149:D149"/>
+    <mergeCell ref="C150:D150"/>
+    <mergeCell ref="N129:T129"/>
+    <mergeCell ref="N130:T130"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="N60:T60"/>
+    <mergeCell ref="N73:T73"/>
+    <mergeCell ref="N81:T81"/>
     <mergeCell ref="C145:D145"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
@@ -9793,18 +9811,6 @@
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
-    <mergeCell ref="N129:T129"/>
-    <mergeCell ref="N130:T130"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="N60:T60"/>
-    <mergeCell ref="N73:T73"/>
-    <mergeCell ref="N81:T81"/>
-    <mergeCell ref="C146:D146"/>
-    <mergeCell ref="C147:D147"/>
-    <mergeCell ref="C148:D148"/>
-    <mergeCell ref="C149:D149"/>
-    <mergeCell ref="C150:D150"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B100" r:id="rId1"/>
@@ -9825,128 +9831,128 @@
       <selection activeCell="I148" sqref="I148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
-      <c r="A1" s="168" t="s">
+      <c r="A1" s="163" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="168"/>
-      <c r="C1" s="168"/>
-      <c r="D1" s="168"/>
-      <c r="E1" s="168"/>
-      <c r="F1" s="168"/>
-      <c r="G1" s="168"/>
-      <c r="H1" s="168"/>
-      <c r="I1" s="168"/>
-      <c r="J1" s="168"/>
-      <c r="K1" s="168"/>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="22.8">
-      <c r="A2" s="169" t="s">
+      <c r="B1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="163"/>
+      <c r="H1" s="163"/>
+      <c r="I1" s="163"/>
+      <c r="J1" s="163"/>
+      <c r="K1" s="163"/>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="22.5">
+      <c r="A2" s="164" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="169"/>
-      <c r="I2" s="169"/>
-      <c r="J2" s="169"/>
-      <c r="K2" s="169"/>
+      <c r="B2" s="164"/>
+      <c r="C2" s="164"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="164"/>
+      <c r="F2" s="164"/>
+      <c r="G2" s="164"/>
+      <c r="H2" s="164"/>
+      <c r="I2" s="164"/>
+      <c r="J2" s="164"/>
+      <c r="K2" s="164"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="152" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="160"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160"/>
+      <c r="B3" s="152"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="152"/>
+      <c r="G3" s="152"/>
+      <c r="H3" s="152"/>
+      <c r="I3" s="152"/>
+      <c r="J3" s="152"/>
+      <c r="K3" s="152"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1">
-      <c r="A4" s="160" t="s">
+      <c r="A4" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="160"/>
-      <c r="C4" s="160"/>
-      <c r="D4" s="160"/>
-      <c r="E4" s="160"/>
-      <c r="F4" s="160"/>
-      <c r="G4" s="160"/>
-      <c r="H4" s="160"/>
-      <c r="I4" s="160"/>
-      <c r="J4" s="160"/>
-      <c r="K4" s="160"/>
-    </row>
-    <row r="5" spans="1:14" ht="17.399999999999999">
-      <c r="A5" s="170" t="s">
+      <c r="B4" s="152"/>
+      <c r="C4" s="152"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="152"/>
+      <c r="F4" s="152"/>
+      <c r="G4" s="152"/>
+      <c r="H4" s="152"/>
+      <c r="I4" s="152"/>
+      <c r="J4" s="152"/>
+      <c r="K4" s="152"/>
+    </row>
+    <row r="5" spans="1:14" ht="18.75">
+      <c r="A5" s="165" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="170"/>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="170"/>
-      <c r="H5" s="170"/>
-      <c r="I5" s="170"/>
-      <c r="J5" s="170"/>
-      <c r="K5" s="170"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.6">
-      <c r="A6" s="150" t="s">
+      <c r="B5" s="165"/>
+      <c r="C5" s="165"/>
+      <c r="D5" s="165"/>
+      <c r="E5" s="165"/>
+      <c r="F5" s="165"/>
+      <c r="G5" s="165"/>
+      <c r="H5" s="165"/>
+      <c r="I5" s="165"/>
+      <c r="J5" s="165"/>
+      <c r="K5" s="165"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.75">
+      <c r="A6" s="156" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="150"/>
-      <c r="C6" s="150"/>
-      <c r="D6" s="150"/>
-      <c r="E6" s="150"/>
-      <c r="F6" s="150"/>
+      <c r="B6" s="156"/>
+      <c r="C6" s="156"/>
+      <c r="D6" s="156"/>
+      <c r="E6" s="156"/>
+      <c r="F6" s="156"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="167" t="s">
+      <c r="H6" s="162" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="167"/>
-      <c r="J6" s="167"/>
-      <c r="K6" s="167"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.6">
-      <c r="A7" s="164" t="s">
+      <c r="I6" s="162"/>
+      <c r="J6" s="162"/>
+      <c r="K6" s="162"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75">
+      <c r="A7" s="166" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="164"/>
-      <c r="C7" s="164"/>
-      <c r="D7" s="164"/>
-      <c r="E7" s="164"/>
-      <c r="F7" s="164"/>
+      <c r="B7" s="166"/>
+      <c r="C7" s="166"/>
+      <c r="D7" s="166"/>
+      <c r="E7" s="166"/>
+      <c r="F7" s="166"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="165" t="s">
+      <c r="H7" s="167" t="s">
         <v>141</v>
       </c>
-      <c r="I7" s="165"/>
-      <c r="J7" s="165"/>
-      <c r="K7" s="165"/>
+      <c r="I7" s="167"/>
+      <c r="J7" s="167"/>
+      <c r="K7" s="167"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1">
       <c r="A8" s="4" t="s">
@@ -9983,7 +9989,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="27.6">
+    <row r="9" spans="1:14" ht="28.5">
       <c r="A9" s="18">
         <v>1</v>
       </c>
@@ -10071,7 +10077,7 @@
       <c r="J12" s="41"/>
       <c r="K12" s="21"/>
     </row>
-    <row r="13" spans="1:14" ht="27.6">
+    <row r="13" spans="1:14" ht="28.5">
       <c r="A13" s="18">
         <v>2</v>
       </c>
@@ -10202,7 +10208,7 @@
       <c r="J18" s="41"/>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="1:14" s="1" customFormat="1" ht="55.2">
+    <row r="19" spans="1:14" s="1" customFormat="1" ht="57">
       <c r="A19" s="59">
         <v>3</v>
       </c>
@@ -10357,7 +10363,7 @@
       <c r="J25" s="41"/>
       <c r="K25" s="21"/>
     </row>
-    <row r="26" spans="1:14" ht="27.6">
+    <row r="26" spans="1:14" ht="28.5">
       <c r="A26" s="18">
         <v>4</v>
       </c>
@@ -10485,7 +10491,7 @@
       <c r="J31" s="41"/>
       <c r="K31" s="21"/>
     </row>
-    <row r="32" spans="1:14" ht="27.6">
+    <row r="32" spans="1:14" ht="28.5">
       <c r="A32" s="18">
         <v>5</v>
       </c>
@@ -10585,7 +10591,7 @@
       <c r="J36" s="41"/>
       <c r="K36" s="21"/>
     </row>
-    <row r="37" spans="1:19" ht="41.4">
+    <row r="37" spans="1:19" ht="42.75">
       <c r="A37" s="18">
         <v>6</v>
       </c>
@@ -10689,7 +10695,7 @@
       <c r="J41" s="41"/>
       <c r="K41" s="21"/>
     </row>
-    <row r="42" spans="1:19" ht="30.6">
+    <row r="42" spans="1:19" ht="30.75">
       <c r="A42" s="18">
         <v>7</v>
       </c>
@@ -10778,7 +10784,7 @@
       <c r="J45" s="40"/>
       <c r="K45" s="21"/>
     </row>
-    <row r="46" spans="1:19" ht="15">
+    <row r="46" spans="1:19">
       <c r="A46" s="18">
         <v>8</v>
       </c>
@@ -11083,7 +11089,7 @@
       </c>
       <c r="K58" s="21"/>
     </row>
-    <row r="59" spans="1:20" ht="15">
+    <row r="59" spans="1:20">
       <c r="A59" s="18"/>
       <c r="B59" s="89"/>
       <c r="C59" s="19"/>
@@ -11096,7 +11102,7 @@
       <c r="J59" s="40"/>
       <c r="K59" s="21"/>
     </row>
-    <row r="60" spans="1:20" ht="39">
+    <row r="60" spans="1:20" ht="39.75">
       <c r="A60" s="18">
         <v>10</v>
       </c>
@@ -11148,15 +11154,15 @@
       <c r="I61" s="39"/>
       <c r="J61" s="39"/>
       <c r="K61" s="61"/>
-      <c r="N61" s="162" t="s">
+      <c r="N61" s="170" t="s">
         <v>87</v>
       </c>
-      <c r="O61" s="162"/>
-      <c r="P61" s="162"/>
-      <c r="Q61" s="162"/>
-      <c r="R61" s="162"/>
-      <c r="S61" s="162"/>
-      <c r="T61" s="162"/>
+      <c r="O61" s="170"/>
+      <c r="P61" s="170"/>
+      <c r="Q61" s="170"/>
+      <c r="R61" s="170"/>
+      <c r="S61" s="170"/>
+      <c r="T61" s="170"/>
     </row>
     <row r="62" spans="1:20" ht="15" customHeight="1">
       <c r="A62" s="18"/>
@@ -11453,15 +11459,15 @@
       <c r="I74" s="39"/>
       <c r="J74" s="39"/>
       <c r="K74" s="61"/>
-      <c r="N74" s="162" t="s">
+      <c r="N74" s="170" t="s">
         <v>87</v>
       </c>
-      <c r="O74" s="162"/>
-      <c r="P74" s="162"/>
-      <c r="Q74" s="162"/>
-      <c r="R74" s="162"/>
-      <c r="S74" s="162"/>
-      <c r="T74" s="162"/>
+      <c r="O74" s="170"/>
+      <c r="P74" s="170"/>
+      <c r="Q74" s="170"/>
+      <c r="R74" s="170"/>
+      <c r="S74" s="170"/>
+      <c r="T74" s="170"/>
     </row>
     <row r="75" spans="1:20" ht="15" customHeight="1">
       <c r="A75" s="18"/>
@@ -11657,15 +11663,15 @@
       <c r="I82" s="39"/>
       <c r="J82" s="39"/>
       <c r="K82" s="61"/>
-      <c r="N82" s="162" t="s">
+      <c r="N82" s="170" t="s">
         <v>87</v>
       </c>
-      <c r="O82" s="162"/>
-      <c r="P82" s="162"/>
-      <c r="Q82" s="162"/>
-      <c r="R82" s="162"/>
-      <c r="S82" s="162"/>
-      <c r="T82" s="162"/>
+      <c r="O82" s="170"/>
+      <c r="P82" s="170"/>
+      <c r="Q82" s="170"/>
+      <c r="R82" s="170"/>
+      <c r="S82" s="170"/>
+      <c r="T82" s="170"/>
     </row>
     <row r="83" spans="1:20" ht="15" customHeight="1">
       <c r="A83" s="18"/>
@@ -11788,7 +11794,7 @@
       <c r="J87" s="41"/>
       <c r="K87" s="21"/>
     </row>
-    <row r="88" spans="1:20" ht="30.6">
+    <row r="88" spans="1:20" ht="30.75">
       <c r="A88" s="18">
         <v>14</v>
       </c>
@@ -11898,7 +11904,7 @@
       <c r="J91" s="125"/>
       <c r="K91" s="123"/>
     </row>
-    <row r="92" spans="1:20" s="1" customFormat="1" ht="27.6">
+    <row r="92" spans="1:20" s="1" customFormat="1" ht="30">
       <c r="A92" s="122"/>
       <c r="B92" s="127" t="s">
         <v>125</v>
@@ -11927,7 +11933,7 @@
       <c r="K92" s="123"/>
       <c r="M92" s="129"/>
     </row>
-    <row r="93" spans="1:20" s="1" customFormat="1" ht="41.4">
+    <row r="93" spans="1:20" s="1" customFormat="1" ht="45">
       <c r="A93" s="122"/>
       <c r="B93" s="127" t="s">
         <v>126</v>
@@ -11983,7 +11989,7 @@
       <c r="K94" s="123"/>
       <c r="M94" s="129"/>
     </row>
-    <row r="95" spans="1:20" s="1" customFormat="1" ht="27.6">
+    <row r="95" spans="1:20" s="1" customFormat="1" ht="30">
       <c r="A95" s="122"/>
       <c r="B95" s="127" t="s">
         <v>133</v>
@@ -12467,7 +12473,7 @@
       <c r="J115" s="125"/>
       <c r="K115" s="21"/>
     </row>
-    <row r="116" spans="1:17" ht="30.6">
+    <row r="116" spans="1:17" ht="30.75">
       <c r="A116" s="18">
         <v>16</v>
       </c>
@@ -12560,7 +12566,7 @@
       <c r="J120" s="40"/>
       <c r="K120" s="21"/>
     </row>
-    <row r="121" spans="1:17" s="1" customFormat="1" ht="46.2">
+    <row r="121" spans="1:17" s="1" customFormat="1" ht="48">
       <c r="A121" s="18">
         <v>17</v>
       </c>
@@ -12657,7 +12663,7 @@
       <c r="J125" s="40"/>
       <c r="K125" s="21"/>
     </row>
-    <row r="126" spans="1:17" s="144" customFormat="1" ht="17.399999999999999">
+    <row r="126" spans="1:17" s="144" customFormat="1" ht="18">
       <c r="A126" s="141">
         <v>18</v>
       </c>
@@ -12882,7 +12888,7 @@
       <c r="J134" s="41"/>
       <c r="K134" s="35"/>
     </row>
-    <row r="135" spans="1:20" s="1" customFormat="1" ht="45">
+    <row r="135" spans="1:20" s="1" customFormat="1" ht="60">
       <c r="A135" s="59">
         <v>19</v>
       </c>
@@ -13102,11 +13108,11 @@
       <c r="B146" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C146" s="163">
+      <c r="C146" s="168">
         <f>J144</f>
         <v>559342.93667359848</v>
       </c>
-      <c r="D146" s="163"/>
+      <c r="D146" s="168"/>
       <c r="E146" s="38">
         <v>100</v>
       </c>
@@ -13122,10 +13128,10 @@
       <c r="B147" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C147" s="166">
+      <c r="C147" s="169">
         <v>500000</v>
       </c>
-      <c r="D147" s="166"/>
+      <c r="D147" s="169"/>
       <c r="E147" s="38"/>
       <c r="F147" s="45"/>
       <c r="G147" s="44"/>
@@ -13139,11 +13145,11 @@
       <c r="B148" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C148" s="166">
+      <c r="C148" s="169">
         <f>C147-C150-C151</f>
         <v>475000</v>
       </c>
-      <c r="D148" s="166"/>
+      <c r="D148" s="169"/>
       <c r="E148" s="38">
         <f>C148/C146*100</f>
         <v>84.921068785603282</v>
@@ -13160,11 +13166,11 @@
       <c r="B149" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C149" s="163">
+      <c r="C149" s="168">
         <f>C146-C148</f>
         <v>84342.93667359848</v>
       </c>
-      <c r="D149" s="163"/>
+      <c r="D149" s="168"/>
       <c r="E149" s="38">
         <f>100-E148</f>
         <v>15.078931214396718</v>
@@ -13181,11 +13187,11 @@
       <c r="B150" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C150" s="163">
+      <c r="C150" s="168">
         <f>C147*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D150" s="163"/>
+      <c r="D150" s="168"/>
       <c r="E150" s="38">
         <v>3</v>
       </c>
@@ -13201,11 +13207,11 @@
       <c r="B151" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C151" s="163">
+      <c r="C151" s="168">
         <f>C147*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D151" s="163"/>
+      <c r="D151" s="168"/>
       <c r="E151" s="38">
         <v>2</v>
       </c>
@@ -13287,13 +13293,6 @@
     <row r="208" s="34" customFormat="1"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C151:D151"/>
-    <mergeCell ref="N131:T131"/>
-    <mergeCell ref="C146:D146"/>
-    <mergeCell ref="C147:D147"/>
-    <mergeCell ref="C148:D148"/>
-    <mergeCell ref="C149:D149"/>
-    <mergeCell ref="C150:D150"/>
     <mergeCell ref="N130:T130"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
@@ -13307,6 +13306,13 @@
     <mergeCell ref="N61:T61"/>
     <mergeCell ref="N74:T74"/>
     <mergeCell ref="N82:T82"/>
+    <mergeCell ref="C151:D151"/>
+    <mergeCell ref="N131:T131"/>
+    <mergeCell ref="C146:D146"/>
+    <mergeCell ref="C147:D147"/>
+    <mergeCell ref="C148:D148"/>
+    <mergeCell ref="C149:D149"/>
+    <mergeCell ref="C150:D150"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B101" r:id="rId1"/>
@@ -13323,132 +13329,131 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F111" sqref="F111"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
-      <c r="A1" s="168" t="s">
+      <c r="A1" s="163" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="168"/>
-      <c r="C1" s="168"/>
-      <c r="D1" s="168"/>
-      <c r="E1" s="168"/>
-      <c r="F1" s="168"/>
-      <c r="G1" s="168"/>
-      <c r="H1" s="168"/>
-      <c r="I1" s="168"/>
-      <c r="J1" s="168"/>
-      <c r="K1" s="168"/>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="22.8">
-      <c r="A2" s="169" t="s">
+      <c r="B1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="163"/>
+      <c r="H1" s="163"/>
+      <c r="I1" s="163"/>
+      <c r="J1" s="163"/>
+      <c r="K1" s="163"/>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="22.5">
+      <c r="A2" s="164" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="169"/>
-      <c r="I2" s="169"/>
-      <c r="J2" s="169"/>
-      <c r="K2" s="169"/>
+      <c r="B2" s="164"/>
+      <c r="C2" s="164"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="164"/>
+      <c r="F2" s="164"/>
+      <c r="G2" s="164"/>
+      <c r="H2" s="164"/>
+      <c r="I2" s="164"/>
+      <c r="J2" s="164"/>
+      <c r="K2" s="164"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="152" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="160"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160"/>
+      <c r="B3" s="152"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="152"/>
+      <c r="G3" s="152"/>
+      <c r="H3" s="152"/>
+      <c r="I3" s="152"/>
+      <c r="J3" s="152"/>
+      <c r="K3" s="152"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1">
-      <c r="A4" s="160" t="s">
+      <c r="A4" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="160"/>
-      <c r="C4" s="160"/>
-      <c r="D4" s="160"/>
-      <c r="E4" s="160"/>
-      <c r="F4" s="160"/>
-      <c r="G4" s="160"/>
-      <c r="H4" s="160"/>
-      <c r="I4" s="160"/>
-      <c r="J4" s="160"/>
-      <c r="K4" s="160"/>
-    </row>
-    <row r="5" spans="1:14" ht="17.399999999999999">
-      <c r="A5" s="170" t="s">
+      <c r="B4" s="152"/>
+      <c r="C4" s="152"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="152"/>
+      <c r="F4" s="152"/>
+      <c r="G4" s="152"/>
+      <c r="H4" s="152"/>
+      <c r="I4" s="152"/>
+      <c r="J4" s="152"/>
+      <c r="K4" s="152"/>
+    </row>
+    <row r="5" spans="1:14" ht="18.75">
+      <c r="A5" s="165" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="170"/>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="170"/>
-      <c r="H5" s="170"/>
-      <c r="I5" s="170"/>
-      <c r="J5" s="170"/>
-      <c r="K5" s="170"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.6">
-      <c r="A6" s="150" t="s">
+      <c r="B5" s="165"/>
+      <c r="C5" s="165"/>
+      <c r="D5" s="165"/>
+      <c r="E5" s="165"/>
+      <c r="F5" s="165"/>
+      <c r="G5" s="165"/>
+      <c r="H5" s="165"/>
+      <c r="I5" s="165"/>
+      <c r="J5" s="165"/>
+      <c r="K5" s="165"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.75">
+      <c r="A6" s="156" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="150"/>
-      <c r="C6" s="150"/>
-      <c r="D6" s="150"/>
-      <c r="E6" s="150"/>
-      <c r="F6" s="150"/>
+      <c r="B6" s="156"/>
+      <c r="C6" s="156"/>
+      <c r="D6" s="156"/>
+      <c r="E6" s="156"/>
+      <c r="F6" s="156"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="167" t="s">
+      <c r="H6" s="162" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="167"/>
-      <c r="J6" s="167"/>
-      <c r="K6" s="167"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.6">
-      <c r="A7" s="164" t="s">
+      <c r="I6" s="162"/>
+      <c r="J6" s="162"/>
+      <c r="K6" s="162"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75">
+      <c r="A7" s="166" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="164"/>
-      <c r="C7" s="164"/>
-      <c r="D7" s="164"/>
-      <c r="E7" s="164"/>
-      <c r="F7" s="164"/>
+      <c r="B7" s="166"/>
+      <c r="C7" s="166"/>
+      <c r="D7" s="166"/>
+      <c r="E7" s="166"/>
+      <c r="F7" s="166"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="165" t="s">
-        <v>141</v>
-      </c>
-      <c r="I7" s="165"/>
-      <c r="J7" s="165"/>
-      <c r="K7" s="165"/>
+      <c r="H7" s="167" t="s">
+        <v>162</v>
+      </c>
+      <c r="I7" s="167"/>
+      <c r="J7" s="167"/>
+      <c r="K7" s="167"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1">
       <c r="A8" s="4" t="s">
@@ -13485,7 +13490,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="27.6">
+    <row r="9" spans="1:14" ht="28.5">
       <c r="A9" s="18">
         <v>1</v>
       </c>
@@ -13573,7 +13578,7 @@
       <c r="J12" s="41"/>
       <c r="K12" s="21"/>
     </row>
-    <row r="13" spans="1:14" ht="27.6">
+    <row r="13" spans="1:14" ht="28.5">
       <c r="A13" s="18">
         <v>2</v>
       </c>
@@ -13704,7 +13709,7 @@
       <c r="J18" s="41"/>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="1:14" s="1" customFormat="1" ht="55.2">
+    <row r="19" spans="1:14" s="1" customFormat="1" ht="57">
       <c r="A19" s="59">
         <v>3</v>
       </c>
@@ -13859,7 +13864,7 @@
       <c r="J25" s="41"/>
       <c r="K25" s="21"/>
     </row>
-    <row r="26" spans="1:14" ht="27.6">
+    <row r="26" spans="1:14" ht="28.5">
       <c r="A26" s="18">
         <v>4</v>
       </c>
@@ -13962,7 +13967,7 @@
       <c r="J30" s="41"/>
       <c r="K30" s="21"/>
     </row>
-    <row r="31" spans="1:14" ht="27.6">
+    <row r="31" spans="1:14" ht="28.5">
       <c r="A31" s="18">
         <v>5</v>
       </c>
@@ -14062,7 +14067,7 @@
       <c r="J35" s="41"/>
       <c r="K35" s="21"/>
     </row>
-    <row r="36" spans="1:19" ht="41.4">
+    <row r="36" spans="1:19" ht="42.75">
       <c r="A36" s="18">
         <v>6</v>
       </c>
@@ -14166,7 +14171,7 @@
       <c r="J40" s="41"/>
       <c r="K40" s="21"/>
     </row>
-    <row r="41" spans="1:19" ht="30.6">
+    <row r="41" spans="1:19" ht="30.75">
       <c r="A41" s="18">
         <v>7</v>
       </c>
@@ -14255,7 +14260,7 @@
       <c r="J44" s="40"/>
       <c r="K44" s="21"/>
     </row>
-    <row r="45" spans="1:19" ht="15">
+    <row r="45" spans="1:19">
       <c r="A45" s="18">
         <v>8</v>
       </c>
@@ -14560,7 +14565,7 @@
       </c>
       <c r="K57" s="21"/>
     </row>
-    <row r="58" spans="1:20" ht="15">
+    <row r="58" spans="1:20">
       <c r="A58" s="18"/>
       <c r="B58" s="89"/>
       <c r="C58" s="19"/>
@@ -14573,7 +14578,7 @@
       <c r="J58" s="40"/>
       <c r="K58" s="21"/>
     </row>
-    <row r="59" spans="1:20" ht="39">
+    <row r="59" spans="1:20" ht="39.75">
       <c r="A59" s="18">
         <v>10</v>
       </c>
@@ -14625,15 +14630,15 @@
       <c r="I60" s="39"/>
       <c r="J60" s="39"/>
       <c r="K60" s="61"/>
-      <c r="N60" s="162" t="s">
+      <c r="N60" s="170" t="s">
         <v>87</v>
       </c>
-      <c r="O60" s="162"/>
-      <c r="P60" s="162"/>
-      <c r="Q60" s="162"/>
-      <c r="R60" s="162"/>
-      <c r="S60" s="162"/>
-      <c r="T60" s="162"/>
+      <c r="O60" s="170"/>
+      <c r="P60" s="170"/>
+      <c r="Q60" s="170"/>
+      <c r="R60" s="170"/>
+      <c r="S60" s="170"/>
+      <c r="T60" s="170"/>
     </row>
     <row r="61" spans="1:20" ht="15" customHeight="1">
       <c r="A61" s="18"/>
@@ -14930,15 +14935,15 @@
       <c r="I73" s="39"/>
       <c r="J73" s="39"/>
       <c r="K73" s="61"/>
-      <c r="N73" s="162" t="s">
+      <c r="N73" s="170" t="s">
         <v>87</v>
       </c>
-      <c r="O73" s="162"/>
-      <c r="P73" s="162"/>
-      <c r="Q73" s="162"/>
-      <c r="R73" s="162"/>
-      <c r="S73" s="162"/>
-      <c r="T73" s="162"/>
+      <c r="O73" s="170"/>
+      <c r="P73" s="170"/>
+      <c r="Q73" s="170"/>
+      <c r="R73" s="170"/>
+      <c r="S73" s="170"/>
+      <c r="T73" s="170"/>
     </row>
     <row r="74" spans="1:20" ht="15" customHeight="1">
       <c r="A74" s="18"/>
@@ -15134,15 +15139,15 @@
       <c r="I81" s="39"/>
       <c r="J81" s="39"/>
       <c r="K81" s="61"/>
-      <c r="N81" s="162" t="s">
+      <c r="N81" s="170" t="s">
         <v>87</v>
       </c>
-      <c r="O81" s="162"/>
-      <c r="P81" s="162"/>
-      <c r="Q81" s="162"/>
-      <c r="R81" s="162"/>
-      <c r="S81" s="162"/>
-      <c r="T81" s="162"/>
+      <c r="O81" s="170"/>
+      <c r="P81" s="170"/>
+      <c r="Q81" s="170"/>
+      <c r="R81" s="170"/>
+      <c r="S81" s="170"/>
+      <c r="T81" s="170"/>
     </row>
     <row r="82" spans="1:20" ht="15" customHeight="1">
       <c r="A82" s="18"/>
@@ -15265,7 +15270,7 @@
       <c r="J86" s="41"/>
       <c r="K86" s="21"/>
     </row>
-    <row r="87" spans="1:20" ht="30.6">
+    <row r="87" spans="1:20" ht="30.75">
       <c r="A87" s="18">
         <v>14</v>
       </c>
@@ -15375,7 +15380,7 @@
       <c r="J90" s="125"/>
       <c r="K90" s="123"/>
     </row>
-    <row r="91" spans="1:20" s="1" customFormat="1" ht="27.6">
+    <row r="91" spans="1:20" s="1" customFormat="1" ht="30">
       <c r="A91" s="122"/>
       <c r="B91" s="127" t="s">
         <v>125</v>
@@ -15433,7 +15438,7 @@
       <c r="K92" s="123"/>
       <c r="M92" s="129"/>
     </row>
-    <row r="93" spans="1:20" s="1" customFormat="1" ht="41.4">
+    <row r="93" spans="1:20" s="1" customFormat="1" ht="45">
       <c r="A93" s="122"/>
       <c r="B93" s="127" t="s">
         <v>126</v>
@@ -15545,7 +15550,7 @@
       <c r="K96" s="123"/>
       <c r="M96" s="129"/>
     </row>
-    <row r="97" spans="1:13" s="1" customFormat="1" ht="27.6">
+    <row r="97" spans="1:13" s="1" customFormat="1" ht="30">
       <c r="A97" s="122"/>
       <c r="B97" s="127" t="s">
         <v>133</v>
@@ -16029,7 +16034,7 @@
       <c r="J117" s="125"/>
       <c r="K117" s="21"/>
     </row>
-    <row r="118" spans="1:11" ht="30.6">
+    <row r="118" spans="1:11" ht="30.75">
       <c r="A118" s="18">
         <v>16</v>
       </c>
@@ -16122,7 +16127,7 @@
       <c r="J122" s="40"/>
       <c r="K122" s="21"/>
     </row>
-    <row r="123" spans="1:11" s="1" customFormat="1" ht="46.2">
+    <row r="123" spans="1:11" s="1" customFormat="1" ht="48">
       <c r="A123" s="18">
         <v>17</v>
       </c>
@@ -16245,7 +16250,7 @@
       <c r="J128" s="40"/>
       <c r="K128" s="21"/>
     </row>
-    <row r="129" spans="1:20" s="144" customFormat="1" ht="17.399999999999999">
+    <row r="129" spans="1:20" s="144" customFormat="1" ht="18">
       <c r="A129" s="141">
         <v>18</v>
       </c>
@@ -16470,22 +16475,22 @@
       <c r="J137" s="41"/>
       <c r="K137" s="35"/>
     </row>
-    <row r="138" spans="1:20" s="1" customFormat="1" ht="45">
-      <c r="A138" s="59">
+    <row r="138" spans="1:20" ht="42.75">
+      <c r="A138" s="18">
         <v>19</v>
       </c>
-      <c r="B138" s="139" t="s">
+      <c r="B138" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="C138" s="140"/>
-      <c r="D138" s="38"/>
-      <c r="E138" s="38"/>
-      <c r="F138" s="38"/>
+      <c r="C138" s="35"/>
+      <c r="D138" s="37"/>
+      <c r="E138" s="37"/>
+      <c r="F138" s="37"/>
       <c r="G138" s="38"/>
-      <c r="H138" s="38"/>
-      <c r="I138" s="38"/>
+      <c r="H138" s="39"/>
+      <c r="I138" s="39"/>
       <c r="J138" s="41"/>
-      <c r="K138" s="28"/>
+      <c r="K138" s="21"/>
     </row>
     <row r="139" spans="1:20" ht="15" customHeight="1">
       <c r="A139" s="39"/>
@@ -16574,7 +16579,7 @@
       <c r="A143" s="18">
         <v>20</v>
       </c>
-      <c r="B143" s="36" t="s">
+      <c r="B143" s="185" t="s">
         <v>139</v>
       </c>
       <c r="C143" s="19">
@@ -16591,11 +16596,11 @@
         <v>140</v>
       </c>
       <c r="I143" s="23">
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="J143" s="33">
         <f>G143*I143</f>
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="K143" s="21"/>
     </row>
@@ -16633,11 +16638,11 @@
         <v>31</v>
       </c>
       <c r="I145" s="23">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J145" s="33">
         <f>G145*I145</f>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K145" s="21"/>
     </row>
@@ -16668,7 +16673,7 @@
       <c r="I147" s="40"/>
       <c r="J147" s="40">
         <f>SUM(J10:J145)</f>
-        <v>568473.01951057301</v>
+        <v>564973.01951057301</v>
       </c>
       <c r="K147" s="35"/>
     </row>
@@ -16690,11 +16695,11 @@
       <c r="B149" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C149" s="163">
+      <c r="C149" s="168">
         <f>J147</f>
-        <v>568473.01951057301</v>
-      </c>
-      <c r="D149" s="163"/>
+        <v>564973.01951057301</v>
+      </c>
+      <c r="D149" s="168"/>
       <c r="E149" s="38">
         <v>100</v>
       </c>
@@ -16710,10 +16715,10 @@
       <c r="B150" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C150" s="166">
+      <c r="C150" s="169">
         <v>500000</v>
       </c>
-      <c r="D150" s="166"/>
+      <c r="D150" s="169"/>
       <c r="E150" s="38"/>
       <c r="F150" s="45"/>
       <c r="G150" s="44"/>
@@ -16727,14 +16732,14 @@
       <c r="B151" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C151" s="166">
+      <c r="C151" s="169">
         <f>C150-C153-C154</f>
         <v>475000</v>
       </c>
-      <c r="D151" s="166"/>
+      <c r="D151" s="169"/>
       <c r="E151" s="38">
         <f>C151/C149*100</f>
-        <v>83.557175749334831</v>
+        <v>84.074811291251535</v>
       </c>
       <c r="F151" s="45"/>
       <c r="G151" s="44"/>
@@ -16748,14 +16753,14 @@
       <c r="B152" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C152" s="163">
+      <c r="C152" s="168">
         <f>C149-C151</f>
-        <v>93473.019510573009</v>
-      </c>
-      <c r="D152" s="163"/>
+        <v>89973.019510573009</v>
+      </c>
+      <c r="D152" s="168"/>
       <c r="E152" s="38">
         <f>100-E151</f>
-        <v>16.442824250665169</v>
+        <v>15.925188708748465</v>
       </c>
       <c r="F152" s="45"/>
       <c r="G152" s="44"/>
@@ -16769,11 +16774,11 @@
       <c r="B153" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C153" s="163">
+      <c r="C153" s="168">
         <f>C150*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D153" s="163"/>
+      <c r="D153" s="168"/>
       <c r="E153" s="38">
         <v>3</v>
       </c>
@@ -16789,11 +16794,11 @@
       <c r="B154" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C154" s="163">
+      <c r="C154" s="168">
         <f>C150*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D154" s="163"/>
+      <c r="D154" s="168"/>
       <c r="E154" s="38">
         <v>2</v>
       </c>
@@ -16875,6 +16880,13 @@
     <row r="211" s="34" customFormat="1"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C154:D154"/>
+    <mergeCell ref="N134:T134"/>
+    <mergeCell ref="C149:D149"/>
+    <mergeCell ref="C150:D150"/>
+    <mergeCell ref="C151:D151"/>
+    <mergeCell ref="C152:D152"/>
+    <mergeCell ref="C153:D153"/>
     <mergeCell ref="N133:T133"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
@@ -16888,21 +16900,17 @@
     <mergeCell ref="N60:T60"/>
     <mergeCell ref="N73:T73"/>
     <mergeCell ref="N81:T81"/>
-    <mergeCell ref="C154:D154"/>
-    <mergeCell ref="N134:T134"/>
-    <mergeCell ref="C149:D149"/>
-    <mergeCell ref="C150:D150"/>
-    <mergeCell ref="C151:D151"/>
-    <mergeCell ref="C152:D152"/>
-    <mergeCell ref="C153:D153"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B103" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="75" orientation="portrait" r:id="rId2"/>
   <headerFooter>
     <oddFooter>&amp;LPrepared By:&amp;CChecked By:&amp;RApproved By:</oddFooter>
   </headerFooter>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="54" max="10" man="1"/>
+  </rowBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
little correction in previous commit
</commit_message>
<xml_diff>
--- a/ofc/estimates/परोपकार भवन मर्मत/परोपकार भवन मर्मत.xlsx
+++ b/ofc/estimates/परोपकार भवन मर्मत/परोपकार भवन मर्मत.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="WCR" sheetId="6" r:id="rId1"/>
@@ -795,7 +795,7 @@
     <t>-at compound</t>
   </si>
   <si>
-    <t>Date:2081/10/13</t>
+    <t>Date:2081/09/28</t>
   </si>
 </sst>
 </file>
@@ -1499,23 +1499,8 @@
     <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1541,6 +1526,37 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1553,36 +1569,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1605,11 +1596,20 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2624,90 +2624,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="150" t="s">
+      <c r="A1" s="159" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="150"/>
-      <c r="D1" s="150"/>
-      <c r="E1" s="150"/>
-      <c r="F1" s="150"/>
-      <c r="G1" s="150"/>
-      <c r="H1" s="150"/>
-      <c r="I1" s="150"/>
-      <c r="J1" s="150"/>
-      <c r="K1" s="150"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
+      <c r="F1" s="159"/>
+      <c r="G1" s="159"/>
+      <c r="H1" s="159"/>
+      <c r="I1" s="159"/>
+      <c r="J1" s="159"/>
+      <c r="K1" s="159"/>
     </row>
     <row r="2" spans="1:11" ht="25.5">
-      <c r="A2" s="151" t="s">
+      <c r="A2" s="160" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="151"/>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
-      <c r="G2" s="151"/>
-      <c r="H2" s="151"/>
-      <c r="I2" s="151"/>
-      <c r="J2" s="151"/>
-      <c r="K2" s="151"/>
+      <c r="B2" s="160"/>
+      <c r="C2" s="160"/>
+      <c r="D2" s="160"/>
+      <c r="E2" s="160"/>
+      <c r="F2" s="160"/>
+      <c r="G2" s="160"/>
+      <c r="H2" s="160"/>
+      <c r="I2" s="160"/>
+      <c r="J2" s="160"/>
+      <c r="K2" s="160"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1">
-      <c r="A3" s="152" t="s">
+      <c r="A3" s="161" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="152"/>
-      <c r="C3" s="152"/>
-      <c r="D3" s="152"/>
-      <c r="E3" s="152"/>
-      <c r="F3" s="152"/>
-      <c r="G3" s="152"/>
-      <c r="H3" s="152"/>
-      <c r="I3" s="152"/>
-      <c r="J3" s="152"/>
-      <c r="K3" s="152"/>
+      <c r="B3" s="161"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="161"/>
+      <c r="F3" s="161"/>
+      <c r="G3" s="161"/>
+      <c r="H3" s="161"/>
+      <c r="I3" s="161"/>
+      <c r="J3" s="161"/>
+      <c r="K3" s="161"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1">
-      <c r="A4" s="152" t="s">
+      <c r="A4" s="161" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="152"/>
-      <c r="C4" s="152"/>
-      <c r="D4" s="152"/>
-      <c r="E4" s="152"/>
-      <c r="F4" s="152"/>
-      <c r="G4" s="152"/>
-      <c r="H4" s="152"/>
-      <c r="I4" s="152"/>
-      <c r="J4" s="152"/>
-      <c r="K4" s="152"/>
+      <c r="B4" s="161"/>
+      <c r="C4" s="161"/>
+      <c r="D4" s="161"/>
+      <c r="E4" s="161"/>
+      <c r="F4" s="161"/>
+      <c r="G4" s="161"/>
+      <c r="H4" s="161"/>
+      <c r="I4" s="161"/>
+      <c r="J4" s="161"/>
+      <c r="K4" s="161"/>
     </row>
     <row r="5" spans="1:11" ht="18.75">
-      <c r="A5" s="153" t="s">
+      <c r="A5" s="162" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="153"/>
-      <c r="C5" s="153"/>
-      <c r="D5" s="153"/>
-      <c r="E5" s="153"/>
-      <c r="F5" s="153"/>
-      <c r="G5" s="153"/>
-      <c r="H5" s="153"/>
-      <c r="I5" s="153"/>
-      <c r="J5" s="153"/>
-      <c r="K5" s="153"/>
+      <c r="B5" s="162"/>
+      <c r="C5" s="162"/>
+      <c r="D5" s="162"/>
+      <c r="E5" s="162"/>
+      <c r="F5" s="162"/>
+      <c r="G5" s="162"/>
+      <c r="H5" s="162"/>
+      <c r="I5" s="162"/>
+      <c r="J5" s="162"/>
+      <c r="K5" s="162"/>
     </row>
     <row r="6" spans="1:11" ht="18.75">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="148" t="e">
+      <c r="C6" s="157" t="e">
         <f>F18</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="149"/>
+      <c r="D6" s="158"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -2715,11 +2715,11 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="148" t="e">
+      <c r="J6" s="157" t="e">
         <f>I18</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="149"/>
+      <c r="K6" s="158"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="25" t="s">
@@ -2728,77 +2728,77 @@
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="157"/>
-      <c r="G7" s="157"/>
-      <c r="I7" s="158" t="s">
+      <c r="F7" s="152"/>
+      <c r="G7" s="152"/>
+      <c r="I7" s="153" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="158"/>
-      <c r="K7" s="158"/>
+      <c r="J7" s="153"/>
+      <c r="K7" s="153"/>
     </row>
     <row r="8" spans="1:11" ht="15.75">
-      <c r="A8" s="156" t="e">
+      <c r="A8" s="151" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="156"/>
-      <c r="C8" s="156"/>
-      <c r="D8" s="156"/>
-      <c r="E8" s="156"/>
-      <c r="F8" s="156"/>
-      <c r="I8" s="159" t="s">
+      <c r="B8" s="151"/>
+      <c r="C8" s="151"/>
+      <c r="D8" s="151"/>
+      <c r="E8" s="151"/>
+      <c r="F8" s="151"/>
+      <c r="I8" s="154" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="159"/>
-      <c r="K8" s="159"/>
+      <c r="J8" s="154"/>
+      <c r="K8" s="154"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="160" t="e">
+      <c r="A9" s="155" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="160"/>
-      <c r="C9" s="160"/>
-      <c r="D9" s="160"/>
-      <c r="E9" s="160"/>
-      <c r="F9" s="160"/>
-      <c r="I9" s="159" t="s">
+      <c r="B9" s="155"/>
+      <c r="C9" s="155"/>
+      <c r="D9" s="155"/>
+      <c r="E9" s="155"/>
+      <c r="F9" s="155"/>
+      <c r="I9" s="154" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="159"/>
-      <c r="K9" s="159"/>
+      <c r="J9" s="154"/>
+      <c r="K9" s="154"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="154" t="s">
+      <c r="A11" s="149" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="154" t="s">
+      <c r="B11" s="149" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="154" t="s">
+      <c r="C11" s="149" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="161" t="s">
+      <c r="D11" s="156" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="161"/>
-      <c r="F11" s="161"/>
-      <c r="G11" s="161" t="s">
+      <c r="E11" s="156"/>
+      <c r="F11" s="156"/>
+      <c r="G11" s="156" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="161"/>
-      <c r="I11" s="161"/>
-      <c r="J11" s="154" t="s">
+      <c r="H11" s="156"/>
+      <c r="I11" s="156"/>
+      <c r="J11" s="149" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="155" t="s">
+      <c r="K11" s="150" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="154"/>
-      <c r="B12" s="154"/>
-      <c r="C12" s="154"/>
+      <c r="A12" s="149"/>
+      <c r="B12" s="149"/>
+      <c r="C12" s="149"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -2817,8 +2817,8 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="154"/>
-      <c r="K12" s="155"/>
+      <c r="J12" s="149"/>
+      <c r="K12" s="150"/>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A13" s="26" t="e">
@@ -2980,6 +2980,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -2993,13 +3000,6 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3036,113 +3036,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
-      <c r="A1" s="163" t="s">
+      <c r="A1" s="169" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
+      <c r="B1" s="169"/>
+      <c r="C1" s="169"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
+      <c r="G1" s="169"/>
+      <c r="H1" s="169"/>
+      <c r="I1" s="169"/>
+      <c r="J1" s="169"/>
+      <c r="K1" s="169"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="22.5">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="170" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="164"/>
-      <c r="C2" s="164"/>
-      <c r="D2" s="164"/>
-      <c r="E2" s="164"/>
-      <c r="F2" s="164"/>
-      <c r="G2" s="164"/>
-      <c r="H2" s="164"/>
-      <c r="I2" s="164"/>
-      <c r="J2" s="164"/>
-      <c r="K2" s="164"/>
+      <c r="B2" s="170"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="170"/>
+      <c r="I2" s="170"/>
+      <c r="J2" s="170"/>
+      <c r="K2" s="170"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1">
-      <c r="A3" s="152" t="s">
+      <c r="A3" s="161" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="152"/>
-      <c r="C3" s="152"/>
-      <c r="D3" s="152"/>
-      <c r="E3" s="152"/>
-      <c r="F3" s="152"/>
-      <c r="G3" s="152"/>
-      <c r="H3" s="152"/>
-      <c r="I3" s="152"/>
-      <c r="J3" s="152"/>
-      <c r="K3" s="152"/>
+      <c r="B3" s="161"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="161"/>
+      <c r="F3" s="161"/>
+      <c r="G3" s="161"/>
+      <c r="H3" s="161"/>
+      <c r="I3" s="161"/>
+      <c r="J3" s="161"/>
+      <c r="K3" s="161"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1">
-      <c r="A4" s="152" t="s">
+      <c r="A4" s="161" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="152"/>
-      <c r="C4" s="152"/>
-      <c r="D4" s="152"/>
-      <c r="E4" s="152"/>
-      <c r="F4" s="152"/>
-      <c r="G4" s="152"/>
-      <c r="H4" s="152"/>
-      <c r="I4" s="152"/>
-      <c r="J4" s="152"/>
-      <c r="K4" s="152"/>
+      <c r="B4" s="161"/>
+      <c r="C4" s="161"/>
+      <c r="D4" s="161"/>
+      <c r="E4" s="161"/>
+      <c r="F4" s="161"/>
+      <c r="G4" s="161"/>
+      <c r="H4" s="161"/>
+      <c r="I4" s="161"/>
+      <c r="J4" s="161"/>
+      <c r="K4" s="161"/>
     </row>
     <row r="5" spans="1:14" ht="18.75">
-      <c r="A5" s="165" t="s">
+      <c r="A5" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="165"/>
-      <c r="C5" s="165"/>
-      <c r="D5" s="165"/>
-      <c r="E5" s="165"/>
-      <c r="F5" s="165"/>
-      <c r="G5" s="165"/>
-      <c r="H5" s="165"/>
-      <c r="I5" s="165"/>
-      <c r="J5" s="165"/>
-      <c r="K5" s="165"/>
+      <c r="B5" s="171"/>
+      <c r="C5" s="171"/>
+      <c r="D5" s="171"/>
+      <c r="E5" s="171"/>
+      <c r="F5" s="171"/>
+      <c r="G5" s="171"/>
+      <c r="H5" s="171"/>
+      <c r="I5" s="171"/>
+      <c r="J5" s="171"/>
+      <c r="K5" s="171"/>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="156" t="s">
+      <c r="A6" s="151" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="156"/>
-      <c r="C6" s="156"/>
-      <c r="D6" s="156"/>
-      <c r="E6" s="156"/>
-      <c r="F6" s="156"/>
+      <c r="B6" s="151"/>
+      <c r="C6" s="151"/>
+      <c r="D6" s="151"/>
+      <c r="E6" s="151"/>
+      <c r="F6" s="151"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="162" t="s">
+      <c r="H6" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="162"/>
-      <c r="J6" s="162"/>
-      <c r="K6" s="162"/>
+      <c r="I6" s="168"/>
+      <c r="J6" s="168"/>
+      <c r="K6" s="168"/>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="166" t="s">
+      <c r="A7" s="165" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="166"/>
-      <c r="C7" s="166"/>
-      <c r="D7" s="166"/>
-      <c r="E7" s="166"/>
-      <c r="F7" s="166"/>
+      <c r="B7" s="165"/>
+      <c r="C7" s="165"/>
+      <c r="D7" s="165"/>
+      <c r="E7" s="165"/>
+      <c r="F7" s="165"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="167" t="s">
+      <c r="H7" s="166" t="s">
         <v>141</v>
       </c>
-      <c r="I7" s="167"/>
-      <c r="J7" s="167"/>
-      <c r="K7" s="167"/>
+      <c r="I7" s="166"/>
+      <c r="J7" s="166"/>
+      <c r="K7" s="166"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1">
       <c r="A8" s="4" t="s">
@@ -3886,15 +3886,15 @@
       <c r="I41" s="39"/>
       <c r="J41" s="39"/>
       <c r="K41" s="61"/>
-      <c r="N41" s="170" t="s">
+      <c r="N41" s="163" t="s">
         <v>87</v>
       </c>
-      <c r="O41" s="170"/>
-      <c r="P41" s="170"/>
-      <c r="Q41" s="170"/>
-      <c r="R41" s="170"/>
-      <c r="S41" s="170"/>
-      <c r="T41" s="170"/>
+      <c r="O41" s="163"/>
+      <c r="P41" s="163"/>
+      <c r="Q41" s="163"/>
+      <c r="R41" s="163"/>
+      <c r="S41" s="163"/>
+      <c r="T41" s="163"/>
     </row>
     <row r="42" spans="1:20" ht="15" customHeight="1">
       <c r="A42" s="18"/>
@@ -4191,15 +4191,15 @@
       <c r="I54" s="39"/>
       <c r="J54" s="39"/>
       <c r="K54" s="61"/>
-      <c r="N54" s="170" t="s">
+      <c r="N54" s="163" t="s">
         <v>87</v>
       </c>
-      <c r="O54" s="170"/>
-      <c r="P54" s="170"/>
-      <c r="Q54" s="170"/>
-      <c r="R54" s="170"/>
-      <c r="S54" s="170"/>
-      <c r="T54" s="170"/>
+      <c r="O54" s="163"/>
+      <c r="P54" s="163"/>
+      <c r="Q54" s="163"/>
+      <c r="R54" s="163"/>
+      <c r="S54" s="163"/>
+      <c r="T54" s="163"/>
     </row>
     <row r="55" spans="1:20" ht="15" customHeight="1">
       <c r="A55" s="18"/>
@@ -4395,15 +4395,15 @@
       <c r="I62" s="39"/>
       <c r="J62" s="39"/>
       <c r="K62" s="61"/>
-      <c r="N62" s="170" t="s">
+      <c r="N62" s="163" t="s">
         <v>87</v>
       </c>
-      <c r="O62" s="170"/>
-      <c r="P62" s="170"/>
-      <c r="Q62" s="170"/>
-      <c r="R62" s="170"/>
-      <c r="S62" s="170"/>
-      <c r="T62" s="170"/>
+      <c r="O62" s="163"/>
+      <c r="P62" s="163"/>
+      <c r="Q62" s="163"/>
+      <c r="R62" s="163"/>
+      <c r="S62" s="163"/>
+      <c r="T62" s="163"/>
     </row>
     <row r="63" spans="1:20" ht="15" customHeight="1">
       <c r="A63" s="18"/>
@@ -5430,11 +5430,11 @@
       <c r="B109" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C109" s="168">
+      <c r="C109" s="164">
         <f>J107</f>
         <v>336917.6969730733</v>
       </c>
-      <c r="D109" s="168"/>
+      <c r="D109" s="164"/>
       <c r="E109" s="38">
         <v>100</v>
       </c>
@@ -5450,10 +5450,10 @@
       <c r="B110" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C110" s="169">
+      <c r="C110" s="167">
         <v>300000</v>
       </c>
-      <c r="D110" s="169"/>
+      <c r="D110" s="167"/>
       <c r="E110" s="38"/>
       <c r="F110" s="45"/>
       <c r="G110" s="44"/>
@@ -5467,11 +5467,11 @@
       <c r="B111" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C111" s="169">
+      <c r="C111" s="167">
         <f>C110-C113-C114</f>
         <v>285000</v>
       </c>
-      <c r="D111" s="169"/>
+      <c r="D111" s="167"/>
       <c r="E111" s="38">
         <f>C111/C109*100</f>
         <v>84.590391825804687</v>
@@ -5488,11 +5488,11 @@
       <c r="B112" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C112" s="168">
+      <c r="C112" s="164">
         <f>C109-C111</f>
         <v>51917.696973073296</v>
       </c>
-      <c r="D112" s="168"/>
+      <c r="D112" s="164"/>
       <c r="E112" s="38">
         <f>100-E111</f>
         <v>15.409608174195313</v>
@@ -5509,11 +5509,11 @@
       <c r="B113" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C113" s="168">
+      <c r="C113" s="164">
         <f>C110*0.03</f>
         <v>9000</v>
       </c>
-      <c r="D113" s="168"/>
+      <c r="D113" s="164"/>
       <c r="E113" s="38">
         <v>3</v>
       </c>
@@ -5529,11 +5529,11 @@
       <c r="B114" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C114" s="168">
+      <c r="C114" s="164">
         <f>C110*0.02</f>
         <v>6000</v>
       </c>
-      <c r="D114" s="168"/>
+      <c r="D114" s="164"/>
       <c r="E114" s="38">
         <v>2</v>
       </c>
@@ -5615,17 +5615,6 @@
     <row r="171" s="34" customFormat="1"/>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="N41:T41"/>
-    <mergeCell ref="N54:T54"/>
-    <mergeCell ref="N62:T62"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C111:D111"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
@@ -5633,6 +5622,17 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="N41:T41"/>
+    <mergeCell ref="N54:T54"/>
+    <mergeCell ref="N62:T62"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C112:D112"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B80" r:id="rId1"/>
@@ -5650,7 +5650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
@@ -5697,27 +5697,27 @@
       <c r="A3" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="171" t="s">
+      <c r="B3" s="181" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="171"/>
-      <c r="D3" s="171"/>
-      <c r="E3" s="171"/>
-      <c r="F3" s="171"/>
-      <c r="G3" s="171"/>
-      <c r="H3" s="171"/>
+      <c r="C3" s="181"/>
+      <c r="D3" s="181"/>
+      <c r="E3" s="181"/>
+      <c r="F3" s="181"/>
+      <c r="G3" s="181"/>
+      <c r="H3" s="181"/>
     </row>
     <row r="4" spans="1:10" ht="15.75">
       <c r="A4" s="68"/>
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="182" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="172"/>
-      <c r="D4" s="172"/>
-      <c r="E4" s="172"/>
-      <c r="F4" s="172"/>
-      <c r="G4" s="172"/>
-      <c r="H4" s="172"/>
+      <c r="C4" s="182"/>
+      <c r="D4" s="182"/>
+      <c r="E4" s="182"/>
+      <c r="F4" s="182"/>
+      <c r="G4" s="182"/>
+      <c r="H4" s="182"/>
     </row>
     <row r="5" spans="1:10" ht="31.5">
       <c r="A5" s="68"/>
@@ -5745,7 +5745,7 @@
     </row>
     <row r="6" spans="1:10" ht="17.25">
       <c r="A6" s="68"/>
-      <c r="B6" s="173" t="s">
+      <c r="B6" s="183" t="s">
         <v>59</v>
       </c>
       <c r="C6" s="69" t="s">
@@ -5768,7 +5768,7 @@
     </row>
     <row r="7" spans="1:10" ht="17.25">
       <c r="A7" s="68"/>
-      <c r="B7" s="174"/>
+      <c r="B7" s="184"/>
       <c r="C7" s="71" t="s">
         <v>62</v>
       </c>
@@ -5792,7 +5792,7 @@
     </row>
     <row r="8" spans="1:10" ht="45">
       <c r="A8" s="68"/>
-      <c r="B8" s="173" t="s">
+      <c r="B8" s="183" t="s">
         <v>63</v>
       </c>
       <c r="C8" s="75" t="s">
@@ -5815,7 +5815,7 @@
     </row>
     <row r="9" spans="1:10" ht="17.25">
       <c r="A9" s="68"/>
-      <c r="B9" s="173"/>
+      <c r="B9" s="183"/>
       <c r="C9" s="71" t="s">
         <v>66</v>
       </c>
@@ -5836,7 +5836,7 @@
     </row>
     <row r="10" spans="1:10" ht="17.25">
       <c r="A10" s="68"/>
-      <c r="B10" s="173"/>
+      <c r="B10" s="183"/>
       <c r="C10" s="71" t="s">
         <v>68</v>
       </c>
@@ -5861,7 +5861,7 @@
     </row>
     <row r="11" spans="1:10" ht="17.25">
       <c r="A11" s="68"/>
-      <c r="B11" s="173"/>
+      <c r="B11" s="183"/>
       <c r="C11" s="71" t="s">
         <v>70</v>
       </c>
@@ -5883,7 +5883,7 @@
     </row>
     <row r="12" spans="1:10" ht="17.25">
       <c r="A12" s="68"/>
-      <c r="B12" s="173"/>
+      <c r="B12" s="183"/>
       <c r="C12" s="71" t="s">
         <v>71</v>
       </c>
@@ -5909,7 +5909,7 @@
     </row>
     <row r="13" spans="1:10" ht="17.25">
       <c r="A13" s="68"/>
-      <c r="B13" s="173"/>
+      <c r="B13" s="183"/>
       <c r="C13" s="71" t="s">
         <v>73</v>
       </c>
@@ -6030,38 +6030,38 @@
         <f>+A9+1</f>
         <v>1</v>
       </c>
-      <c r="B22" s="175"/>
-      <c r="C22" s="175"/>
-      <c r="D22" s="175"/>
-      <c r="E22" s="175"/>
-      <c r="F22" s="175"/>
-      <c r="G22" s="175"/>
-      <c r="H22" s="175"/>
+      <c r="B22" s="173"/>
+      <c r="C22" s="173"/>
+      <c r="D22" s="173"/>
+      <c r="E22" s="173"/>
+      <c r="F22" s="173"/>
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
     </row>
     <row r="23" spans="1:8" s="94" customFormat="1" ht="19.5">
       <c r="A23" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="175" t="s">
+      <c r="B23" s="173" t="s">
         <v>116</v>
       </c>
-      <c r="C23" s="175"/>
-      <c r="D23" s="175"/>
-      <c r="E23" s="175"/>
-      <c r="F23" s="175"/>
-      <c r="G23" s="175"/>
-      <c r="H23" s="175"/>
+      <c r="C23" s="173"/>
+      <c r="D23" s="173"/>
+      <c r="E23" s="173"/>
+      <c r="F23" s="173"/>
+      <c r="G23" s="173"/>
+      <c r="H23" s="173"/>
     </row>
     <row r="24" spans="1:8" s="94" customFormat="1" ht="15">
-      <c r="B24" s="177" t="s">
+      <c r="B24" s="174" t="s">
         <v>103</v>
       </c>
-      <c r="C24" s="177"/>
-      <c r="D24" s="177"/>
-      <c r="E24" s="177"/>
-      <c r="F24" s="177"/>
-      <c r="G24" s="177"/>
-      <c r="H24" s="177"/>
+      <c r="C24" s="174"/>
+      <c r="D24" s="174"/>
+      <c r="E24" s="174"/>
+      <c r="F24" s="174"/>
+      <c r="G24" s="174"/>
+      <c r="H24" s="174"/>
     </row>
     <row r="25" spans="1:8" s="94" customFormat="1" ht="30" customHeight="1">
       <c r="B25" s="96" t="s">
@@ -6087,7 +6087,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" s="94" customFormat="1" ht="24.75" customHeight="1">
-      <c r="B26" s="178" t="s">
+      <c r="B26" s="175" t="s">
         <v>59</v>
       </c>
       <c r="C26" s="97" t="s">
@@ -6109,7 +6109,7 @@
       <c r="H26" s="102"/>
     </row>
     <row r="27" spans="1:8" s="94" customFormat="1" ht="17.25">
-      <c r="B27" s="179"/>
+      <c r="B27" s="176"/>
       <c r="C27" s="103" t="s">
         <v>62</v>
       </c>
@@ -6132,7 +6132,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" s="94" customFormat="1" ht="17.25">
-      <c r="B28" s="180" t="s">
+      <c r="B28" s="177" t="s">
         <v>63</v>
       </c>
       <c r="C28" s="99" t="s">
@@ -6154,7 +6154,7 @@
       <c r="H28" s="102"/>
     </row>
     <row r="29" spans="1:8" s="94" customFormat="1" ht="17.25">
-      <c r="B29" s="181"/>
+      <c r="B29" s="178"/>
       <c r="C29" s="103" t="s">
         <v>106</v>
       </c>
@@ -6175,7 +6175,7 @@
       <c r="H29" s="107"/>
     </row>
     <row r="30" spans="1:8" s="94" customFormat="1" ht="27.75">
-      <c r="B30" s="181"/>
+      <c r="B30" s="178"/>
       <c r="C30" s="110" t="s">
         <v>117</v>
       </c>
@@ -6196,7 +6196,7 @@
       <c r="H30" s="107"/>
     </row>
     <row r="31" spans="1:8" s="94" customFormat="1" ht="17.25">
-      <c r="B31" s="182"/>
+      <c r="B31" s="179"/>
       <c r="C31" s="105" t="s">
         <v>108</v>
       </c>
@@ -6273,16 +6273,16 @@
       </c>
     </row>
     <row r="36" spans="1:8" s="94" customFormat="1" ht="12" customHeight="1">
-      <c r="A36" s="183" t="s">
+      <c r="A36" s="180" t="s">
         <v>118</v>
       </c>
-      <c r="B36" s="183"/>
-      <c r="C36" s="183"/>
-      <c r="D36" s="183"/>
-      <c r="E36" s="183"/>
-      <c r="F36" s="183"/>
-      <c r="G36" s="183"/>
-      <c r="H36" s="183"/>
+      <c r="B36" s="180"/>
+      <c r="C36" s="180"/>
+      <c r="D36" s="180"/>
+      <c r="E36" s="180"/>
+      <c r="F36" s="180"/>
+      <c r="G36" s="180"/>
+      <c r="H36" s="180"/>
     </row>
     <row r="37" spans="1:8" s="94" customFormat="1" ht="12" customHeight="1">
       <c r="B37" s="119" t="s">
@@ -6290,16 +6290,16 @@
       </c>
     </row>
     <row r="38" spans="1:8" s="94" customFormat="1" ht="12" customHeight="1">
-      <c r="A38" s="176" t="s">
+      <c r="A38" s="172" t="s">
         <v>112</v>
       </c>
-      <c r="B38" s="176"/>
-      <c r="C38" s="176"/>
-      <c r="D38" s="176"/>
-      <c r="E38" s="176"/>
-      <c r="F38" s="176"/>
-      <c r="G38" s="176"/>
-      <c r="H38" s="176"/>
+      <c r="B38" s="172"/>
+      <c r="C38" s="172"/>
+      <c r="D38" s="172"/>
+      <c r="E38" s="172"/>
+      <c r="F38" s="172"/>
+      <c r="G38" s="172"/>
+      <c r="H38" s="172"/>
     </row>
     <row r="39" spans="1:8" s="94" customFormat="1" ht="12" customHeight="1">
       <c r="B39" s="119" t="s">
@@ -6307,16 +6307,16 @@
       </c>
     </row>
     <row r="40" spans="1:8" s="94" customFormat="1" ht="12" customHeight="1">
-      <c r="A40" s="176" t="s">
+      <c r="A40" s="172" t="s">
         <v>114</v>
       </c>
-      <c r="B40" s="176"/>
-      <c r="C40" s="176"/>
-      <c r="D40" s="176"/>
-      <c r="E40" s="176"/>
-      <c r="F40" s="176"/>
-      <c r="G40" s="176"/>
-      <c r="H40" s="176"/>
+      <c r="B40" s="172"/>
+      <c r="C40" s="172"/>
+      <c r="D40" s="172"/>
+      <c r="E40" s="172"/>
+      <c r="F40" s="172"/>
+      <c r="G40" s="172"/>
+      <c r="H40" s="172"/>
     </row>
     <row r="41" spans="1:8" s="94" customFormat="1" ht="12" customHeight="1">
       <c r="B41" s="119" t="s">
@@ -6328,6 +6328,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="B22:H22"/>
     <mergeCell ref="A38:H38"/>
     <mergeCell ref="A40:H40"/>
     <mergeCell ref="B23:H23"/>
@@ -6335,11 +6340,6 @@
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="A36:H36"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="B22:H22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6369,113 +6369,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
-      <c r="A1" s="163" t="s">
+      <c r="A1" s="169" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
+      <c r="B1" s="169"/>
+      <c r="C1" s="169"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
+      <c r="G1" s="169"/>
+      <c r="H1" s="169"/>
+      <c r="I1" s="169"/>
+      <c r="J1" s="169"/>
+      <c r="K1" s="169"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="22.5">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="170" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="164"/>
-      <c r="C2" s="164"/>
-      <c r="D2" s="164"/>
-      <c r="E2" s="164"/>
-      <c r="F2" s="164"/>
-      <c r="G2" s="164"/>
-      <c r="H2" s="164"/>
-      <c r="I2" s="164"/>
-      <c r="J2" s="164"/>
-      <c r="K2" s="164"/>
+      <c r="B2" s="170"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="170"/>
+      <c r="I2" s="170"/>
+      <c r="J2" s="170"/>
+      <c r="K2" s="170"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1">
-      <c r="A3" s="152" t="s">
+      <c r="A3" s="161" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="152"/>
-      <c r="C3" s="152"/>
-      <c r="D3" s="152"/>
-      <c r="E3" s="152"/>
-      <c r="F3" s="152"/>
-      <c r="G3" s="152"/>
-      <c r="H3" s="152"/>
-      <c r="I3" s="152"/>
-      <c r="J3" s="152"/>
-      <c r="K3" s="152"/>
+      <c r="B3" s="161"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="161"/>
+      <c r="F3" s="161"/>
+      <c r="G3" s="161"/>
+      <c r="H3" s="161"/>
+      <c r="I3" s="161"/>
+      <c r="J3" s="161"/>
+      <c r="K3" s="161"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1">
-      <c r="A4" s="152" t="s">
+      <c r="A4" s="161" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="152"/>
-      <c r="C4" s="152"/>
-      <c r="D4" s="152"/>
-      <c r="E4" s="152"/>
-      <c r="F4" s="152"/>
-      <c r="G4" s="152"/>
-      <c r="H4" s="152"/>
-      <c r="I4" s="152"/>
-      <c r="J4" s="152"/>
-      <c r="K4" s="152"/>
+      <c r="B4" s="161"/>
+      <c r="C4" s="161"/>
+      <c r="D4" s="161"/>
+      <c r="E4" s="161"/>
+      <c r="F4" s="161"/>
+      <c r="G4" s="161"/>
+      <c r="H4" s="161"/>
+      <c r="I4" s="161"/>
+      <c r="J4" s="161"/>
+      <c r="K4" s="161"/>
     </row>
     <row r="5" spans="1:14" ht="18.75">
-      <c r="A5" s="165" t="s">
+      <c r="A5" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="165"/>
-      <c r="C5" s="165"/>
-      <c r="D5" s="165"/>
-      <c r="E5" s="165"/>
-      <c r="F5" s="165"/>
-      <c r="G5" s="165"/>
-      <c r="H5" s="165"/>
-      <c r="I5" s="165"/>
-      <c r="J5" s="165"/>
-      <c r="K5" s="165"/>
+      <c r="B5" s="171"/>
+      <c r="C5" s="171"/>
+      <c r="D5" s="171"/>
+      <c r="E5" s="171"/>
+      <c r="F5" s="171"/>
+      <c r="G5" s="171"/>
+      <c r="H5" s="171"/>
+      <c r="I5" s="171"/>
+      <c r="J5" s="171"/>
+      <c r="K5" s="171"/>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="156" t="s">
+      <c r="A6" s="151" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="156"/>
-      <c r="C6" s="156"/>
-      <c r="D6" s="156"/>
-      <c r="E6" s="156"/>
-      <c r="F6" s="156"/>
+      <c r="B6" s="151"/>
+      <c r="C6" s="151"/>
+      <c r="D6" s="151"/>
+      <c r="E6" s="151"/>
+      <c r="F6" s="151"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="162" t="s">
+      <c r="H6" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="162"/>
-      <c r="J6" s="162"/>
-      <c r="K6" s="162"/>
+      <c r="I6" s="168"/>
+      <c r="J6" s="168"/>
+      <c r="K6" s="168"/>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="166" t="s">
+      <c r="A7" s="165" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="166"/>
-      <c r="C7" s="166"/>
-      <c r="D7" s="166"/>
-      <c r="E7" s="166"/>
-      <c r="F7" s="166"/>
+      <c r="B7" s="165"/>
+      <c r="C7" s="165"/>
+      <c r="D7" s="165"/>
+      <c r="E7" s="165"/>
+      <c r="F7" s="165"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="167" t="s">
+      <c r="H7" s="166" t="s">
         <v>141</v>
       </c>
-      <c r="I7" s="167"/>
-      <c r="J7" s="167"/>
-      <c r="K7" s="167"/>
+      <c r="I7" s="166"/>
+      <c r="J7" s="166"/>
+      <c r="K7" s="166"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1">
       <c r="A8" s="4" t="s">
@@ -7652,15 +7652,15 @@
       <c r="I60" s="39"/>
       <c r="J60" s="39"/>
       <c r="K60" s="61"/>
-      <c r="N60" s="170" t="s">
+      <c r="N60" s="163" t="s">
         <v>87</v>
       </c>
-      <c r="O60" s="170"/>
-      <c r="P60" s="170"/>
-      <c r="Q60" s="170"/>
-      <c r="R60" s="170"/>
-      <c r="S60" s="170"/>
-      <c r="T60" s="170"/>
+      <c r="O60" s="163"/>
+      <c r="P60" s="163"/>
+      <c r="Q60" s="163"/>
+      <c r="R60" s="163"/>
+      <c r="S60" s="163"/>
+      <c r="T60" s="163"/>
     </row>
     <row r="61" spans="1:20" ht="15" customHeight="1">
       <c r="A61" s="18"/>
@@ -7957,15 +7957,15 @@
       <c r="I73" s="39"/>
       <c r="J73" s="39"/>
       <c r="K73" s="61"/>
-      <c r="N73" s="170" t="s">
+      <c r="N73" s="163" t="s">
         <v>87</v>
       </c>
-      <c r="O73" s="170"/>
-      <c r="P73" s="170"/>
-      <c r="Q73" s="170"/>
-      <c r="R73" s="170"/>
-      <c r="S73" s="170"/>
-      <c r="T73" s="170"/>
+      <c r="O73" s="163"/>
+      <c r="P73" s="163"/>
+      <c r="Q73" s="163"/>
+      <c r="R73" s="163"/>
+      <c r="S73" s="163"/>
+      <c r="T73" s="163"/>
     </row>
     <row r="74" spans="1:20" ht="15" customHeight="1">
       <c r="A74" s="18"/>
@@ -8161,15 +8161,15 @@
       <c r="I81" s="39"/>
       <c r="J81" s="39"/>
       <c r="K81" s="61"/>
-      <c r="N81" s="170" t="s">
+      <c r="N81" s="163" t="s">
         <v>87</v>
       </c>
-      <c r="O81" s="170"/>
-      <c r="P81" s="170"/>
-      <c r="Q81" s="170"/>
-      <c r="R81" s="170"/>
-      <c r="S81" s="170"/>
-      <c r="T81" s="170"/>
+      <c r="O81" s="163"/>
+      <c r="P81" s="163"/>
+      <c r="Q81" s="163"/>
+      <c r="R81" s="163"/>
+      <c r="S81" s="163"/>
+      <c r="T81" s="163"/>
     </row>
     <row r="82" spans="1:20" ht="15" customHeight="1">
       <c r="A82" s="18"/>
@@ -9286,15 +9286,15 @@
       <c r="J129" s="39"/>
       <c r="K129" s="21"/>
       <c r="M129" s="1"/>
-      <c r="N129" s="184" t="s">
+      <c r="N129" s="185" t="s">
         <v>146</v>
       </c>
-      <c r="O129" s="184"/>
-      <c r="P129" s="184"/>
-      <c r="Q129" s="184"/>
-      <c r="R129" s="184"/>
-      <c r="S129" s="184"/>
-      <c r="T129" s="184"/>
+      <c r="O129" s="185"/>
+      <c r="P129" s="185"/>
+      <c r="Q129" s="185"/>
+      <c r="R129" s="185"/>
+      <c r="S129" s="185"/>
+      <c r="T129" s="185"/>
     </row>
     <row r="130" spans="1:20" ht="15" customHeight="1">
       <c r="A130" s="18"/>
@@ -9319,15 +9319,15 @@
       <c r="J130" s="39"/>
       <c r="K130" s="21"/>
       <c r="M130" s="1"/>
-      <c r="N130" s="184" t="s">
+      <c r="N130" s="185" t="s">
         <v>147</v>
       </c>
-      <c r="O130" s="184"/>
-      <c r="P130" s="184"/>
-      <c r="Q130" s="184"/>
-      <c r="R130" s="184"/>
-      <c r="S130" s="184"/>
-      <c r="T130" s="184"/>
+      <c r="O130" s="185"/>
+      <c r="P130" s="185"/>
+      <c r="Q130" s="185"/>
+      <c r="R130" s="185"/>
+      <c r="S130" s="185"/>
+      <c r="T130" s="185"/>
     </row>
     <row r="131" spans="1:20" ht="15" customHeight="1">
       <c r="A131" s="39"/>
@@ -9606,11 +9606,11 @@
       <c r="B145" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C145" s="168">
+      <c r="C145" s="164">
         <f>J143</f>
         <v>487209.35310074891</v>
       </c>
-      <c r="D145" s="168"/>
+      <c r="D145" s="164"/>
       <c r="E145" s="38">
         <v>100</v>
       </c>
@@ -9626,10 +9626,10 @@
       <c r="B146" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C146" s="169">
+      <c r="C146" s="167">
         <v>500000</v>
       </c>
-      <c r="D146" s="169"/>
+      <c r="D146" s="167"/>
       <c r="E146" s="38"/>
       <c r="F146" s="45"/>
       <c r="G146" s="44"/>
@@ -9643,11 +9643,11 @@
       <c r="B147" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C147" s="169">
+      <c r="C147" s="167">
         <f>C146-C149-C150</f>
         <v>475000</v>
       </c>
-      <c r="D147" s="169"/>
+      <c r="D147" s="167"/>
       <c r="E147" s="38">
         <f>C147/C145*100</f>
         <v>97.494023252418117</v>
@@ -9664,11 +9664,11 @@
       <c r="B148" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C148" s="168">
+      <c r="C148" s="164">
         <f>C145-C147</f>
         <v>12209.353100748907</v>
       </c>
-      <c r="D148" s="168"/>
+      <c r="D148" s="164"/>
       <c r="E148" s="38">
         <f>100-E147</f>
         <v>2.505976747581883</v>
@@ -9685,11 +9685,11 @@
       <c r="B149" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C149" s="168">
+      <c r="C149" s="164">
         <f>C146*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D149" s="168"/>
+      <c r="D149" s="164"/>
       <c r="E149" s="38">
         <v>3</v>
       </c>
@@ -9705,11 +9705,11 @@
       <c r="B150" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C150" s="168">
+      <c r="C150" s="164">
         <f>C146*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D150" s="168"/>
+      <c r="D150" s="164"/>
       <c r="E150" s="38">
         <v>2</v>
       </c>
@@ -9791,18 +9791,6 @@
     <row r="207" s="34" customFormat="1"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C146:D146"/>
-    <mergeCell ref="C147:D147"/>
-    <mergeCell ref="C148:D148"/>
-    <mergeCell ref="C149:D149"/>
-    <mergeCell ref="C150:D150"/>
-    <mergeCell ref="N129:T129"/>
-    <mergeCell ref="N130:T130"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="N60:T60"/>
-    <mergeCell ref="N73:T73"/>
-    <mergeCell ref="N81:T81"/>
     <mergeCell ref="C145:D145"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
@@ -9811,6 +9799,18 @@
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
+    <mergeCell ref="N129:T129"/>
+    <mergeCell ref="N130:T130"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="N60:T60"/>
+    <mergeCell ref="N73:T73"/>
+    <mergeCell ref="N81:T81"/>
+    <mergeCell ref="C146:D146"/>
+    <mergeCell ref="C147:D147"/>
+    <mergeCell ref="C148:D148"/>
+    <mergeCell ref="C149:D149"/>
+    <mergeCell ref="C150:D150"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B100" r:id="rId1"/>
@@ -9846,113 +9846,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
-      <c r="A1" s="163" t="s">
+      <c r="A1" s="169" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
+      <c r="B1" s="169"/>
+      <c r="C1" s="169"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
+      <c r="G1" s="169"/>
+      <c r="H1" s="169"/>
+      <c r="I1" s="169"/>
+      <c r="J1" s="169"/>
+      <c r="K1" s="169"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="22.5">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="170" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="164"/>
-      <c r="C2" s="164"/>
-      <c r="D2" s="164"/>
-      <c r="E2" s="164"/>
-      <c r="F2" s="164"/>
-      <c r="G2" s="164"/>
-      <c r="H2" s="164"/>
-      <c r="I2" s="164"/>
-      <c r="J2" s="164"/>
-      <c r="K2" s="164"/>
+      <c r="B2" s="170"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="170"/>
+      <c r="I2" s="170"/>
+      <c r="J2" s="170"/>
+      <c r="K2" s="170"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1">
-      <c r="A3" s="152" t="s">
+      <c r="A3" s="161" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="152"/>
-      <c r="C3" s="152"/>
-      <c r="D3" s="152"/>
-      <c r="E3" s="152"/>
-      <c r="F3" s="152"/>
-      <c r="G3" s="152"/>
-      <c r="H3" s="152"/>
-      <c r="I3" s="152"/>
-      <c r="J3" s="152"/>
-      <c r="K3" s="152"/>
+      <c r="B3" s="161"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="161"/>
+      <c r="F3" s="161"/>
+      <c r="G3" s="161"/>
+      <c r="H3" s="161"/>
+      <c r="I3" s="161"/>
+      <c r="J3" s="161"/>
+      <c r="K3" s="161"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1">
-      <c r="A4" s="152" t="s">
+      <c r="A4" s="161" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="152"/>
-      <c r="C4" s="152"/>
-      <c r="D4" s="152"/>
-      <c r="E4" s="152"/>
-      <c r="F4" s="152"/>
-      <c r="G4" s="152"/>
-      <c r="H4" s="152"/>
-      <c r="I4" s="152"/>
-      <c r="J4" s="152"/>
-      <c r="K4" s="152"/>
+      <c r="B4" s="161"/>
+      <c r="C4" s="161"/>
+      <c r="D4" s="161"/>
+      <c r="E4" s="161"/>
+      <c r="F4" s="161"/>
+      <c r="G4" s="161"/>
+      <c r="H4" s="161"/>
+      <c r="I4" s="161"/>
+      <c r="J4" s="161"/>
+      <c r="K4" s="161"/>
     </row>
     <row r="5" spans="1:14" ht="18.75">
-      <c r="A5" s="165" t="s">
+      <c r="A5" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="165"/>
-      <c r="C5" s="165"/>
-      <c r="D5" s="165"/>
-      <c r="E5" s="165"/>
-      <c r="F5" s="165"/>
-      <c r="G5" s="165"/>
-      <c r="H5" s="165"/>
-      <c r="I5" s="165"/>
-      <c r="J5" s="165"/>
-      <c r="K5" s="165"/>
+      <c r="B5" s="171"/>
+      <c r="C5" s="171"/>
+      <c r="D5" s="171"/>
+      <c r="E5" s="171"/>
+      <c r="F5" s="171"/>
+      <c r="G5" s="171"/>
+      <c r="H5" s="171"/>
+      <c r="I5" s="171"/>
+      <c r="J5" s="171"/>
+      <c r="K5" s="171"/>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="156" t="s">
+      <c r="A6" s="151" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="156"/>
-      <c r="C6" s="156"/>
-      <c r="D6" s="156"/>
-      <c r="E6" s="156"/>
-      <c r="F6" s="156"/>
+      <c r="B6" s="151"/>
+      <c r="C6" s="151"/>
+      <c r="D6" s="151"/>
+      <c r="E6" s="151"/>
+      <c r="F6" s="151"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="162" t="s">
+      <c r="H6" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="162"/>
-      <c r="J6" s="162"/>
-      <c r="K6" s="162"/>
+      <c r="I6" s="168"/>
+      <c r="J6" s="168"/>
+      <c r="K6" s="168"/>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="166" t="s">
+      <c r="A7" s="165" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="166"/>
-      <c r="C7" s="166"/>
-      <c r="D7" s="166"/>
-      <c r="E7" s="166"/>
-      <c r="F7" s="166"/>
+      <c r="B7" s="165"/>
+      <c r="C7" s="165"/>
+      <c r="D7" s="165"/>
+      <c r="E7" s="165"/>
+      <c r="F7" s="165"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="167" t="s">
+      <c r="H7" s="166" t="s">
         <v>141</v>
       </c>
-      <c r="I7" s="167"/>
-      <c r="J7" s="167"/>
-      <c r="K7" s="167"/>
+      <c r="I7" s="166"/>
+      <c r="J7" s="166"/>
+      <c r="K7" s="166"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1">
       <c r="A8" s="4" t="s">
@@ -11154,15 +11154,15 @@
       <c r="I61" s="39"/>
       <c r="J61" s="39"/>
       <c r="K61" s="61"/>
-      <c r="N61" s="170" t="s">
+      <c r="N61" s="163" t="s">
         <v>87</v>
       </c>
-      <c r="O61" s="170"/>
-      <c r="P61" s="170"/>
-      <c r="Q61" s="170"/>
-      <c r="R61" s="170"/>
-      <c r="S61" s="170"/>
-      <c r="T61" s="170"/>
+      <c r="O61" s="163"/>
+      <c r="P61" s="163"/>
+      <c r="Q61" s="163"/>
+      <c r="R61" s="163"/>
+      <c r="S61" s="163"/>
+      <c r="T61" s="163"/>
     </row>
     <row r="62" spans="1:20" ht="15" customHeight="1">
       <c r="A62" s="18"/>
@@ -11459,15 +11459,15 @@
       <c r="I74" s="39"/>
       <c r="J74" s="39"/>
       <c r="K74" s="61"/>
-      <c r="N74" s="170" t="s">
+      <c r="N74" s="163" t="s">
         <v>87</v>
       </c>
-      <c r="O74" s="170"/>
-      <c r="P74" s="170"/>
-      <c r="Q74" s="170"/>
-      <c r="R74" s="170"/>
-      <c r="S74" s="170"/>
-      <c r="T74" s="170"/>
+      <c r="O74" s="163"/>
+      <c r="P74" s="163"/>
+      <c r="Q74" s="163"/>
+      <c r="R74" s="163"/>
+      <c r="S74" s="163"/>
+      <c r="T74" s="163"/>
     </row>
     <row r="75" spans="1:20" ht="15" customHeight="1">
       <c r="A75" s="18"/>
@@ -11663,15 +11663,15 @@
       <c r="I82" s="39"/>
       <c r="J82" s="39"/>
       <c r="K82" s="61"/>
-      <c r="N82" s="170" t="s">
+      <c r="N82" s="163" t="s">
         <v>87</v>
       </c>
-      <c r="O82" s="170"/>
-      <c r="P82" s="170"/>
-      <c r="Q82" s="170"/>
-      <c r="R82" s="170"/>
-      <c r="S82" s="170"/>
-      <c r="T82" s="170"/>
+      <c r="O82" s="163"/>
+      <c r="P82" s="163"/>
+      <c r="Q82" s="163"/>
+      <c r="R82" s="163"/>
+      <c r="S82" s="163"/>
+      <c r="T82" s="163"/>
     </row>
     <row r="83" spans="1:20" ht="15" customHeight="1">
       <c r="A83" s="18"/>
@@ -12788,15 +12788,15 @@
       <c r="J130" s="39"/>
       <c r="K130" s="21"/>
       <c r="M130" s="1"/>
-      <c r="N130" s="184" t="s">
+      <c r="N130" s="185" t="s">
         <v>146</v>
       </c>
-      <c r="O130" s="184"/>
-      <c r="P130" s="184"/>
-      <c r="Q130" s="184"/>
-      <c r="R130" s="184"/>
-      <c r="S130" s="184"/>
-      <c r="T130" s="184"/>
+      <c r="O130" s="185"/>
+      <c r="P130" s="185"/>
+      <c r="Q130" s="185"/>
+      <c r="R130" s="185"/>
+      <c r="S130" s="185"/>
+      <c r="T130" s="185"/>
     </row>
     <row r="131" spans="1:20" ht="15" customHeight="1">
       <c r="A131" s="18"/>
@@ -12821,15 +12821,15 @@
       <c r="J131" s="39"/>
       <c r="K131" s="21"/>
       <c r="M131" s="1"/>
-      <c r="N131" s="184" t="s">
+      <c r="N131" s="185" t="s">
         <v>147</v>
       </c>
-      <c r="O131" s="184"/>
-      <c r="P131" s="184"/>
-      <c r="Q131" s="184"/>
-      <c r="R131" s="184"/>
-      <c r="S131" s="184"/>
-      <c r="T131" s="184"/>
+      <c r="O131" s="185"/>
+      <c r="P131" s="185"/>
+      <c r="Q131" s="185"/>
+      <c r="R131" s="185"/>
+      <c r="S131" s="185"/>
+      <c r="T131" s="185"/>
     </row>
     <row r="132" spans="1:20" ht="15" customHeight="1">
       <c r="A132" s="39"/>
@@ -13108,11 +13108,11 @@
       <c r="B146" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C146" s="168">
+      <c r="C146" s="164">
         <f>J144</f>
         <v>559342.93667359848</v>
       </c>
-      <c r="D146" s="168"/>
+      <c r="D146" s="164"/>
       <c r="E146" s="38">
         <v>100</v>
       </c>
@@ -13128,10 +13128,10 @@
       <c r="B147" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C147" s="169">
+      <c r="C147" s="167">
         <v>500000</v>
       </c>
-      <c r="D147" s="169"/>
+      <c r="D147" s="167"/>
       <c r="E147" s="38"/>
       <c r="F147" s="45"/>
       <c r="G147" s="44"/>
@@ -13145,11 +13145,11 @@
       <c r="B148" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C148" s="169">
+      <c r="C148" s="167">
         <f>C147-C150-C151</f>
         <v>475000</v>
       </c>
-      <c r="D148" s="169"/>
+      <c r="D148" s="167"/>
       <c r="E148" s="38">
         <f>C148/C146*100</f>
         <v>84.921068785603282</v>
@@ -13166,11 +13166,11 @@
       <c r="B149" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C149" s="168">
+      <c r="C149" s="164">
         <f>C146-C148</f>
         <v>84342.93667359848</v>
       </c>
-      <c r="D149" s="168"/>
+      <c r="D149" s="164"/>
       <c r="E149" s="38">
         <f>100-E148</f>
         <v>15.078931214396718</v>
@@ -13187,11 +13187,11 @@
       <c r="B150" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C150" s="168">
+      <c r="C150" s="164">
         <f>C147*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D150" s="168"/>
+      <c r="D150" s="164"/>
       <c r="E150" s="38">
         <v>3</v>
       </c>
@@ -13207,11 +13207,11 @@
       <c r="B151" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C151" s="168">
+      <c r="C151" s="164">
         <f>C147*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D151" s="168"/>
+      <c r="D151" s="164"/>
       <c r="E151" s="38">
         <v>2</v>
       </c>
@@ -13293,6 +13293,13 @@
     <row r="208" s="34" customFormat="1"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C151:D151"/>
+    <mergeCell ref="N131:T131"/>
+    <mergeCell ref="C146:D146"/>
+    <mergeCell ref="C147:D147"/>
+    <mergeCell ref="C148:D148"/>
+    <mergeCell ref="C149:D149"/>
+    <mergeCell ref="C150:D150"/>
     <mergeCell ref="N130:T130"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
@@ -13306,13 +13313,6 @@
     <mergeCell ref="N61:T61"/>
     <mergeCell ref="N74:T74"/>
     <mergeCell ref="N82:T82"/>
-    <mergeCell ref="C151:D151"/>
-    <mergeCell ref="N131:T131"/>
-    <mergeCell ref="C146:D146"/>
-    <mergeCell ref="C147:D147"/>
-    <mergeCell ref="C148:D148"/>
-    <mergeCell ref="C149:D149"/>
-    <mergeCell ref="C150:D150"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B101" r:id="rId1"/>
@@ -13329,8 +13329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T211"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A145" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13347,113 +13347,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
-      <c r="A1" s="163" t="s">
+      <c r="A1" s="169" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
+      <c r="B1" s="169"/>
+      <c r="C1" s="169"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
+      <c r="G1" s="169"/>
+      <c r="H1" s="169"/>
+      <c r="I1" s="169"/>
+      <c r="J1" s="169"/>
+      <c r="K1" s="169"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="22.5">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="170" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="164"/>
-      <c r="C2" s="164"/>
-      <c r="D2" s="164"/>
-      <c r="E2" s="164"/>
-      <c r="F2" s="164"/>
-      <c r="G2" s="164"/>
-      <c r="H2" s="164"/>
-      <c r="I2" s="164"/>
-      <c r="J2" s="164"/>
-      <c r="K2" s="164"/>
+      <c r="B2" s="170"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="170"/>
+      <c r="I2" s="170"/>
+      <c r="J2" s="170"/>
+      <c r="K2" s="170"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1">
-      <c r="A3" s="152" t="s">
+      <c r="A3" s="161" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="152"/>
-      <c r="C3" s="152"/>
-      <c r="D3" s="152"/>
-      <c r="E3" s="152"/>
-      <c r="F3" s="152"/>
-      <c r="G3" s="152"/>
-      <c r="H3" s="152"/>
-      <c r="I3" s="152"/>
-      <c r="J3" s="152"/>
-      <c r="K3" s="152"/>
+      <c r="B3" s="161"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="161"/>
+      <c r="F3" s="161"/>
+      <c r="G3" s="161"/>
+      <c r="H3" s="161"/>
+      <c r="I3" s="161"/>
+      <c r="J3" s="161"/>
+      <c r="K3" s="161"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1">
-      <c r="A4" s="152" t="s">
+      <c r="A4" s="161" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="152"/>
-      <c r="C4" s="152"/>
-      <c r="D4" s="152"/>
-      <c r="E4" s="152"/>
-      <c r="F4" s="152"/>
-      <c r="G4" s="152"/>
-      <c r="H4" s="152"/>
-      <c r="I4" s="152"/>
-      <c r="J4" s="152"/>
-      <c r="K4" s="152"/>
+      <c r="B4" s="161"/>
+      <c r="C4" s="161"/>
+      <c r="D4" s="161"/>
+      <c r="E4" s="161"/>
+      <c r="F4" s="161"/>
+      <c r="G4" s="161"/>
+      <c r="H4" s="161"/>
+      <c r="I4" s="161"/>
+      <c r="J4" s="161"/>
+      <c r="K4" s="161"/>
     </row>
     <row r="5" spans="1:14" ht="18.75">
-      <c r="A5" s="165" t="s">
+      <c r="A5" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="165"/>
-      <c r="C5" s="165"/>
-      <c r="D5" s="165"/>
-      <c r="E5" s="165"/>
-      <c r="F5" s="165"/>
-      <c r="G5" s="165"/>
-      <c r="H5" s="165"/>
-      <c r="I5" s="165"/>
-      <c r="J5" s="165"/>
-      <c r="K5" s="165"/>
+      <c r="B5" s="171"/>
+      <c r="C5" s="171"/>
+      <c r="D5" s="171"/>
+      <c r="E5" s="171"/>
+      <c r="F5" s="171"/>
+      <c r="G5" s="171"/>
+      <c r="H5" s="171"/>
+      <c r="I5" s="171"/>
+      <c r="J5" s="171"/>
+      <c r="K5" s="171"/>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="156" t="s">
+      <c r="A6" s="151" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="156"/>
-      <c r="C6" s="156"/>
-      <c r="D6" s="156"/>
-      <c r="E6" s="156"/>
-      <c r="F6" s="156"/>
+      <c r="B6" s="151"/>
+      <c r="C6" s="151"/>
+      <c r="D6" s="151"/>
+      <c r="E6" s="151"/>
+      <c r="F6" s="151"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="162" t="s">
+      <c r="H6" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="162"/>
-      <c r="J6" s="162"/>
-      <c r="K6" s="162"/>
+      <c r="I6" s="168"/>
+      <c r="J6" s="168"/>
+      <c r="K6" s="168"/>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="166" t="s">
+      <c r="A7" s="165" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="166"/>
-      <c r="C7" s="166"/>
-      <c r="D7" s="166"/>
-      <c r="E7" s="166"/>
-      <c r="F7" s="166"/>
+      <c r="B7" s="165"/>
+      <c r="C7" s="165"/>
+      <c r="D7" s="165"/>
+      <c r="E7" s="165"/>
+      <c r="F7" s="165"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="167" t="s">
+      <c r="H7" s="166" t="s">
         <v>162</v>
       </c>
-      <c r="I7" s="167"/>
-      <c r="J7" s="167"/>
-      <c r="K7" s="167"/>
+      <c r="I7" s="166"/>
+      <c r="J7" s="166"/>
+      <c r="K7" s="166"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1">
       <c r="A8" s="4" t="s">
@@ -14630,15 +14630,15 @@
       <c r="I60" s="39"/>
       <c r="J60" s="39"/>
       <c r="K60" s="61"/>
-      <c r="N60" s="170" t="s">
+      <c r="N60" s="163" t="s">
         <v>87</v>
       </c>
-      <c r="O60" s="170"/>
-      <c r="P60" s="170"/>
-      <c r="Q60" s="170"/>
-      <c r="R60" s="170"/>
-      <c r="S60" s="170"/>
-      <c r="T60" s="170"/>
+      <c r="O60" s="163"/>
+      <c r="P60" s="163"/>
+      <c r="Q60" s="163"/>
+      <c r="R60" s="163"/>
+      <c r="S60" s="163"/>
+      <c r="T60" s="163"/>
     </row>
     <row r="61" spans="1:20" ht="15" customHeight="1">
       <c r="A61" s="18"/>
@@ -14935,15 +14935,15 @@
       <c r="I73" s="39"/>
       <c r="J73" s="39"/>
       <c r="K73" s="61"/>
-      <c r="N73" s="170" t="s">
+      <c r="N73" s="163" t="s">
         <v>87</v>
       </c>
-      <c r="O73" s="170"/>
-      <c r="P73" s="170"/>
-      <c r="Q73" s="170"/>
-      <c r="R73" s="170"/>
-      <c r="S73" s="170"/>
-      <c r="T73" s="170"/>
+      <c r="O73" s="163"/>
+      <c r="P73" s="163"/>
+      <c r="Q73" s="163"/>
+      <c r="R73" s="163"/>
+      <c r="S73" s="163"/>
+      <c r="T73" s="163"/>
     </row>
     <row r="74" spans="1:20" ht="15" customHeight="1">
       <c r="A74" s="18"/>
@@ -15139,15 +15139,15 @@
       <c r="I81" s="39"/>
       <c r="J81" s="39"/>
       <c r="K81" s="61"/>
-      <c r="N81" s="170" t="s">
+      <c r="N81" s="163" t="s">
         <v>87</v>
       </c>
-      <c r="O81" s="170"/>
-      <c r="P81" s="170"/>
-      <c r="Q81" s="170"/>
-      <c r="R81" s="170"/>
-      <c r="S81" s="170"/>
-      <c r="T81" s="170"/>
+      <c r="O81" s="163"/>
+      <c r="P81" s="163"/>
+      <c r="Q81" s="163"/>
+      <c r="R81" s="163"/>
+      <c r="S81" s="163"/>
+      <c r="T81" s="163"/>
     </row>
     <row r="82" spans="1:20" ht="15" customHeight="1">
       <c r="A82" s="18"/>
@@ -16375,15 +16375,15 @@
       <c r="J133" s="39"/>
       <c r="K133" s="21"/>
       <c r="M133" s="1"/>
-      <c r="N133" s="184" t="s">
+      <c r="N133" s="185" t="s">
         <v>146</v>
       </c>
-      <c r="O133" s="184"/>
-      <c r="P133" s="184"/>
-      <c r="Q133" s="184"/>
-      <c r="R133" s="184"/>
-      <c r="S133" s="184"/>
-      <c r="T133" s="184"/>
+      <c r="O133" s="185"/>
+      <c r="P133" s="185"/>
+      <c r="Q133" s="185"/>
+      <c r="R133" s="185"/>
+      <c r="S133" s="185"/>
+      <c r="T133" s="185"/>
     </row>
     <row r="134" spans="1:20" ht="15" customHeight="1">
       <c r="A134" s="18"/>
@@ -16408,15 +16408,15 @@
       <c r="J134" s="39"/>
       <c r="K134" s="21"/>
       <c r="M134" s="1"/>
-      <c r="N134" s="184" t="s">
+      <c r="N134" s="185" t="s">
         <v>147</v>
       </c>
-      <c r="O134" s="184"/>
-      <c r="P134" s="184"/>
-      <c r="Q134" s="184"/>
-      <c r="R134" s="184"/>
-      <c r="S134" s="184"/>
-      <c r="T134" s="184"/>
+      <c r="O134" s="185"/>
+      <c r="P134" s="185"/>
+      <c r="Q134" s="185"/>
+      <c r="R134" s="185"/>
+      <c r="S134" s="185"/>
+      <c r="T134" s="185"/>
     </row>
     <row r="135" spans="1:20" ht="15" customHeight="1">
       <c r="A135" s="39"/>
@@ -16579,7 +16579,7 @@
       <c r="A143" s="18">
         <v>20</v>
       </c>
-      <c r="B143" s="185" t="s">
+      <c r="B143" s="148" t="s">
         <v>139</v>
       </c>
       <c r="C143" s="19">
@@ -16695,11 +16695,11 @@
       <c r="B149" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C149" s="168">
+      <c r="C149" s="164">
         <f>J147</f>
         <v>564973.01951057301</v>
       </c>
-      <c r="D149" s="168"/>
+      <c r="D149" s="164"/>
       <c r="E149" s="38">
         <v>100</v>
       </c>
@@ -16715,10 +16715,10 @@
       <c r="B150" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C150" s="169">
+      <c r="C150" s="167">
         <v>500000</v>
       </c>
-      <c r="D150" s="169"/>
+      <c r="D150" s="167"/>
       <c r="E150" s="38"/>
       <c r="F150" s="45"/>
       <c r="G150" s="44"/>
@@ -16732,11 +16732,11 @@
       <c r="B151" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C151" s="169">
+      <c r="C151" s="167">
         <f>C150-C153-C154</f>
         <v>475000</v>
       </c>
-      <c r="D151" s="169"/>
+      <c r="D151" s="167"/>
       <c r="E151" s="38">
         <f>C151/C149*100</f>
         <v>84.074811291251535</v>
@@ -16753,11 +16753,11 @@
       <c r="B152" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C152" s="168">
+      <c r="C152" s="164">
         <f>C149-C151</f>
         <v>89973.019510573009</v>
       </c>
-      <c r="D152" s="168"/>
+      <c r="D152" s="164"/>
       <c r="E152" s="38">
         <f>100-E151</f>
         <v>15.925188708748465</v>
@@ -16774,11 +16774,11 @@
       <c r="B153" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C153" s="168">
+      <c r="C153" s="164">
         <f>C150*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D153" s="168"/>
+      <c r="D153" s="164"/>
       <c r="E153" s="38">
         <v>3</v>
       </c>
@@ -16794,11 +16794,11 @@
       <c r="B154" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C154" s="168">
+      <c r="C154" s="164">
         <f>C150*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D154" s="168"/>
+      <c r="D154" s="164"/>
       <c r="E154" s="38">
         <v>2</v>
       </c>
@@ -16880,13 +16880,6 @@
     <row r="211" s="34" customFormat="1"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C154:D154"/>
-    <mergeCell ref="N134:T134"/>
-    <mergeCell ref="C149:D149"/>
-    <mergeCell ref="C150:D150"/>
-    <mergeCell ref="C151:D151"/>
-    <mergeCell ref="C152:D152"/>
-    <mergeCell ref="C153:D153"/>
     <mergeCell ref="N133:T133"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
@@ -16900,6 +16893,13 @@
     <mergeCell ref="N60:T60"/>
     <mergeCell ref="N73:T73"/>
     <mergeCell ref="N81:T81"/>
+    <mergeCell ref="C154:D154"/>
+    <mergeCell ref="N134:T134"/>
+    <mergeCell ref="C149:D149"/>
+    <mergeCell ref="C150:D150"/>
+    <mergeCell ref="C151:D151"/>
+    <mergeCell ref="C152:D152"/>
+    <mergeCell ref="C153:D153"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B103" r:id="rId1"/>

</xml_diff>